<commit_message>
Atualizado por script em
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V130"/>
+  <dimension ref="A1:V134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2137,71 +2137,71 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G19" t="n">
+        <v>2</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
         <v>1</v>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Lanus</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
       <c r="J19" t="n">
-        <v>2.19</v>
+        <v>1.74</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>2.09</v>
+        <v>1.94</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:43</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="N19" t="n">
-        <v>2.94</v>
+        <v>3.44</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="P19" t="n">
-        <v>3.01</v>
+        <v>3.23</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:43</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="R19" t="n">
-        <v>3.79</v>
+        <v>5.57</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="T19" t="n">
-        <v>4.48</v>
+        <v>4.73</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:42</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-lanus/OdYgrAqL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-huracan/l4ycuMBq/</t>
         </is>
       </c>
     </row>
@@ -2229,71 +2229,71 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>1.74</v>
+        <v>2.19</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>1.94</v>
+        <v>2.09</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:43</t>
         </is>
       </c>
       <c r="N20" t="n">
-        <v>3.44</v>
+        <v>2.94</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="P20" t="n">
-        <v>3.23</v>
+        <v>3.01</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:43</t>
         </is>
       </c>
       <c r="R20" t="n">
-        <v>5.57</v>
+        <v>3.79</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="T20" t="n">
-        <v>4.73</v>
+        <v>4.48</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:42</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-huracan/l4ycuMBq/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-lanus/OdYgrAqL/</t>
         </is>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -3801,63 +3801,63 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>1.76</v>
+        <v>2.67</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>29/08/2023 00:12</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>1.75</v>
+        <v>3.38</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
+          <t>03/09/2023 21:07</t>
+        </is>
+      </c>
+      <c r="N37" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P37" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="N37" t="n">
-        <v>3.56</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="P37" t="n">
-        <v>3.46</v>
-      </c>
-      <c r="Q37" t="inlineStr">
+      <c r="R37" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T37" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="U37" t="inlineStr">
         <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="R37" t="n">
-        <v>5.34</v>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="T37" t="n">
-        <v>5.63</v>
-      </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>03/09/2023 21:13</t>
-        </is>
-      </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
         </is>
       </c>
     </row>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -3893,38 +3893,38 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J38" t="n">
-        <v>2.67</v>
+        <v>1.76</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="L38" t="n">
-        <v>3.38</v>
+        <v>1.75</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>03/09/2023 21:07</t>
+          <t>03/09/2023 21:13</t>
         </is>
       </c>
       <c r="N38" t="n">
-        <v>3.13</v>
+        <v>3.56</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="P38" t="n">
-        <v>3.18</v>
+        <v>3.46</v>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
@@ -3932,15 +3932,15 @@
         </is>
       </c>
       <c r="R38" t="n">
-        <v>2.73</v>
+        <v>5.34</v>
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="T38" t="n">
-        <v>2.36</v>
+        <v>5.63</v>
       </c>
       <c r="U38" t="inlineStr">
         <is>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
         </is>
       </c>
     </row>
@@ -6093,71 +6093,71 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I62" t="n">
         <v>0</v>
       </c>
       <c r="J62" t="n">
-        <v>2.49</v>
+        <v>2.72</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="L62" t="n">
-        <v>2.67</v>
+        <v>3.41</v>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:58</t>
+          <t>20/09/2023 20:59</t>
         </is>
       </c>
       <c r="N62" t="n">
-        <v>3.2</v>
+        <v>2.92</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="P62" t="n">
-        <v>3.03</v>
+        <v>2.8</v>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:53</t>
+          <t>20/09/2023 20:52</t>
         </is>
       </c>
       <c r="R62" t="n">
-        <v>3.05</v>
+        <v>3</v>
       </c>
       <c r="S62" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="T62" t="n">
-        <v>3.04</v>
+        <v>2.61</v>
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:53</t>
+          <t>20/09/2023 20:59</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-tigre/0bg4FEAA/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-banfield/UDN4fDYp/</t>
         </is>
       </c>
     </row>
@@ -6185,71 +6185,71 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I63" t="n">
         <v>0</v>
       </c>
       <c r="J63" t="n">
-        <v>2.72</v>
+        <v>2.49</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="L63" t="n">
-        <v>3.41</v>
+        <v>2.67</v>
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:59</t>
+          <t>20/09/2023 20:58</t>
         </is>
       </c>
       <c r="N63" t="n">
-        <v>2.92</v>
+        <v>3.2</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="P63" t="n">
-        <v>2.8</v>
+        <v>3.03</v>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:52</t>
+          <t>20/09/2023 20:53</t>
         </is>
       </c>
       <c r="R63" t="n">
-        <v>3</v>
+        <v>3.05</v>
       </c>
       <c r="S63" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="T63" t="n">
-        <v>2.61</v>
+        <v>3.04</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:59</t>
+          <t>20/09/2023 20:53</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-banfield/UDN4fDYp/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-tigre/0bg4FEAA/</t>
         </is>
       </c>
     </row>
@@ -6277,71 +6277,71 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Velez Sarsfield</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>San Lorenzo</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>1.69</v>
+        <v>2.04</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="L64" t="n">
-        <v>1.74</v>
+        <v>2.29</v>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:23</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="N64" t="n">
-        <v>3.41</v>
+        <v>3.04</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="P64" t="n">
-        <v>3.4</v>
+        <v>2.85</v>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:23</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="R64" t="n">
-        <v>5.46</v>
+        <v>4.47</v>
       </c>
       <c r="S64" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="T64" t="n">
-        <v>6</v>
+        <v>4.05</v>
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:27</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-arsenal-sarandi/OEeXCLlC/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-san-lorenzo/IZPUVZfi/</t>
         </is>
       </c>
     </row>
@@ -6369,71 +6369,71 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Velez Sarsfield</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>San Lorenzo</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J65" t="n">
-        <v>2.04</v>
+        <v>1.69</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="L65" t="n">
-        <v>2.29</v>
+        <v>1.74</v>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:23</t>
         </is>
       </c>
       <c r="N65" t="n">
-        <v>3.04</v>
+        <v>3.41</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="P65" t="n">
-        <v>2.85</v>
+        <v>3.4</v>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:23</t>
         </is>
       </c>
       <c r="R65" t="n">
-        <v>4.47</v>
+        <v>5.46</v>
       </c>
       <c r="S65" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="T65" t="n">
-        <v>4.05</v>
+        <v>6</v>
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:27</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-san-lorenzo/IZPUVZfi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-arsenal-sarandi/OEeXCLlC/</t>
         </is>
       </c>
     </row>
@@ -6461,71 +6461,71 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Racing Club</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I66" t="n">
         <v>1</v>
       </c>
       <c r="J66" t="n">
-        <v>2.62</v>
+        <v>2.04</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="L66" t="n">
-        <v>2.35</v>
+        <v>2.18</v>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="N66" t="n">
-        <v>2.94</v>
+        <v>3.19</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="P66" t="n">
-        <v>3.13</v>
+        <v>3</v>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="R66" t="n">
-        <v>3.12</v>
+        <v>4.18</v>
       </c>
       <c r="S66" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="T66" t="n">
-        <v>3.47</v>
+        <v>4.13</v>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-newells-old-boys/4Wym7jIj/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-colon-santa-fe/A90iIGQi/</t>
         </is>
       </c>
     </row>
@@ -6553,71 +6553,71 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Racing Club</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="I67" t="n">
         <v>1</v>
       </c>
       <c r="J67" t="n">
-        <v>2.04</v>
+        <v>2.62</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="L67" t="n">
-        <v>2.18</v>
+        <v>2.35</v>
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="N67" t="n">
-        <v>3.19</v>
+        <v>2.94</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="P67" t="n">
-        <v>3</v>
+        <v>3.13</v>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="R67" t="n">
-        <v>4.18</v>
+        <v>3.12</v>
       </c>
       <c r="S67" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="T67" t="n">
-        <v>4.13</v>
+        <v>3.47</v>
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-colon-santa-fe/A90iIGQi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-newells-old-boys/4Wym7jIj/</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -9229,22 +9229,22 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>2.3</v>
+        <v>2.25</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.14</v>
+        <v>2.49</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
@@ -9252,15 +9252,15 @@
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.05</v>
+        <v>3.04</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.03</v>
+        <v>2.86</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
@@ -9268,16 +9268,16 @@
         </is>
       </c>
       <c r="R96" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>25/09/2023 22:42</t>
+        </is>
+      </c>
+      <c r="T96" t="n">
         <v>3.54</v>
       </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>26/09/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T96" t="n">
-        <v>4.22</v>
-      </c>
       <c r="U96" t="inlineStr">
         <is>
           <t>02/10/2023 23:29</t>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
         </is>
       </c>
     </row>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -9321,22 +9321,22 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>2.25</v>
+        <v>2.3</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>2.49</v>
+        <v>2.14</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
@@ -9344,15 +9344,15 @@
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.04</v>
+        <v>3.05</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>2.86</v>
+        <v>3.03</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
@@ -9360,15 +9360,15 @@
         </is>
       </c>
       <c r="R97" t="n">
-        <v>3.7</v>
+        <v>3.54</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="T97" t="n">
-        <v>3.54</v>
+        <v>4.22</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
         </is>
       </c>
     </row>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -9413,14 +9413,14 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>3.31</v>
+        <v>1.93</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
         </is>
       </c>
       <c r="L98" t="n">
-        <v>3.28</v>
+        <v>1.91</v>
       </c>
       <c r="M98" t="inlineStr">
         <is>
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="N98" t="n">
-        <v>2.97</v>
+        <v>3.29</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -9444,7 +9444,7 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>2.93</v>
+        <v>3.2</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
@@ -9452,7 +9452,7 @@
         </is>
       </c>
       <c r="R98" t="n">
-        <v>2.47</v>
+        <v>4.52</v>
       </c>
       <c r="S98" t="inlineStr">
         <is>
@@ -9460,7 +9460,7 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>2.59</v>
+        <v>5.03</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
@@ -9469,7 +9469,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
         </is>
       </c>
     </row>
@@ -9497,7 +9497,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G99" t="n">
@@ -9505,14 +9505,14 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I99" t="n">
         <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>1.93</v>
+        <v>3.31</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -9520,7 +9520,7 @@
         </is>
       </c>
       <c r="L99" t="n">
-        <v>1.91</v>
+        <v>3.28</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
@@ -9528,7 +9528,7 @@
         </is>
       </c>
       <c r="N99" t="n">
-        <v>3.29</v>
+        <v>2.97</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -9536,7 +9536,7 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>3.2</v>
+        <v>2.93</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
@@ -9544,7 +9544,7 @@
         </is>
       </c>
       <c r="R99" t="n">
-        <v>4.52</v>
+        <v>2.47</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
@@ -9552,7 +9552,7 @@
         </is>
       </c>
       <c r="T99" t="n">
-        <v>5.03</v>
+        <v>2.59</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
@@ -9561,7 +9561,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,63 +9781,63 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J102" t="n">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>2.17</v>
+        <v>1.9</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.37</v>
+        <v>3.58</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.06</v>
+        <v>3.47</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>4.33</v>
+        <v>4.7</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>4.04</v>
+        <v>4.55</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -9873,63 +9873,63 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J103" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>1.9</v>
+        <v>2.17</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.58</v>
+        <v>3.37</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.47</v>
+        <v>3.06</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>4.7</v>
+        <v>4.33</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4.55</v>
+        <v>4.04</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
         </is>
       </c>
     </row>
@@ -12414,6 +12414,374 @@
       <c r="V130" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-gimnasia-l-p/Or5Z6WFo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E131" s="2" t="n">
+        <v>45223.91666666666</v>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Union de Santa Fe</t>
+        </is>
+      </c>
+      <c r="G131" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Defensa y Justicia</t>
+        </is>
+      </c>
+      <c r="I131" t="n">
+        <v>0</v>
+      </c>
+      <c r="J131" t="n">
+        <v>2</v>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>21/10/2023 01:42</t>
+        </is>
+      </c>
+      <c r="L131" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>24/10/2023 21:57</t>
+        </is>
+      </c>
+      <c r="N131" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>21/10/2023 01:42</t>
+        </is>
+      </c>
+      <c r="P131" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>24/10/2023 21:57</t>
+        </is>
+      </c>
+      <c r="R131" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="S131" t="inlineStr">
+        <is>
+          <t>21/10/2023 01:42</t>
+        </is>
+      </c>
+      <c r="T131" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="U131" t="inlineStr">
+        <is>
+          <t>24/10/2023 21:57</t>
+        </is>
+      </c>
+      <c r="V131" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-defensa-y-justicia/4b0f28UG/</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E132" s="2" t="n">
+        <v>45224</v>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Racing Club</t>
+        </is>
+      </c>
+      <c r="G132" t="n">
+        <v>2</v>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>Boca Juniors</t>
+        </is>
+      </c>
+      <c r="I132" t="n">
+        <v>1</v>
+      </c>
+      <c r="J132" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>21/10/2023 01:42</t>
+        </is>
+      </c>
+      <c r="L132" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>24/10/2023 23:59</t>
+        </is>
+      </c>
+      <c r="N132" t="n">
+        <v>3</v>
+      </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>21/10/2023 01:42</t>
+        </is>
+      </c>
+      <c r="P132" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>24/10/2023 23:59</t>
+        </is>
+      </c>
+      <c r="R132" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="S132" t="inlineStr">
+        <is>
+          <t>21/10/2023 01:42</t>
+        </is>
+      </c>
+      <c r="T132" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="U132" t="inlineStr">
+        <is>
+          <t>24/10/2023 23:59</t>
+        </is>
+      </c>
+      <c r="V132" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-boca-juniors/nNka1SqN/</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E133" s="2" t="n">
+        <v>45224.10416666666</v>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Instituto</t>
+        </is>
+      </c>
+      <c r="G133" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>Rosario Central</t>
+        </is>
+      </c>
+      <c r="I133" t="n">
+        <v>0</v>
+      </c>
+      <c r="J133" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L133" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:29</t>
+        </is>
+      </c>
+      <c r="N133" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P133" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:26</t>
+        </is>
+      </c>
+      <c r="R133" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="S133" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T133" t="n">
+        <v>4.84</v>
+      </c>
+      <c r="U133" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:29</t>
+        </is>
+      </c>
+      <c r="V133" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E134" s="2" t="n">
+        <v>45224.10416666666</v>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Argentinos Jrs</t>
+        </is>
+      </c>
+      <c r="G134" t="n">
+        <v>1</v>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="I134" t="n">
+        <v>2</v>
+      </c>
+      <c r="J134" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L134" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:23</t>
+        </is>
+      </c>
+      <c r="N134" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P134" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:23</t>
+        </is>
+      </c>
+      <c r="R134" t="n">
+        <v>4.51</v>
+      </c>
+      <c r="S134" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T134" t="n">
+        <v>5.33</v>
+      </c>
+      <c r="U134" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:27</t>
+        </is>
+      </c>
+      <c r="V134" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 25-10-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V134"/>
+  <dimension ref="A1:V135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9957,22 +9957,22 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Independiente</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I104" t="n">
         <v>0</v>
       </c>
       <c r="J104" t="n">
-        <v>1.84</v>
+        <v>2.85</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -9980,7 +9980,7 @@
         </is>
       </c>
       <c r="L104" t="n">
-        <v>2.1</v>
+        <v>3.4</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
@@ -9988,7 +9988,7 @@
         </is>
       </c>
       <c r="N104" t="n">
-        <v>3.42</v>
+        <v>3.01</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -9996,32 +9996,32 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>3.09</v>
+        <v>3.02</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
+          <t>08/10/2023 02:26</t>
+        </is>
+      </c>
+      <c r="R104" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>03/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T104" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="U104" t="inlineStr">
+        <is>
           <t>08/10/2023 02:29</t>
         </is>
       </c>
-      <c r="R104" t="n">
-        <v>4.38</v>
-      </c>
-      <c r="S104" t="inlineStr">
-        <is>
-          <t>03/10/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T104" t="n">
-        <v>4.26</v>
-      </c>
-      <c r="U104" t="inlineStr">
-        <is>
-          <t>08/10/2023 02:29</t>
-        </is>
-      </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-independiente/ba6Jq3IK/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-tigre/KA8nw1el/</t>
         </is>
       </c>
     </row>
@@ -10049,22 +10049,22 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Independiente</t>
         </is>
       </c>
       <c r="I105" t="n">
         <v>0</v>
       </c>
       <c r="J105" t="n">
-        <v>2.85</v>
+        <v>1.84</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
@@ -10072,7 +10072,7 @@
         </is>
       </c>
       <c r="L105" t="n">
-        <v>3.4</v>
+        <v>2.1</v>
       </c>
       <c r="M105" t="inlineStr">
         <is>
@@ -10080,7 +10080,7 @@
         </is>
       </c>
       <c r="N105" t="n">
-        <v>3.01</v>
+        <v>3.42</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -10088,15 +10088,15 @@
         </is>
       </c>
       <c r="P105" t="n">
-        <v>3.02</v>
+        <v>3.09</v>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>08/10/2023 02:26</t>
+          <t>08/10/2023 02:29</t>
         </is>
       </c>
       <c r="R105" t="n">
-        <v>2.79</v>
+        <v>4.38</v>
       </c>
       <c r="S105" t="inlineStr">
         <is>
@@ -10104,7 +10104,7 @@
         </is>
       </c>
       <c r="T105" t="n">
-        <v>2.45</v>
+        <v>4.26</v>
       </c>
       <c r="U105" t="inlineStr">
         <is>
@@ -10113,7 +10113,7 @@
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-tigre/KA8nw1el/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-independiente/ba6Jq3IK/</t>
         </is>
       </c>
     </row>
@@ -12782,6 +12782,98 @@
       <c r="V134" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E135" s="2" t="n">
+        <v>45224.875</v>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Arsenal Sarandi</t>
+        </is>
+      </c>
+      <c r="G135" t="n">
+        <v>1</v>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Colon Santa Fe</t>
+        </is>
+      </c>
+      <c r="I135" t="n">
+        <v>0</v>
+      </c>
+      <c r="J135" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L135" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>25/10/2023 20:55</t>
+        </is>
+      </c>
+      <c r="N135" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="O135" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P135" t="n">
+        <v>3.02</v>
+      </c>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>25/10/2023 20:55</t>
+        </is>
+      </c>
+      <c r="R135" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="S135" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T135" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="U135" t="inlineStr">
+        <is>
+          <t>25/10/2023 20:55</t>
+        </is>
+      </c>
+      <c r="V135" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-colon-santa-fe/8WUPnTUT/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 26-10-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V135"/>
+  <dimension ref="A1:V138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3333,22 +3333,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I32" t="n">
         <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>2.74</v>
+        <v>1.98</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -3356,15 +3356,15 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>2.85</v>
+        <v>2.12</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>2.8</v>
+        <v>3.19</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3372,15 +3372,15 @@
         </is>
       </c>
       <c r="P32" t="n">
-        <v>2.67</v>
+        <v>2.93</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>3.12</v>
+        <v>4.44</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
@@ -3388,16 +3388,16 @@
         </is>
       </c>
       <c r="T32" t="n">
-        <v>3.25</v>
+        <v>4.54</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-newells-old-boys/plSOG3km/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-colon-santa-fe/xr5c0r56/</t>
         </is>
       </c>
     </row>
@@ -3425,22 +3425,22 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="I33" t="n">
         <v>1</v>
       </c>
       <c r="J33" t="n">
-        <v>1.98</v>
+        <v>2.74</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -3448,15 +3448,15 @@
         </is>
       </c>
       <c r="L33" t="n">
-        <v>2.12</v>
+        <v>2.85</v>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="N33" t="n">
-        <v>3.19</v>
+        <v>2.8</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -3464,15 +3464,15 @@
         </is>
       </c>
       <c r="P33" t="n">
-        <v>2.93</v>
+        <v>2.67</v>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="R33" t="n">
-        <v>4.44</v>
+        <v>3.12</v>
       </c>
       <c r="S33" t="inlineStr">
         <is>
@@ -3480,16 +3480,16 @@
         </is>
       </c>
       <c r="T33" t="n">
-        <v>4.54</v>
+        <v>3.25</v>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-colon-santa-fe/xr5c0r56/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-newells-old-boys/plSOG3km/</t>
         </is>
       </c>
     </row>
@@ -3609,71 +3609,71 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I35" t="n">
         <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>1.97</v>
+        <v>2.38</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>2.41</v>
+        <v>2.45</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="N35" t="n">
-        <v>3.39</v>
+        <v>2.92</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="P35" t="n">
-        <v>3.13</v>
+        <v>2.74</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="R35" t="n">
-        <v>4.13</v>
+        <v>3.56</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="T35" t="n">
-        <v>3.35</v>
+        <v>3.85</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-sarmiento-junin/nDnlN5CJ/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-banfield/Wp2k24zf/</t>
         </is>
       </c>
     </row>
@@ -3701,71 +3701,71 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>2.38</v>
+        <v>1.97</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>2.45</v>
+        <v>2.41</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="N36" t="n">
-        <v>2.92</v>
+        <v>3.39</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="P36" t="n">
-        <v>2.74</v>
+        <v>3.13</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="R36" t="n">
-        <v>3.56</v>
+        <v>4.13</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="T36" t="n">
-        <v>3.85</v>
+        <v>3.35</v>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-banfield/Wp2k24zf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-sarmiento-junin/nDnlN5CJ/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,63 +9781,63 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J102" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>1.9</v>
+        <v>2.17</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.58</v>
+        <v>3.37</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.47</v>
+        <v>3.06</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>4.7</v>
+        <v>4.33</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>4.55</v>
+        <v>4.04</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -9873,63 +9873,63 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J103" t="n">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>2.17</v>
+        <v>1.9</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.37</v>
+        <v>3.58</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.06</v>
+        <v>3.47</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>4.33</v>
+        <v>4.7</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4.04</v>
+        <v>4.55</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
         </is>
       </c>
     </row>
@@ -12625,22 +12625,22 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="I133" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J133" t="n">
-        <v>2.08</v>
+        <v>1.88</v>
       </c>
       <c r="K133" t="inlineStr">
         <is>
@@ -12648,15 +12648,15 @@
         </is>
       </c>
       <c r="L133" t="n">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="N133" t="n">
-        <v>3.15</v>
+        <v>3.23</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -12664,15 +12664,15 @@
         </is>
       </c>
       <c r="P133" t="n">
-        <v>3.15</v>
+        <v>3.11</v>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:26</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="R133" t="n">
-        <v>4.07</v>
+        <v>4.51</v>
       </c>
       <c r="S133" t="inlineStr">
         <is>
@@ -12680,16 +12680,16 @@
         </is>
       </c>
       <c r="T133" t="n">
-        <v>4.84</v>
+        <v>5.33</v>
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:27</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
         </is>
       </c>
     </row>
@@ -12717,22 +12717,22 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="I134" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J134" t="n">
-        <v>1.88</v>
+        <v>2.08</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>3.23</v>
+        <v>3.15</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>3.11</v>
+        <v>3.15</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:26</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>4.51</v>
+        <v>4.07</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>5.33</v>
+        <v>4.84</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:27</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
         </is>
       </c>
     </row>
@@ -12874,6 +12874,282 @@
       <c r="V135" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-colon-santa-fe/8WUPnTUT/</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E136" s="2" t="n">
+        <v>45224.97916666666</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Atl. Tucuman</t>
+        </is>
+      </c>
+      <c r="G136" t="n">
+        <v>1</v>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>Talleres Cordoba</t>
+        </is>
+      </c>
+      <c r="I136" t="n">
+        <v>0</v>
+      </c>
+      <c r="J136" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L136" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:27</t>
+        </is>
+      </c>
+      <c r="N136" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P136" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:27</t>
+        </is>
+      </c>
+      <c r="R136" t="n">
+        <v>2.78</v>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>20/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T136" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="U136" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:27</t>
+        </is>
+      </c>
+      <c r="V136" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E137" s="2" t="n">
+        <v>45224.97916666666</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Belgrano</t>
+        </is>
+      </c>
+      <c r="G137" t="n">
+        <v>1</v>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Central Cordoba</t>
+        </is>
+      </c>
+      <c r="I137" t="n">
+        <v>1</v>
+      </c>
+      <c r="J137" t="n">
+        <v>1.94</v>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:42</t>
+        </is>
+      </c>
+      <c r="L137" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:26</t>
+        </is>
+      </c>
+      <c r="N137" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="O137" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:42</t>
+        </is>
+      </c>
+      <c r="P137" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="Q137" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:26</t>
+        </is>
+      </c>
+      <c r="R137" t="n">
+        <v>4.62</v>
+      </c>
+      <c r="S137" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:42</t>
+        </is>
+      </c>
+      <c r="T137" t="n">
+        <v>5.29</v>
+      </c>
+      <c r="U137" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:26</t>
+        </is>
+      </c>
+      <c r="V137" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E138" s="2" t="n">
+        <v>45225.08333333334</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>River Plate</t>
+        </is>
+      </c>
+      <c r="G138" t="n">
+        <v>3</v>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Independiente</t>
+        </is>
+      </c>
+      <c r="I138" t="n">
+        <v>0</v>
+      </c>
+      <c r="J138" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>19/10/2023 22:42</t>
+        </is>
+      </c>
+      <c r="L138" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>26/10/2023 01:59</t>
+        </is>
+      </c>
+      <c r="N138" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>19/10/2023 22:42</t>
+        </is>
+      </c>
+      <c r="P138" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>26/10/2023 01:59</t>
+        </is>
+      </c>
+      <c r="R138" t="n">
+        <v>7.52</v>
+      </c>
+      <c r="S138" t="inlineStr">
+        <is>
+          <t>19/10/2023 22:42</t>
+        </is>
+      </c>
+      <c r="T138" t="n">
+        <v>5.51</v>
+      </c>
+      <c r="U138" t="inlineStr">
+        <is>
+          <t>26/10/2023 01:59</t>
+        </is>
+      </c>
+      <c r="V138" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/river-plate-independiente/AuHirmwo/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 27-10-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V138"/>
+  <dimension ref="A1:V141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3333,22 +3333,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="I32" t="n">
         <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>1.98</v>
+        <v>2.74</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -3356,15 +3356,15 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>2.12</v>
+        <v>2.85</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>3.19</v>
+        <v>2.8</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3372,15 +3372,15 @@
         </is>
       </c>
       <c r="P32" t="n">
-        <v>2.93</v>
+        <v>2.67</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>4.44</v>
+        <v>3.12</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
@@ -3388,16 +3388,16 @@
         </is>
       </c>
       <c r="T32" t="n">
-        <v>4.54</v>
+        <v>3.25</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-colon-santa-fe/xr5c0r56/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-newells-old-boys/plSOG3km/</t>
         </is>
       </c>
     </row>
@@ -3425,22 +3425,22 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I33" t="n">
         <v>1</v>
       </c>
       <c r="J33" t="n">
-        <v>2.74</v>
+        <v>1.98</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -3448,15 +3448,15 @@
         </is>
       </c>
       <c r="L33" t="n">
-        <v>2.85</v>
+        <v>2.12</v>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="N33" t="n">
-        <v>2.8</v>
+        <v>3.19</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -3464,15 +3464,15 @@
         </is>
       </c>
       <c r="P33" t="n">
-        <v>2.67</v>
+        <v>2.93</v>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="R33" t="n">
-        <v>3.12</v>
+        <v>4.44</v>
       </c>
       <c r="S33" t="inlineStr">
         <is>
@@ -3480,16 +3480,16 @@
         </is>
       </c>
       <c r="T33" t="n">
-        <v>3.25</v>
+        <v>4.54</v>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-newells-old-boys/plSOG3km/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-colon-santa-fe/xr5c0r56/</t>
         </is>
       </c>
     </row>
@@ -3609,71 +3609,71 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I35" t="n">
         <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>2.38</v>
+        <v>1.97</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>2.45</v>
+        <v>2.41</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="N35" t="n">
-        <v>2.92</v>
+        <v>3.39</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="P35" t="n">
-        <v>2.74</v>
+        <v>3.13</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="R35" t="n">
-        <v>3.56</v>
+        <v>4.13</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="T35" t="n">
-        <v>3.85</v>
+        <v>3.35</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-banfield/Wp2k24zf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-sarmiento-junin/nDnlN5CJ/</t>
         </is>
       </c>
     </row>
@@ -3701,71 +3701,71 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>1.97</v>
+        <v>2.38</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>2.41</v>
+        <v>2.45</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="N36" t="n">
-        <v>3.39</v>
+        <v>2.92</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="P36" t="n">
-        <v>3.13</v>
+        <v>2.74</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="R36" t="n">
-        <v>4.13</v>
+        <v>3.56</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="T36" t="n">
-        <v>3.35</v>
+        <v>3.85</v>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-sarmiento-junin/nDnlN5CJ/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-banfield/Wp2k24zf/</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -9229,22 +9229,22 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>2.25</v>
+        <v>2.3</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.49</v>
+        <v>2.14</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
@@ -9252,15 +9252,15 @@
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.04</v>
+        <v>3.05</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="P96" t="n">
-        <v>2.86</v>
+        <v>3.03</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
@@ -9268,15 +9268,15 @@
         </is>
       </c>
       <c r="R96" t="n">
-        <v>3.7</v>
+        <v>3.54</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="T96" t="n">
-        <v>3.54</v>
+        <v>4.22</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
         </is>
       </c>
     </row>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -9321,22 +9321,22 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>2.3</v>
+        <v>2.25</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>2.14</v>
+        <v>2.49</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
@@ -9344,15 +9344,15 @@
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.05</v>
+        <v>3.04</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>3.03</v>
+        <v>2.86</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
@@ -9360,16 +9360,16 @@
         </is>
       </c>
       <c r="R97" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>25/09/2023 22:42</t>
+        </is>
+      </c>
+      <c r="T97" t="n">
         <v>3.54</v>
       </c>
-      <c r="S97" t="inlineStr">
-        <is>
-          <t>26/09/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T97" t="n">
-        <v>4.22</v>
-      </c>
       <c r="U97" t="inlineStr">
         <is>
           <t>02/10/2023 23:29</t>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
         </is>
       </c>
     </row>
@@ -9957,22 +9957,22 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Independiente</t>
         </is>
       </c>
       <c r="I104" t="n">
         <v>0</v>
       </c>
       <c r="J104" t="n">
-        <v>2.85</v>
+        <v>1.84</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -9980,7 +9980,7 @@
         </is>
       </c>
       <c r="L104" t="n">
-        <v>3.4</v>
+        <v>2.1</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
@@ -9988,7 +9988,7 @@
         </is>
       </c>
       <c r="N104" t="n">
-        <v>3.01</v>
+        <v>3.42</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -9996,15 +9996,15 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>3.02</v>
+        <v>3.09</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>08/10/2023 02:26</t>
+          <t>08/10/2023 02:29</t>
         </is>
       </c>
       <c r="R104" t="n">
-        <v>2.79</v>
+        <v>4.38</v>
       </c>
       <c r="S104" t="inlineStr">
         <is>
@@ -10012,7 +10012,7 @@
         </is>
       </c>
       <c r="T104" t="n">
-        <v>2.45</v>
+        <v>4.26</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
@@ -10021,7 +10021,7 @@
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-tigre/KA8nw1el/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-independiente/ba6Jq3IK/</t>
         </is>
       </c>
     </row>
@@ -10049,22 +10049,22 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="G105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Independiente</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I105" t="n">
         <v>0</v>
       </c>
       <c r="J105" t="n">
-        <v>1.84</v>
+        <v>2.85</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
@@ -10072,7 +10072,7 @@
         </is>
       </c>
       <c r="L105" t="n">
-        <v>2.1</v>
+        <v>3.4</v>
       </c>
       <c r="M105" t="inlineStr">
         <is>
@@ -10080,7 +10080,7 @@
         </is>
       </c>
       <c r="N105" t="n">
-        <v>3.42</v>
+        <v>3.01</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -10088,32 +10088,32 @@
         </is>
       </c>
       <c r="P105" t="n">
-        <v>3.09</v>
+        <v>3.02</v>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
+          <t>08/10/2023 02:26</t>
+        </is>
+      </c>
+      <c r="R105" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>03/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T105" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="U105" t="inlineStr">
+        <is>
           <t>08/10/2023 02:29</t>
         </is>
       </c>
-      <c r="R105" t="n">
-        <v>4.38</v>
-      </c>
-      <c r="S105" t="inlineStr">
-        <is>
-          <t>03/10/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T105" t="n">
-        <v>4.26</v>
-      </c>
-      <c r="U105" t="inlineStr">
-        <is>
-          <t>08/10/2023 02:29</t>
-        </is>
-      </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-independiente/ba6Jq3IK/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-tigre/KA8nw1el/</t>
         </is>
       </c>
     </row>
@@ -13150,6 +13150,282 @@
       <c r="V138" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/river-plate-independiente/AuHirmwo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E139" s="2" t="n">
+        <v>45225.97916666666</v>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="G139" t="n">
+        <v>1</v>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>Platense</t>
+        </is>
+      </c>
+      <c r="I139" t="n">
+        <v>1</v>
+      </c>
+      <c r="J139" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>19/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L139" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>26/10/2023 23:28</t>
+        </is>
+      </c>
+      <c r="N139" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="O139" t="inlineStr">
+        <is>
+          <t>19/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P139" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>26/10/2023 23:28</t>
+        </is>
+      </c>
+      <c r="R139" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="S139" t="inlineStr">
+        <is>
+          <t>19/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T139" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="U139" t="inlineStr">
+        <is>
+          <t>26/10/2023 23:28</t>
+        </is>
+      </c>
+      <c r="V139" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/san-lorenzo-platense/I5tVe67p/</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E140" s="2" t="n">
+        <v>45226.08333333334</v>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Newells Old Boys</t>
+        </is>
+      </c>
+      <c r="G140" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="I140" t="n">
+        <v>2</v>
+      </c>
+      <c r="J140" t="n">
+        <v>2</v>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>20/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L140" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:34</t>
+        </is>
+      </c>
+      <c r="N140" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>20/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P140" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:34</t>
+        </is>
+      </c>
+      <c r="R140" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>20/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T140" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="U140" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:34</t>
+        </is>
+      </c>
+      <c r="V140" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-godoy-cruz/dduZfQMj/</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E141" s="2" t="n">
+        <v>45226.08333333334</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Lanus</t>
+        </is>
+      </c>
+      <c r="G141" t="n">
+        <v>2</v>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Tigre</t>
+        </is>
+      </c>
+      <c r="I141" t="n">
+        <v>1</v>
+      </c>
+      <c r="J141" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>20/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L141" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:59</t>
+        </is>
+      </c>
+      <c r="N141" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>20/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P141" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="Q141" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:28</t>
+        </is>
+      </c>
+      <c r="R141" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="S141" t="inlineStr">
+        <is>
+          <t>20/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T141" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="U141" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:56</t>
+        </is>
+      </c>
+      <c r="V141" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-tigre/dYdn4Ua4/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 31-10-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V141"/>
+  <dimension ref="A1:V152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2137,71 +2137,71 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>1.74</v>
+        <v>2.19</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>1.94</v>
+        <v>2.09</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:43</t>
         </is>
       </c>
       <c r="N19" t="n">
-        <v>3.44</v>
+        <v>2.94</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="P19" t="n">
-        <v>3.23</v>
+        <v>3.01</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:43</t>
         </is>
       </c>
       <c r="R19" t="n">
-        <v>5.57</v>
+        <v>3.79</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="T19" t="n">
-        <v>4.73</v>
+        <v>4.48</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:42</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-huracan/l4ycuMBq/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-lanus/OdYgrAqL/</t>
         </is>
       </c>
     </row>
@@ -2229,71 +2229,71 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G20" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
         <v>1</v>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Lanus</t>
-        </is>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
       <c r="J20" t="n">
-        <v>2.19</v>
+        <v>1.74</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>2.09</v>
+        <v>1.94</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:43</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="N20" t="n">
-        <v>2.94</v>
+        <v>3.44</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="P20" t="n">
-        <v>3.01</v>
+        <v>3.23</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:43</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="R20" t="n">
-        <v>3.79</v>
+        <v>5.57</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="T20" t="n">
-        <v>4.48</v>
+        <v>4.73</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:42</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-lanus/OdYgrAqL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-huracan/l4ycuMBq/</t>
         </is>
       </c>
     </row>
@@ -2413,71 +2413,71 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>2.61</v>
+        <v>1.87</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>2.08</v>
+        <v>1.85</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:27</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.05</v>
+        <v>3.32</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.11</v>
+        <v>3.44</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:22</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>2.86</v>
+        <v>4.39</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="T22" t="n">
-        <v>4.32</v>
+        <v>4.87</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:27</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-defensa-y-justicia/8U9Qxl7r/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-central-cordoba-santiago-del-estero/6LNbsUbR/</t>
         </is>
       </c>
     </row>
@@ -2505,71 +2505,71 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>1.87</v>
+        <v>2.61</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>1.85</v>
+        <v>2.08</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:27</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>3.32</v>
+        <v>3.05</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.44</v>
+        <v>3.11</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:22</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>4.39</v>
+        <v>2.86</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="T23" t="n">
-        <v>4.87</v>
+        <v>4.32</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:27</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-central-cordoba-santiago-del-estero/6LNbsUbR/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-defensa-y-justicia/8U9Qxl7r/</t>
         </is>
       </c>
     </row>
@@ -3333,22 +3333,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I32" t="n">
         <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>2.74</v>
+        <v>1.98</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -3356,15 +3356,15 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>2.85</v>
+        <v>2.12</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>2.8</v>
+        <v>3.19</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3372,15 +3372,15 @@
         </is>
       </c>
       <c r="P32" t="n">
-        <v>2.67</v>
+        <v>2.93</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>3.12</v>
+        <v>4.44</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
@@ -3388,16 +3388,16 @@
         </is>
       </c>
       <c r="T32" t="n">
-        <v>3.25</v>
+        <v>4.54</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-newells-old-boys/plSOG3km/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-colon-santa-fe/xr5c0r56/</t>
         </is>
       </c>
     </row>
@@ -3425,22 +3425,22 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="I33" t="n">
         <v>1</v>
       </c>
       <c r="J33" t="n">
-        <v>1.98</v>
+        <v>2.74</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -3448,15 +3448,15 @@
         </is>
       </c>
       <c r="L33" t="n">
-        <v>2.12</v>
+        <v>2.85</v>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="N33" t="n">
-        <v>3.19</v>
+        <v>2.8</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -3464,15 +3464,15 @@
         </is>
       </c>
       <c r="P33" t="n">
-        <v>2.93</v>
+        <v>2.67</v>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="R33" t="n">
-        <v>4.44</v>
+        <v>3.12</v>
       </c>
       <c r="S33" t="inlineStr">
         <is>
@@ -3480,16 +3480,16 @@
         </is>
       </c>
       <c r="T33" t="n">
-        <v>4.54</v>
+        <v>3.25</v>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-colon-santa-fe/xr5c0r56/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-newells-old-boys/plSOG3km/</t>
         </is>
       </c>
     </row>
@@ -3609,71 +3609,71 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I35" t="n">
         <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>1.97</v>
+        <v>2.38</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>2.41</v>
+        <v>2.45</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="N35" t="n">
-        <v>3.39</v>
+        <v>2.92</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="P35" t="n">
-        <v>3.13</v>
+        <v>2.74</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="R35" t="n">
-        <v>4.13</v>
+        <v>3.56</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="T35" t="n">
-        <v>3.35</v>
+        <v>3.85</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-sarmiento-junin/nDnlN5CJ/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-banfield/Wp2k24zf/</t>
         </is>
       </c>
     </row>
@@ -3701,71 +3701,71 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>2.38</v>
+        <v>1.97</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>2.45</v>
+        <v>2.41</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="N36" t="n">
-        <v>2.92</v>
+        <v>3.39</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="P36" t="n">
-        <v>2.74</v>
+        <v>3.13</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="R36" t="n">
-        <v>3.56</v>
+        <v>4.13</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="T36" t="n">
-        <v>3.85</v>
+        <v>3.35</v>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-banfield/Wp2k24zf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-sarmiento-junin/nDnlN5CJ/</t>
         </is>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -3801,38 +3801,38 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J37" t="n">
-        <v>2.67</v>
+        <v>1.76</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>3.38</v>
+        <v>1.75</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>03/09/2023 21:07</t>
+          <t>03/09/2023 21:13</t>
         </is>
       </c>
       <c r="N37" t="n">
-        <v>3.13</v>
+        <v>3.56</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="P37" t="n">
-        <v>3.18</v>
+        <v>3.46</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
@@ -3840,15 +3840,15 @@
         </is>
       </c>
       <c r="R37" t="n">
-        <v>2.73</v>
+        <v>5.34</v>
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="T37" t="n">
-        <v>2.36</v>
+        <v>5.63</v>
       </c>
       <c r="U37" t="inlineStr">
         <is>
@@ -3857,7 +3857,7 @@
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
         </is>
       </c>
     </row>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -3893,63 +3893,63 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>1.76</v>
+        <v>2.67</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>29/08/2023 00:12</t>
         </is>
       </c>
       <c r="L38" t="n">
-        <v>1.75</v>
+        <v>3.38</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
+          <t>03/09/2023 21:07</t>
+        </is>
+      </c>
+      <c r="N38" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P38" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="N38" t="n">
-        <v>3.56</v>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="P38" t="n">
-        <v>3.46</v>
-      </c>
-      <c r="Q38" t="inlineStr">
+      <c r="R38" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T38" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="U38" t="inlineStr">
         <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="R38" t="n">
-        <v>5.34</v>
-      </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="T38" t="n">
-        <v>5.63</v>
-      </c>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>03/09/2023 21:13</t>
-        </is>
-      </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
         </is>
       </c>
     </row>
@@ -4989,22 +4989,22 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="I50" t="n">
         <v>1</v>
       </c>
       <c r="J50" t="n">
-        <v>2.74</v>
+        <v>2.49</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -5012,15 +5012,15 @@
         </is>
       </c>
       <c r="L50" t="n">
-        <v>3.68</v>
+        <v>2.44</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>16/09/2023 01:58</t>
+          <t>16/09/2023 01:50</t>
         </is>
       </c>
       <c r="N50" t="n">
-        <v>2.93</v>
+        <v>3.13</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -5028,15 +5028,15 @@
         </is>
       </c>
       <c r="P50" t="n">
-        <v>2.98</v>
+        <v>3.2</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>16/09/2023 01:58</t>
+          <t>16/09/2023 01:59</t>
         </is>
       </c>
       <c r="R50" t="n">
-        <v>2.82</v>
+        <v>3.1</v>
       </c>
       <c r="S50" t="inlineStr">
         <is>
@@ -5044,16 +5044,16 @@
         </is>
       </c>
       <c r="T50" t="n">
-        <v>2.35</v>
+        <v>3.23</v>
       </c>
       <c r="U50" t="inlineStr">
         <is>
-          <t>16/09/2023 01:58</t>
+          <t>16/09/2023 01:59</t>
         </is>
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-argentinos-jrs/6Z2XeTDK/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-rosario-central/A79Ockq8/</t>
         </is>
       </c>
     </row>
@@ -5081,22 +5081,22 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I51" t="n">
         <v>1</v>
       </c>
       <c r="J51" t="n">
-        <v>2.49</v>
+        <v>2.74</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -5104,15 +5104,15 @@
         </is>
       </c>
       <c r="L51" t="n">
-        <v>2.44</v>
+        <v>3.68</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>16/09/2023 01:50</t>
+          <t>16/09/2023 01:58</t>
         </is>
       </c>
       <c r="N51" t="n">
-        <v>3.13</v>
+        <v>2.93</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -5120,15 +5120,15 @@
         </is>
       </c>
       <c r="P51" t="n">
-        <v>3.2</v>
+        <v>2.98</v>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>16/09/2023 01:59</t>
+          <t>16/09/2023 01:58</t>
         </is>
       </c>
       <c r="R51" t="n">
-        <v>3.1</v>
+        <v>2.82</v>
       </c>
       <c r="S51" t="inlineStr">
         <is>
@@ -5136,16 +5136,16 @@
         </is>
       </c>
       <c r="T51" t="n">
-        <v>3.23</v>
+        <v>2.35</v>
       </c>
       <c r="U51" t="inlineStr">
         <is>
-          <t>16/09/2023 01:59</t>
+          <t>16/09/2023 01:58</t>
         </is>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-rosario-central/A79Ockq8/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-argentinos-jrs/6Z2XeTDK/</t>
         </is>
       </c>
     </row>
@@ -5909,30 +5909,30 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Gimnasia L.P.</t>
+          <t>Independiente</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" t="n">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>15/09/2023 01:13</t>
+          <t>16/09/2023 01:13</t>
         </is>
       </c>
       <c r="L60" t="n">
-        <v>1.9</v>
+        <v>2.78</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
@@ -5940,15 +5940,15 @@
         </is>
       </c>
       <c r="N60" t="n">
-        <v>3.3</v>
+        <v>3.12</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>15/09/2023 01:13</t>
+          <t>16/09/2023 01:13</t>
         </is>
       </c>
       <c r="P60" t="n">
-        <v>3.1</v>
+        <v>3.02</v>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
@@ -5956,15 +5956,15 @@
         </is>
       </c>
       <c r="R60" t="n">
-        <v>4.82</v>
+        <v>4.04</v>
       </c>
       <c r="S60" t="inlineStr">
         <is>
-          <t>15/09/2023 01:13</t>
+          <t>16/09/2023 01:13</t>
         </is>
       </c>
       <c r="T60" t="n">
-        <v>5.38</v>
+        <v>2.93</v>
       </c>
       <c r="U60" t="inlineStr">
         <is>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-gimnasia-l-p/IZ3aGfe4/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-independiente/vq5eHztb/</t>
         </is>
       </c>
     </row>
@@ -6001,30 +6001,30 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Independiente</t>
+          <t>Gimnasia L.P.</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>16/09/2023 01:13</t>
+          <t>15/09/2023 01:13</t>
         </is>
       </c>
       <c r="L61" t="n">
-        <v>2.78</v>
+        <v>1.9</v>
       </c>
       <c r="M61" t="inlineStr">
         <is>
@@ -6032,15 +6032,15 @@
         </is>
       </c>
       <c r="N61" t="n">
-        <v>3.12</v>
+        <v>3.3</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>16/09/2023 01:13</t>
+          <t>15/09/2023 01:13</t>
         </is>
       </c>
       <c r="P61" t="n">
-        <v>3.02</v>
+        <v>3.1</v>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
@@ -6048,15 +6048,15 @@
         </is>
       </c>
       <c r="R61" t="n">
-        <v>4.04</v>
+        <v>4.82</v>
       </c>
       <c r="S61" t="inlineStr">
         <is>
-          <t>16/09/2023 01:13</t>
+          <t>15/09/2023 01:13</t>
         </is>
       </c>
       <c r="T61" t="n">
-        <v>2.93</v>
+        <v>5.38</v>
       </c>
       <c r="U61" t="inlineStr">
         <is>
@@ -6065,7 +6065,7 @@
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-independiente/vq5eHztb/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-gimnasia-l-p/IZ3aGfe4/</t>
         </is>
       </c>
     </row>
@@ -7749,34 +7749,34 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="I80" t="n">
         <v>0</v>
       </c>
       <c r="J80" t="n">
-        <v>2.37</v>
+        <v>2.64</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>3.16</v>
+        <v>2.59</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="N80" t="n">
@@ -7784,11 +7784,11 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="P80" t="n">
-        <v>2.72</v>
+        <v>2.77</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
@@ -7796,24 +7796,24 @@
         </is>
       </c>
       <c r="R80" t="n">
-        <v>3.51</v>
+        <v>2.9</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="T80" t="n">
-        <v>2.86</v>
+        <v>3.5</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
         </is>
       </c>
     </row>
@@ -7841,34 +7841,34 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="I81" t="n">
         <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>2.64</v>
+        <v>2.37</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>2.59</v>
+        <v>3.16</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="N81" t="n">
@@ -7876,11 +7876,11 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="P81" t="n">
-        <v>2.77</v>
+        <v>2.72</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
@@ -7888,24 +7888,24 @@
         </is>
       </c>
       <c r="R81" t="n">
-        <v>2.9</v>
+        <v>3.51</v>
       </c>
       <c r="S81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="T81" t="n">
-        <v>3.5</v>
+        <v>2.86</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
         </is>
       </c>
     </row>
@@ -7933,71 +7933,71 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Racing Club</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I82" t="n">
         <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>2.34</v>
+        <v>3.03</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>24/09/2023 05:42</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="L82" t="n">
-        <v>2.29</v>
+        <v>2.95</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
+          <t>25/09/2023 23:25</t>
+        </is>
+      </c>
+      <c r="N82" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>21/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P82" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>25/09/2023 23:20</t>
+        </is>
+      </c>
+      <c r="R82" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>21/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T82" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
           <t>25/09/2023 23:29</t>
         </is>
       </c>
-      <c r="N82" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>24/09/2023 05:42</t>
-        </is>
-      </c>
-      <c r="P82" t="n">
-        <v>3.36</v>
-      </c>
-      <c r="Q82" t="inlineStr">
-        <is>
-          <t>25/09/2023 23:29</t>
-        </is>
-      </c>
-      <c r="R82" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="S82" t="inlineStr">
-        <is>
-          <t>24/09/2023 05:42</t>
-        </is>
-      </c>
-      <c r="T82" t="n">
-        <v>3.35</v>
-      </c>
-      <c r="U82" t="inlineStr">
-        <is>
-          <t>25/09/2023 23:29</t>
-        </is>
-      </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-racing-club/8OvDrDvc/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-argentinos-jrs/0IHoSifG/</t>
         </is>
       </c>
     </row>
@@ -8025,62 +8025,62 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Racing Club</t>
         </is>
       </c>
       <c r="I83" t="n">
         <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>3.03</v>
+        <v>2.34</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>2.95</v>
+        <v>2.29</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>25/09/2023 23:25</t>
+          <t>25/09/2023 23:29</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>3.09</v>
+        <v>3.2</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="P83" t="n">
-        <v>3.16</v>
+        <v>3.36</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>25/09/2023 23:20</t>
+          <t>25/09/2023 23:29</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>2.46</v>
+        <v>3.3</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="T83" t="n">
-        <v>2.64</v>
+        <v>3.35</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
@@ -8089,7 +8089,7 @@
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-argentinos-jrs/0IHoSifG/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-racing-club/8OvDrDvc/</t>
         </is>
       </c>
     </row>
@@ -8117,30 +8117,30 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I84" t="n">
         <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1.52</v>
+        <v>1.74</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="L84" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
@@ -8148,15 +8148,15 @@
         </is>
       </c>
       <c r="N84" t="n">
-        <v>4.1</v>
+        <v>3.47</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.69</v>
+        <v>3.54</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
@@ -8164,15 +8164,15 @@
         </is>
       </c>
       <c r="R84" t="n">
-        <v>6.9</v>
+        <v>5.5</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="T84" t="n">
-        <v>5.96</v>
+        <v>5.8</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
         </is>
       </c>
     </row>
@@ -8209,30 +8209,30 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="I85" t="n">
         <v>0</v>
       </c>
       <c r="J85" t="n">
-        <v>1.74</v>
+        <v>1.52</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="L85" t="n">
-        <v>1.72</v>
+        <v>1.67</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
@@ -8240,15 +8240,15 @@
         </is>
       </c>
       <c r="N85" t="n">
-        <v>3.47</v>
+        <v>4.1</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.54</v>
+        <v>3.69</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
@@ -8256,15 +8256,15 @@
         </is>
       </c>
       <c r="R85" t="n">
-        <v>5.5</v>
+        <v>6.9</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="T85" t="n">
-        <v>5.8</v>
+        <v>5.96</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
@@ -8273,7 +8273,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -9229,22 +9229,22 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>2.3</v>
+        <v>2.25</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.14</v>
+        <v>2.49</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
@@ -9252,15 +9252,15 @@
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.05</v>
+        <v>3.04</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.03</v>
+        <v>2.86</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
@@ -9268,16 +9268,16 @@
         </is>
       </c>
       <c r="R96" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>25/09/2023 22:42</t>
+        </is>
+      </c>
+      <c r="T96" t="n">
         <v>3.54</v>
       </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>26/09/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T96" t="n">
-        <v>4.22</v>
-      </c>
       <c r="U96" t="inlineStr">
         <is>
           <t>02/10/2023 23:29</t>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
         </is>
       </c>
     </row>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -9321,22 +9321,22 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>2.25</v>
+        <v>2.3</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>2.49</v>
+        <v>2.14</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
@@ -9344,15 +9344,15 @@
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.04</v>
+        <v>3.05</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>2.86</v>
+        <v>3.03</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
@@ -9360,15 +9360,15 @@
         </is>
       </c>
       <c r="R97" t="n">
-        <v>3.7</v>
+        <v>3.54</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="T97" t="n">
-        <v>3.54</v>
+        <v>4.22</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
         </is>
       </c>
     </row>
@@ -12625,22 +12625,22 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="I133" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J133" t="n">
-        <v>1.88</v>
+        <v>2.08</v>
       </c>
       <c r="K133" t="inlineStr">
         <is>
@@ -12648,15 +12648,15 @@
         </is>
       </c>
       <c r="L133" t="n">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="N133" t="n">
-        <v>3.23</v>
+        <v>3.15</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -12664,15 +12664,15 @@
         </is>
       </c>
       <c r="P133" t="n">
-        <v>3.11</v>
+        <v>3.15</v>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:26</t>
         </is>
       </c>
       <c r="R133" t="n">
-        <v>4.51</v>
+        <v>4.07</v>
       </c>
       <c r="S133" t="inlineStr">
         <is>
@@ -12680,16 +12680,16 @@
         </is>
       </c>
       <c r="T133" t="n">
-        <v>5.33</v>
+        <v>4.84</v>
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:27</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
         </is>
       </c>
     </row>
@@ -12717,22 +12717,22 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="I134" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J134" t="n">
-        <v>2.08</v>
+        <v>1.88</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>3.15</v>
+        <v>3.23</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>3.15</v>
+        <v>3.11</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:26</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>4.07</v>
+        <v>4.51</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>4.84</v>
+        <v>5.33</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:27</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
         </is>
       </c>
     </row>
@@ -13269,22 +13269,22 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G140" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I140" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J140" t="n">
-        <v>2</v>
+        <v>2.24</v>
       </c>
       <c r="K140" t="inlineStr">
         <is>
@@ -13292,15 +13292,15 @@
         </is>
       </c>
       <c r="L140" t="n">
-        <v>2.15</v>
+        <v>2.6</v>
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:59</t>
         </is>
       </c>
       <c r="N140" t="n">
-        <v>3.16</v>
+        <v>3.08</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -13308,15 +13308,15 @@
         </is>
       </c>
       <c r="P140" t="n">
-        <v>3.04</v>
+        <v>2.96</v>
       </c>
       <c r="Q140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:28</t>
         </is>
       </c>
       <c r="R140" t="n">
-        <v>4.07</v>
+        <v>3.65</v>
       </c>
       <c r="S140" t="inlineStr">
         <is>
@@ -13324,16 +13324,16 @@
         </is>
       </c>
       <c r="T140" t="n">
-        <v>4.18</v>
+        <v>3.19</v>
       </c>
       <c r="U140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:56</t>
         </is>
       </c>
       <c r="V140" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-godoy-cruz/dduZfQMj/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-tigre/dYdn4Ua4/</t>
         </is>
       </c>
     </row>
@@ -13361,71 +13361,1083 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
+          <t>Newells Old Boys</t>
+        </is>
+      </c>
+      <c r="G141" t="n">
+        <v>0</v>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="I141" t="n">
+        <v>2</v>
+      </c>
+      <c r="J141" t="n">
+        <v>2</v>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>20/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L141" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:34</t>
+        </is>
+      </c>
+      <c r="N141" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>20/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P141" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="Q141" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:34</t>
+        </is>
+      </c>
+      <c r="R141" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="S141" t="inlineStr">
+        <is>
+          <t>20/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T141" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="U141" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:34</t>
+        </is>
+      </c>
+      <c r="V141" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-godoy-cruz/dduZfQMj/</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E142" s="2" t="n">
+        <v>45228</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Boca Juniors</t>
+        </is>
+      </c>
+      <c r="G142" t="n">
+        <v>0</v>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Estudiantes L.P.</t>
+        </is>
+      </c>
+      <c r="I142" t="n">
+        <v>0</v>
+      </c>
+      <c r="J142" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>25/10/2023 00:23</t>
+        </is>
+      </c>
+      <c r="L142" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>28/10/2023 23:59</t>
+        </is>
+      </c>
+      <c r="N142" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>25/10/2023 00:23</t>
+        </is>
+      </c>
+      <c r="P142" t="n">
+        <v>2.94</v>
+      </c>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>28/10/2023 23:57</t>
+        </is>
+      </c>
+      <c r="R142" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="S142" t="inlineStr">
+        <is>
+          <t>25/10/2023 00:23</t>
+        </is>
+      </c>
+      <c r="T142" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="U142" t="inlineStr">
+        <is>
+          <t>28/10/2023 23:57</t>
+        </is>
+      </c>
+      <c r="V142" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/boca-juniors-estudiantes-l-p/UFOjWnqc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E143" s="2" t="n">
+        <v>45228.10416666666</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Instituto</t>
+        </is>
+      </c>
+      <c r="G143" t="n">
+        <v>0</v>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Velez Sarsfield</t>
+        </is>
+      </c>
+      <c r="I143" t="n">
+        <v>1</v>
+      </c>
+      <c r="J143" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:43</t>
+        </is>
+      </c>
+      <c r="L143" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>29/10/2023 02:26</t>
+        </is>
+      </c>
+      <c r="N143" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:43</t>
+        </is>
+      </c>
+      <c r="P143" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="Q143" t="inlineStr">
+        <is>
+          <t>29/10/2023 02:26</t>
+        </is>
+      </c>
+      <c r="R143" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="S143" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:43</t>
+        </is>
+      </c>
+      <c r="T143" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="U143" t="inlineStr">
+        <is>
+          <t>29/10/2023 02:26</t>
+        </is>
+      </c>
+      <c r="V143" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-velez-sarsfield/ra09J9ai/</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E144" s="2" t="n">
+        <v>45228.75</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Colon Santa Fe</t>
+        </is>
+      </c>
+      <c r="G144" t="n">
+        <v>1</v>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Atl. Tucuman</t>
+        </is>
+      </c>
+      <c r="I144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J144" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="L144" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>29/10/2023 17:51</t>
+        </is>
+      </c>
+      <c r="N144" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P144" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>29/10/2023 17:57</t>
+        </is>
+      </c>
+      <c r="R144" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="S144" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T144" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="U144" t="inlineStr">
+        <is>
+          <t>29/10/2023 17:57</t>
+        </is>
+      </c>
+      <c r="V144" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-atl-tucuman/jVjUEoEM/</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E145" s="2" t="n">
+        <v>45228.85416666666</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Rosario Central</t>
+        </is>
+      </c>
+      <c r="G145" t="n">
+        <v>3</v>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Argentinos Jrs</t>
+        </is>
+      </c>
+      <c r="I145" t="n">
+        <v>1</v>
+      </c>
+      <c r="J145" t="n">
+        <v>3.02</v>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:43</t>
+        </is>
+      </c>
+      <c r="L145" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t>29/10/2023 20:27</t>
+        </is>
+      </c>
+      <c r="N145" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="O145" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:43</t>
+        </is>
+      </c>
+      <c r="P145" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="Q145" t="inlineStr">
+        <is>
+          <t>29/10/2023 20:27</t>
+        </is>
+      </c>
+      <c r="R145" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="S145" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:43</t>
+        </is>
+      </c>
+      <c r="T145" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="U145" t="inlineStr">
+        <is>
+          <t>29/10/2023 20:27</t>
+        </is>
+      </c>
+      <c r="V145" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-argentinos-jrs/MkaDITEc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E146" s="2" t="n">
+        <v>45228.89583333334</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Gimnasia L.P.</t>
+        </is>
+      </c>
+      <c r="G146" t="n">
+        <v>1</v>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>River Plate</t>
+        </is>
+      </c>
+      <c r="I146" t="n">
+        <v>2</v>
+      </c>
+      <c r="J146" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>26/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L146" t="n">
+        <v>5.41</v>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>29/10/2023 21:28</t>
+        </is>
+      </c>
+      <c r="N146" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>26/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P146" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="Q146" t="inlineStr">
+        <is>
+          <t>29/10/2023 21:21</t>
+        </is>
+      </c>
+      <c r="R146" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="S146" t="inlineStr">
+        <is>
+          <t>26/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T146" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="U146" t="inlineStr">
+        <is>
+          <t>29/10/2023 21:21</t>
+        </is>
+      </c>
+      <c r="V146" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/gimnasia-l-p-river-plate/UF2LG7qA/</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E147" s="2" t="n">
+        <v>45229.04166666666</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Independiente</t>
+        </is>
+      </c>
+      <c r="G147" t="n">
+        <v>0</v>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Arsenal Sarandi</t>
+        </is>
+      </c>
+      <c r="I147" t="n">
+        <v>0</v>
+      </c>
+      <c r="J147" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>26/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L147" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>30/10/2023 00:53</t>
+        </is>
+      </c>
+      <c r="N147" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>26/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P147" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>30/10/2023 00:53</t>
+        </is>
+      </c>
+      <c r="R147" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>26/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T147" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="U147" t="inlineStr">
+        <is>
+          <t>30/10/2023 00:59</t>
+        </is>
+      </c>
+      <c r="V147" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/independiente-arsenal-sarandi/CvhQFRbG/</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E148" s="2" t="n">
+        <v>45229.83333333334</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Talleres Cordoba</t>
+        </is>
+      </c>
+      <c r="G148" t="n">
+        <v>0</v>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Banfield</t>
+        </is>
+      </c>
+      <c r="I148" t="n">
+        <v>0</v>
+      </c>
+      <c r="J148" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="L148" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>30/10/2023 19:58</t>
+        </is>
+      </c>
+      <c r="N148" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="O148" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P148" t="n">
+        <v>3.26</v>
+      </c>
+      <c r="Q148" t="inlineStr">
+        <is>
+          <t>30/10/2023 19:58</t>
+        </is>
+      </c>
+      <c r="R148" t="n">
+        <v>4.44</v>
+      </c>
+      <c r="S148" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T148" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="U148" t="inlineStr">
+        <is>
+          <t>30/10/2023 19:58</t>
+        </is>
+      </c>
+      <c r="V148" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-banfield/K4eYD5TS/</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E149" s="2" t="n">
+        <v>45229.9375</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
           <t>Lanus</t>
         </is>
       </c>
-      <c r="G141" t="n">
+      <c r="G149" t="n">
         <v>2</v>
       </c>
-      <c r="H141" t="inlineStr">
-        <is>
-          <t>Tigre</t>
-        </is>
-      </c>
-      <c r="I141" t="n">
-        <v>1</v>
-      </c>
-      <c r="J141" t="n">
-        <v>2.24</v>
-      </c>
-      <c r="K141" t="inlineStr">
-        <is>
-          <t>20/10/2023 21:12</t>
-        </is>
-      </c>
-      <c r="L141" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="M141" t="inlineStr">
-        <is>
-          <t>27/10/2023 01:59</t>
-        </is>
-      </c>
-      <c r="N141" t="n">
-        <v>3.08</v>
-      </c>
-      <c r="O141" t="inlineStr">
-        <is>
-          <t>20/10/2023 21:12</t>
-        </is>
-      </c>
-      <c r="P141" t="n">
-        <v>2.96</v>
-      </c>
-      <c r="Q141" t="inlineStr">
-        <is>
-          <t>27/10/2023 01:28</t>
-        </is>
-      </c>
-      <c r="R141" t="n">
-        <v>3.65</v>
-      </c>
-      <c r="S141" t="inlineStr">
-        <is>
-          <t>20/10/2023 21:12</t>
-        </is>
-      </c>
-      <c r="T141" t="n">
-        <v>3.19</v>
-      </c>
-      <c r="U141" t="inlineStr">
-        <is>
-          <t>27/10/2023 01:56</t>
-        </is>
-      </c>
-      <c r="V141" t="inlineStr">
-        <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-tigre/dYdn4Ua4/</t>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Belgrano</t>
+        </is>
+      </c>
+      <c r="I149" t="n">
+        <v>0</v>
+      </c>
+      <c r="J149" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>27/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L149" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>30/10/2023 22:25</t>
+        </is>
+      </c>
+      <c r="N149" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O149" t="inlineStr">
+        <is>
+          <t>27/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P149" t="n">
+        <v>2.94</v>
+      </c>
+      <c r="Q149" t="inlineStr">
+        <is>
+          <t>30/10/2023 22:05</t>
+        </is>
+      </c>
+      <c r="R149" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="S149" t="inlineStr">
+        <is>
+          <t>27/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T149" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="U149" t="inlineStr">
+        <is>
+          <t>30/10/2023 22:25</t>
+        </is>
+      </c>
+      <c r="V149" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-ca-belgrano-de-cordoba/4YG3TpTF/</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E150" s="2" t="n">
+        <v>45229.95833333334</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Sarmiento Junin</t>
+        </is>
+      </c>
+      <c r="G150" t="n">
+        <v>0</v>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="I150" t="n">
+        <v>0</v>
+      </c>
+      <c r="J150" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>26/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="L150" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>30/10/2023 22:50</t>
+        </is>
+      </c>
+      <c r="N150" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="O150" t="inlineStr">
+        <is>
+          <t>26/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P150" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>30/10/2023 22:50</t>
+        </is>
+      </c>
+      <c r="R150" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="S150" t="inlineStr">
+        <is>
+          <t>26/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T150" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="U150" t="inlineStr">
+        <is>
+          <t>30/10/2023 22:58</t>
+        </is>
+      </c>
+      <c r="V150" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-san-lorenzo/GCz9736d/</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E151" s="2" t="n">
+        <v>45230.04166666666</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="G151" t="n">
+        <v>0</v>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>Barracas Central</t>
+        </is>
+      </c>
+      <c r="I151" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:44</t>
+        </is>
+      </c>
+      <c r="L151" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:59</t>
+        </is>
+      </c>
+      <c r="N151" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="O151" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:44</t>
+        </is>
+      </c>
+      <c r="P151" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="Q151" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:59</t>
+        </is>
+      </c>
+      <c r="R151" t="n">
+        <v>4.62</v>
+      </c>
+      <c r="S151" t="inlineStr">
+        <is>
+          <t>25/10/2023 02:44</t>
+        </is>
+      </c>
+      <c r="T151" t="n">
+        <v>5.58</v>
+      </c>
+      <c r="U151" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:59</t>
+        </is>
+      </c>
+      <c r="V151" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-barracas-central/GCbHHmU3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E152" s="2" t="n">
+        <v>45230.05208333334</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Platense</t>
+        </is>
+      </c>
+      <c r="G152" t="n">
+        <v>0</v>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>Newells Old Boys</t>
+        </is>
+      </c>
+      <c r="I152" t="n">
+        <v>0</v>
+      </c>
+      <c r="J152" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>27/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L152" t="n">
+        <v>2.91</v>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:19</t>
+        </is>
+      </c>
+      <c r="N152" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="O152" t="inlineStr">
+        <is>
+          <t>27/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P152" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="Q152" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:19</t>
+        </is>
+      </c>
+      <c r="R152" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="S152" t="inlineStr">
+        <is>
+          <t>27/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T152" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="U152" t="inlineStr">
+        <is>
+          <t>31/10/2023 00:19</t>
+        </is>
+      </c>
+      <c r="V152" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-newells-old-boys/4xX48qij/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 01-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V152"/>
+  <dimension ref="A1:V154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3333,22 +3333,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="I32" t="n">
         <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>1.98</v>
+        <v>2.74</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -3356,15 +3356,15 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>2.12</v>
+        <v>2.85</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>3.19</v>
+        <v>2.8</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3372,15 +3372,15 @@
         </is>
       </c>
       <c r="P32" t="n">
-        <v>2.93</v>
+        <v>2.67</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>4.44</v>
+        <v>3.12</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
@@ -3388,16 +3388,16 @@
         </is>
       </c>
       <c r="T32" t="n">
-        <v>4.54</v>
+        <v>3.25</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-colon-santa-fe/xr5c0r56/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-newells-old-boys/plSOG3km/</t>
         </is>
       </c>
     </row>
@@ -3425,22 +3425,22 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I33" t="n">
         <v>1</v>
       </c>
       <c r="J33" t="n">
-        <v>2.74</v>
+        <v>1.98</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -3448,15 +3448,15 @@
         </is>
       </c>
       <c r="L33" t="n">
-        <v>2.85</v>
+        <v>2.12</v>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="N33" t="n">
-        <v>2.8</v>
+        <v>3.19</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -3464,15 +3464,15 @@
         </is>
       </c>
       <c r="P33" t="n">
-        <v>2.67</v>
+        <v>2.93</v>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="R33" t="n">
-        <v>3.12</v>
+        <v>4.44</v>
       </c>
       <c r="S33" t="inlineStr">
         <is>
@@ -3480,16 +3480,16 @@
         </is>
       </c>
       <c r="T33" t="n">
-        <v>3.25</v>
+        <v>4.54</v>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-newells-old-boys/plSOG3km/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-colon-santa-fe/xr5c0r56/</t>
         </is>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -3801,63 +3801,63 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>1.76</v>
+        <v>2.67</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>29/08/2023 00:12</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>1.75</v>
+        <v>3.38</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
+          <t>03/09/2023 21:07</t>
+        </is>
+      </c>
+      <c r="N37" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P37" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="N37" t="n">
-        <v>3.56</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="P37" t="n">
-        <v>3.46</v>
-      </c>
-      <c r="Q37" t="inlineStr">
+      <c r="R37" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T37" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="U37" t="inlineStr">
         <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="R37" t="n">
-        <v>5.34</v>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="T37" t="n">
-        <v>5.63</v>
-      </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>03/09/2023 21:13</t>
-        </is>
-      </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
         </is>
       </c>
     </row>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -3893,38 +3893,38 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J38" t="n">
-        <v>2.67</v>
+        <v>1.76</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="L38" t="n">
-        <v>3.38</v>
+        <v>1.75</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>03/09/2023 21:07</t>
+          <t>03/09/2023 21:13</t>
         </is>
       </c>
       <c r="N38" t="n">
-        <v>3.13</v>
+        <v>3.56</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="P38" t="n">
-        <v>3.18</v>
+        <v>3.46</v>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
@@ -3932,15 +3932,15 @@
         </is>
       </c>
       <c r="R38" t="n">
-        <v>2.73</v>
+        <v>5.34</v>
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="T38" t="n">
-        <v>2.36</v>
+        <v>5.63</v>
       </c>
       <c r="U38" t="inlineStr">
         <is>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
         </is>
       </c>
     </row>
@@ -11889,7 +11889,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G125" t="n">
@@ -11897,14 +11897,14 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I125" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J125" t="n">
-        <v>2.03</v>
+        <v>1.43</v>
       </c>
       <c r="K125" t="inlineStr">
         <is>
@@ -11912,15 +11912,15 @@
         </is>
       </c>
       <c r="L125" t="n">
-        <v>2.04</v>
+        <v>1.48</v>
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:58</t>
+          <t>20/10/2023 23:52</t>
         </is>
       </c>
       <c r="N125" t="n">
-        <v>3.07</v>
+        <v>4.42</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -11928,15 +11928,15 @@
         </is>
       </c>
       <c r="P125" t="n">
-        <v>2.89</v>
+        <v>4.33</v>
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:56</t>
+          <t>20/10/2023 23:59</t>
         </is>
       </c>
       <c r="R125" t="n">
-        <v>4.41</v>
+        <v>6.91</v>
       </c>
       <c r="S125" t="inlineStr">
         <is>
@@ -11944,16 +11944,16 @@
         </is>
       </c>
       <c r="T125" t="n">
-        <v>5.06</v>
+        <v>7.59</v>
       </c>
       <c r="U125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:58</t>
+          <t>20/10/2023 23:52</t>
         </is>
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-instituto/KOmLi0As/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-arsenal-sarandi/l4uxlI96/</t>
         </is>
       </c>
     </row>
@@ -11981,7 +11981,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G126" t="n">
@@ -11989,14 +11989,14 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I126" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J126" t="n">
-        <v>1.43</v>
+        <v>2.03</v>
       </c>
       <c r="K126" t="inlineStr">
         <is>
@@ -12004,15 +12004,15 @@
         </is>
       </c>
       <c r="L126" t="n">
-        <v>1.48</v>
+        <v>2.04</v>
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:52</t>
+          <t>20/10/2023 23:58</t>
         </is>
       </c>
       <c r="N126" t="n">
-        <v>4.42</v>
+        <v>3.07</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -12020,15 +12020,15 @@
         </is>
       </c>
       <c r="P126" t="n">
-        <v>4.33</v>
+        <v>2.89</v>
       </c>
       <c r="Q126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:59</t>
+          <t>20/10/2023 23:56</t>
         </is>
       </c>
       <c r="R126" t="n">
-        <v>6.91</v>
+        <v>4.41</v>
       </c>
       <c r="S126" t="inlineStr">
         <is>
@@ -12036,16 +12036,16 @@
         </is>
       </c>
       <c r="T126" t="n">
-        <v>7.59</v>
+        <v>5.06</v>
       </c>
       <c r="U126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:52</t>
+          <t>20/10/2023 23:58</t>
         </is>
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-arsenal-sarandi/l4uxlI96/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-instituto/KOmLi0As/</t>
         </is>
       </c>
     </row>
@@ -12625,22 +12625,22 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="I133" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J133" t="n">
-        <v>2.08</v>
+        <v>1.88</v>
       </c>
       <c r="K133" t="inlineStr">
         <is>
@@ -12648,15 +12648,15 @@
         </is>
       </c>
       <c r="L133" t="n">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="N133" t="n">
-        <v>3.15</v>
+        <v>3.23</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -12664,15 +12664,15 @@
         </is>
       </c>
       <c r="P133" t="n">
-        <v>3.15</v>
+        <v>3.11</v>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:26</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="R133" t="n">
-        <v>4.07</v>
+        <v>4.51</v>
       </c>
       <c r="S133" t="inlineStr">
         <is>
@@ -12680,16 +12680,16 @@
         </is>
       </c>
       <c r="T133" t="n">
-        <v>4.84</v>
+        <v>5.33</v>
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:27</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
         </is>
       </c>
     </row>
@@ -12717,22 +12717,22 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="I134" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J134" t="n">
-        <v>1.88</v>
+        <v>2.08</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>3.23</v>
+        <v>3.15</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>3.11</v>
+        <v>3.15</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:26</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>4.51</v>
+        <v>4.07</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>5.33</v>
+        <v>4.84</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:27</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
         </is>
       </c>
     </row>
@@ -14438,6 +14438,190 @@
       <c r="V152" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-newells-old-boys/4xX48qij/</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E153" s="2" t="n">
+        <v>45230.95833333334</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Tigre</t>
+        </is>
+      </c>
+      <c r="G153" t="n">
+        <v>1</v>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="I153" t="n">
+        <v>0</v>
+      </c>
+      <c r="J153" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>27/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L153" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>31/10/2023 22:59</t>
+        </is>
+      </c>
+      <c r="N153" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
+          <t>27/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P153" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>31/10/2023 22:59</t>
+        </is>
+      </c>
+      <c r="R153" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="S153" t="inlineStr">
+        <is>
+          <t>27/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T153" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="U153" t="inlineStr">
+        <is>
+          <t>31/10/2023 22:57</t>
+        </is>
+      </c>
+      <c r="V153" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/tigre-godoy-cruz/MDs09Pyp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E154" s="2" t="n">
+        <v>45231.04166666666</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Central Cordoba</t>
+        </is>
+      </c>
+      <c r="G154" t="n">
+        <v>2</v>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>Union de Santa Fe</t>
+        </is>
+      </c>
+      <c r="I154" t="n">
+        <v>0</v>
+      </c>
+      <c r="J154" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="L154" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>01/11/2023 00:57</t>
+        </is>
+      </c>
+      <c r="N154" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="O154" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P154" t="n">
+        <v>2.72</v>
+      </c>
+      <c r="Q154" t="inlineStr">
+        <is>
+          <t>01/11/2023 00:57</t>
+        </is>
+      </c>
+      <c r="R154" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="S154" t="inlineStr">
+        <is>
+          <t>25/10/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T154" t="n">
+        <v>3.02</v>
+      </c>
+      <c r="U154" t="inlineStr">
+        <is>
+          <t>01/11/2023 00:57</t>
+        </is>
+      </c>
+      <c r="V154" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-union-de-santa-fe/QsIaUQD9/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 02-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V154"/>
+  <dimension ref="A1:V155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -9413,14 +9413,14 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>1.93</v>
+        <v>3.31</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
         </is>
       </c>
       <c r="L98" t="n">
-        <v>1.91</v>
+        <v>3.28</v>
       </c>
       <c r="M98" t="inlineStr">
         <is>
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="N98" t="n">
-        <v>3.29</v>
+        <v>2.97</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -9444,7 +9444,7 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>3.2</v>
+        <v>2.93</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
@@ -9452,7 +9452,7 @@
         </is>
       </c>
       <c r="R98" t="n">
-        <v>4.52</v>
+        <v>2.47</v>
       </c>
       <c r="S98" t="inlineStr">
         <is>
@@ -9460,7 +9460,7 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>5.03</v>
+        <v>2.59</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
@@ -9469,7 +9469,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
         </is>
       </c>
     </row>
@@ -9497,7 +9497,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G99" t="n">
@@ -9505,14 +9505,14 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I99" t="n">
         <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>3.31</v>
+        <v>1.93</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -9520,7 +9520,7 @@
         </is>
       </c>
       <c r="L99" t="n">
-        <v>3.28</v>
+        <v>1.91</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
@@ -9528,7 +9528,7 @@
         </is>
       </c>
       <c r="N99" t="n">
-        <v>2.97</v>
+        <v>3.29</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -9536,7 +9536,7 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>2.93</v>
+        <v>3.2</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
@@ -9544,7 +9544,7 @@
         </is>
       </c>
       <c r="R99" t="n">
-        <v>2.47</v>
+        <v>4.52</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
@@ -9552,7 +9552,7 @@
         </is>
       </c>
       <c r="T99" t="n">
-        <v>2.59</v>
+        <v>5.03</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
@@ -9561,7 +9561,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
         </is>
       </c>
     </row>
@@ -10141,7 +10141,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="G106" t="n">
@@ -10149,14 +10149,14 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Gimnasia L.P.</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J106" t="n">
-        <v>1.93</v>
+        <v>1.96</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
@@ -10164,15 +10164,15 @@
         </is>
       </c>
       <c r="L106" t="n">
-        <v>2.08</v>
+        <v>1.88</v>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:05</t>
         </is>
       </c>
       <c r="N106" t="n">
-        <v>3.23</v>
+        <v>3.24</v>
       </c>
       <c r="O106" t="inlineStr">
         <is>
@@ -10180,15 +10180,15 @@
         </is>
       </c>
       <c r="P106" t="n">
-        <v>2.95</v>
+        <v>3.14</v>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:05</t>
         </is>
       </c>
       <c r="R106" t="n">
-        <v>4.21</v>
+        <v>4.4</v>
       </c>
       <c r="S106" t="inlineStr">
         <is>
@@ -10196,16 +10196,16 @@
         </is>
       </c>
       <c r="T106" t="n">
-        <v>4.67</v>
+        <v>5.34</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:06</t>
         </is>
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-gimnasia-l-p/xj5NrNXQ/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-sarmiento-junin/Aa1azau7/</t>
         </is>
       </c>
     </row>
@@ -10233,7 +10233,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -10241,14 +10241,14 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Gimnasia L.P.</t>
         </is>
       </c>
       <c r="I107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J107" t="n">
-        <v>1.96</v>
+        <v>1.93</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -10256,15 +10256,15 @@
         </is>
       </c>
       <c r="L107" t="n">
-        <v>1.88</v>
+        <v>2.08</v>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:05</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>3.24</v>
+        <v>3.23</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -10272,15 +10272,15 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>3.14</v>
+        <v>2.95</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:05</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="R107" t="n">
-        <v>4.4</v>
+        <v>4.21</v>
       </c>
       <c r="S107" t="inlineStr">
         <is>
@@ -10288,16 +10288,16 @@
         </is>
       </c>
       <c r="T107" t="n">
-        <v>5.34</v>
+        <v>4.67</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:06</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-sarmiento-junin/Aa1azau7/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-gimnasia-l-p/xj5NrNXQ/</t>
         </is>
       </c>
     </row>
@@ -11889,7 +11889,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G125" t="n">
@@ -11897,14 +11897,14 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I125" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J125" t="n">
-        <v>1.43</v>
+        <v>2.03</v>
       </c>
       <c r="K125" t="inlineStr">
         <is>
@@ -11912,15 +11912,15 @@
         </is>
       </c>
       <c r="L125" t="n">
-        <v>1.48</v>
+        <v>2.04</v>
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:52</t>
+          <t>20/10/2023 23:58</t>
         </is>
       </c>
       <c r="N125" t="n">
-        <v>4.42</v>
+        <v>3.07</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -11928,15 +11928,15 @@
         </is>
       </c>
       <c r="P125" t="n">
-        <v>4.33</v>
+        <v>2.89</v>
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:59</t>
+          <t>20/10/2023 23:56</t>
         </is>
       </c>
       <c r="R125" t="n">
-        <v>6.91</v>
+        <v>4.41</v>
       </c>
       <c r="S125" t="inlineStr">
         <is>
@@ -11944,16 +11944,16 @@
         </is>
       </c>
       <c r="T125" t="n">
-        <v>7.59</v>
+        <v>5.06</v>
       </c>
       <c r="U125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:52</t>
+          <t>20/10/2023 23:58</t>
         </is>
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-arsenal-sarandi/l4uxlI96/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-instituto/KOmLi0As/</t>
         </is>
       </c>
     </row>
@@ -11981,7 +11981,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G126" t="n">
@@ -11989,14 +11989,14 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I126" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J126" t="n">
-        <v>2.03</v>
+        <v>1.43</v>
       </c>
       <c r="K126" t="inlineStr">
         <is>
@@ -12004,15 +12004,15 @@
         </is>
       </c>
       <c r="L126" t="n">
-        <v>2.04</v>
+        <v>1.48</v>
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:58</t>
+          <t>20/10/2023 23:52</t>
         </is>
       </c>
       <c r="N126" t="n">
-        <v>3.07</v>
+        <v>4.42</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -12020,15 +12020,15 @@
         </is>
       </c>
       <c r="P126" t="n">
-        <v>2.89</v>
+        <v>4.33</v>
       </c>
       <c r="Q126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:56</t>
+          <t>20/10/2023 23:59</t>
         </is>
       </c>
       <c r="R126" t="n">
-        <v>4.41</v>
+        <v>6.91</v>
       </c>
       <c r="S126" t="inlineStr">
         <is>
@@ -12036,16 +12036,16 @@
         </is>
       </c>
       <c r="T126" t="n">
-        <v>5.06</v>
+        <v>7.59</v>
       </c>
       <c r="U126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:58</t>
+          <t>20/10/2023 23:52</t>
         </is>
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-instituto/KOmLi0As/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-arsenal-sarandi/l4uxlI96/</t>
         </is>
       </c>
     </row>
@@ -12901,7 +12901,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -12909,63 +12909,63 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J136" t="n">
-        <v>2.74</v>
+        <v>1.94</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="L136" t="n">
-        <v>2.55</v>
+        <v>1.89</v>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="N136" t="n">
-        <v>2.98</v>
+        <v>3.2</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="P136" t="n">
-        <v>3.06</v>
+        <v>3.14</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="R136" t="n">
-        <v>2.78</v>
+        <v>4.62</v>
       </c>
       <c r="S136" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="T136" t="n">
-        <v>3.18</v>
+        <v>5.29</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
         </is>
       </c>
     </row>
@@ -12993,7 +12993,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G137" t="n">
@@ -13001,63 +13001,63 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J137" t="n">
-        <v>1.94</v>
+        <v>2.74</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="L137" t="n">
-        <v>1.89</v>
+        <v>2.55</v>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="N137" t="n">
-        <v>3.2</v>
+        <v>2.98</v>
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="P137" t="n">
-        <v>3.14</v>
+        <v>3.06</v>
       </c>
       <c r="Q137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="R137" t="n">
-        <v>4.62</v>
+        <v>2.78</v>
       </c>
       <c r="S137" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="T137" t="n">
-        <v>5.29</v>
+        <v>3.18</v>
       </c>
       <c r="U137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
         </is>
       </c>
     </row>
@@ -14622,6 +14622,98 @@
       <c r="V154" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-union-de-santa-fe/QsIaUQD9/</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E155" s="2" t="n">
+        <v>45232</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Defensa y Justicia</t>
+        </is>
+      </c>
+      <c r="G155" t="n">
+        <v>2</v>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>Racing Club</t>
+        </is>
+      </c>
+      <c r="I155" t="n">
+        <v>2</v>
+      </c>
+      <c r="J155" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>26/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L155" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>01/11/2023 23:58</t>
+        </is>
+      </c>
+      <c r="N155" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="O155" t="inlineStr">
+        <is>
+          <t>26/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P155" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="Q155" t="inlineStr">
+        <is>
+          <t>01/11/2023 23:51</t>
+        </is>
+      </c>
+      <c r="R155" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="S155" t="inlineStr">
+        <is>
+          <t>26/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T155" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="U155" t="inlineStr">
+        <is>
+          <t>01/11/2023 23:58</t>
+        </is>
+      </c>
+      <c r="V155" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-racing-club/86NfV6b3/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 04-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V155"/>
+  <dimension ref="A1:V157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5909,30 +5909,30 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Independiente</t>
+          <t>Gimnasia L.P.</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>16/09/2023 01:13</t>
+          <t>15/09/2023 01:13</t>
         </is>
       </c>
       <c r="L60" t="n">
-        <v>2.78</v>
+        <v>1.9</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
@@ -5940,15 +5940,15 @@
         </is>
       </c>
       <c r="N60" t="n">
-        <v>3.12</v>
+        <v>3.3</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>16/09/2023 01:13</t>
+          <t>15/09/2023 01:13</t>
         </is>
       </c>
       <c r="P60" t="n">
-        <v>3.02</v>
+        <v>3.1</v>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
@@ -5956,15 +5956,15 @@
         </is>
       </c>
       <c r="R60" t="n">
-        <v>4.04</v>
+        <v>4.82</v>
       </c>
       <c r="S60" t="inlineStr">
         <is>
-          <t>16/09/2023 01:13</t>
+          <t>15/09/2023 01:13</t>
         </is>
       </c>
       <c r="T60" t="n">
-        <v>2.93</v>
+        <v>5.38</v>
       </c>
       <c r="U60" t="inlineStr">
         <is>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-independiente/vq5eHztb/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-gimnasia-l-p/IZ3aGfe4/</t>
         </is>
       </c>
     </row>
@@ -6001,30 +6001,30 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Gimnasia L.P.</t>
+          <t>Independiente</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" t="n">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>15/09/2023 01:13</t>
+          <t>16/09/2023 01:13</t>
         </is>
       </c>
       <c r="L61" t="n">
-        <v>1.9</v>
+        <v>2.78</v>
       </c>
       <c r="M61" t="inlineStr">
         <is>
@@ -6032,15 +6032,15 @@
         </is>
       </c>
       <c r="N61" t="n">
-        <v>3.3</v>
+        <v>3.12</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>15/09/2023 01:13</t>
+          <t>16/09/2023 01:13</t>
         </is>
       </c>
       <c r="P61" t="n">
-        <v>3.1</v>
+        <v>3.02</v>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
@@ -6048,15 +6048,15 @@
         </is>
       </c>
       <c r="R61" t="n">
-        <v>4.82</v>
+        <v>4.04</v>
       </c>
       <c r="S61" t="inlineStr">
         <is>
-          <t>15/09/2023 01:13</t>
+          <t>16/09/2023 01:13</t>
         </is>
       </c>
       <c r="T61" t="n">
-        <v>5.38</v>
+        <v>2.93</v>
       </c>
       <c r="U61" t="inlineStr">
         <is>
@@ -6065,7 +6065,7 @@
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-gimnasia-l-p/IZ3aGfe4/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-independiente/vq5eHztb/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,63 +9781,63 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J102" t="n">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>2.17</v>
+        <v>1.9</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.37</v>
+        <v>3.58</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.06</v>
+        <v>3.47</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>4.33</v>
+        <v>4.7</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>4.04</v>
+        <v>4.55</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -9873,63 +9873,63 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J103" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>1.9</v>
+        <v>2.17</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.58</v>
+        <v>3.37</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.47</v>
+        <v>3.06</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>4.7</v>
+        <v>4.33</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4.55</v>
+        <v>4.04</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
         </is>
       </c>
     </row>
@@ -10141,7 +10141,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G106" t="n">
@@ -10149,14 +10149,14 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Gimnasia L.P.</t>
         </is>
       </c>
       <c r="I106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J106" t="n">
-        <v>1.96</v>
+        <v>1.93</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
@@ -10164,15 +10164,15 @@
         </is>
       </c>
       <c r="L106" t="n">
-        <v>1.88</v>
+        <v>2.08</v>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:05</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="N106" t="n">
-        <v>3.24</v>
+        <v>3.23</v>
       </c>
       <c r="O106" t="inlineStr">
         <is>
@@ -10180,15 +10180,15 @@
         </is>
       </c>
       <c r="P106" t="n">
-        <v>3.14</v>
+        <v>2.95</v>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:05</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="R106" t="n">
-        <v>4.4</v>
+        <v>4.21</v>
       </c>
       <c r="S106" t="inlineStr">
         <is>
@@ -10196,16 +10196,16 @@
         </is>
       </c>
       <c r="T106" t="n">
-        <v>5.34</v>
+        <v>4.67</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:06</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-sarmiento-junin/Aa1azau7/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-gimnasia-l-p/xj5NrNXQ/</t>
         </is>
       </c>
     </row>
@@ -10233,7 +10233,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -10241,14 +10241,14 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Gimnasia L.P.</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J107" t="n">
-        <v>1.93</v>
+        <v>1.96</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -10256,15 +10256,15 @@
         </is>
       </c>
       <c r="L107" t="n">
-        <v>2.08</v>
+        <v>1.88</v>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:05</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>3.23</v>
+        <v>3.24</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -10272,15 +10272,15 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>2.95</v>
+        <v>3.14</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:05</t>
         </is>
       </c>
       <c r="R107" t="n">
-        <v>4.21</v>
+        <v>4.4</v>
       </c>
       <c r="S107" t="inlineStr">
         <is>
@@ -10288,16 +10288,16 @@
         </is>
       </c>
       <c r="T107" t="n">
-        <v>4.67</v>
+        <v>5.34</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:06</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-gimnasia-l-p/xj5NrNXQ/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-sarmiento-junin/Aa1azau7/</t>
         </is>
       </c>
     </row>
@@ -12901,7 +12901,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -12909,63 +12909,63 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J136" t="n">
-        <v>1.94</v>
+        <v>2.74</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="L136" t="n">
-        <v>1.89</v>
+        <v>2.55</v>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="N136" t="n">
-        <v>3.2</v>
+        <v>2.98</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="P136" t="n">
-        <v>3.14</v>
+        <v>3.06</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="R136" t="n">
-        <v>4.62</v>
+        <v>2.78</v>
       </c>
       <c r="S136" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="T136" t="n">
-        <v>5.29</v>
+        <v>3.18</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
         </is>
       </c>
     </row>
@@ -12993,7 +12993,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G137" t="n">
@@ -13001,63 +13001,63 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J137" t="n">
-        <v>2.74</v>
+        <v>1.94</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="L137" t="n">
-        <v>2.55</v>
+        <v>1.89</v>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="N137" t="n">
-        <v>2.98</v>
+        <v>3.2</v>
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="P137" t="n">
-        <v>3.06</v>
+        <v>3.14</v>
       </c>
       <c r="Q137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="R137" t="n">
-        <v>2.78</v>
+        <v>4.62</v>
       </c>
       <c r="S137" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="T137" t="n">
-        <v>3.18</v>
+        <v>5.29</v>
       </c>
       <c r="U137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
         </is>
       </c>
     </row>
@@ -14714,6 +14714,190 @@
       <c r="V155" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-racing-club/86NfV6b3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E156" s="2" t="n">
+        <v>45233.95833333334</v>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Arsenal Sarandi</t>
+        </is>
+      </c>
+      <c r="G156" t="n">
+        <v>0</v>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>Gimnasia L.P.</t>
+        </is>
+      </c>
+      <c r="I156" t="n">
+        <v>0</v>
+      </c>
+      <c r="J156" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>30/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L156" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="M156" t="inlineStr">
+        <is>
+          <t>03/11/2023 22:58</t>
+        </is>
+      </c>
+      <c r="N156" t="n">
+        <v>2.97</v>
+      </c>
+      <c r="O156" t="inlineStr">
+        <is>
+          <t>30/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P156" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="Q156" t="inlineStr">
+        <is>
+          <t>03/11/2023 22:54</t>
+        </is>
+      </c>
+      <c r="R156" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="S156" t="inlineStr">
+        <is>
+          <t>30/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T156" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="U156" t="inlineStr">
+        <is>
+          <t>03/11/2023 22:58</t>
+        </is>
+      </c>
+      <c r="V156" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-gimnasia-l-p/dWerM2Lk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E157" s="2" t="n">
+        <v>45234.04166666666</v>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>River Plate</t>
+        </is>
+      </c>
+      <c r="G157" t="n">
+        <v>1</v>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="I157" t="n">
+        <v>2</v>
+      </c>
+      <c r="J157" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:13</t>
+        </is>
+      </c>
+      <c r="L157" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="M157" t="inlineStr">
+        <is>
+          <t>04/11/2023 00:42</t>
+        </is>
+      </c>
+      <c r="N157" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="O157" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:13</t>
+        </is>
+      </c>
+      <c r="P157" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="Q157" t="inlineStr">
+        <is>
+          <t>04/11/2023 00:50</t>
+        </is>
+      </c>
+      <c r="R157" t="n">
+        <v>7.08</v>
+      </c>
+      <c r="S157" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:13</t>
+        </is>
+      </c>
+      <c r="T157" t="n">
+        <v>7.83</v>
+      </c>
+      <c r="U157" t="inlineStr">
+        <is>
+          <t>04/11/2023 00:50</t>
+        </is>
+      </c>
+      <c r="V157" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/river-plate-huracan/4denLMzd/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 05-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V157"/>
+  <dimension ref="A1:V159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2137,71 +2137,71 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G19" t="n">
+        <v>2</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
         <v>1</v>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Lanus</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
       <c r="J19" t="n">
-        <v>2.19</v>
+        <v>1.74</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>2.09</v>
+        <v>1.94</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:43</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="N19" t="n">
-        <v>2.94</v>
+        <v>3.44</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="P19" t="n">
-        <v>3.01</v>
+        <v>3.23</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:43</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="R19" t="n">
-        <v>3.79</v>
+        <v>5.57</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="T19" t="n">
-        <v>4.48</v>
+        <v>4.73</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:42</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-lanus/OdYgrAqL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-huracan/l4ycuMBq/</t>
         </is>
       </c>
     </row>
@@ -2229,71 +2229,71 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>1.74</v>
+        <v>2.19</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>1.94</v>
+        <v>2.09</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:43</t>
         </is>
       </c>
       <c r="N20" t="n">
-        <v>3.44</v>
+        <v>2.94</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="P20" t="n">
-        <v>3.23</v>
+        <v>3.01</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:43</t>
         </is>
       </c>
       <c r="R20" t="n">
-        <v>5.57</v>
+        <v>3.79</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="T20" t="n">
-        <v>4.73</v>
+        <v>4.48</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:42</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-huracan/l4ycuMBq/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-lanus/OdYgrAqL/</t>
         </is>
       </c>
     </row>
@@ -2413,71 +2413,71 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>1.87</v>
+        <v>2.61</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>1.85</v>
+        <v>2.08</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:27</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.32</v>
+        <v>3.05</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.44</v>
+        <v>3.11</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:22</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>4.39</v>
+        <v>2.86</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="T22" t="n">
-        <v>4.87</v>
+        <v>4.32</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:27</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-central-cordoba-santiago-del-estero/6LNbsUbR/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-defensa-y-justicia/8U9Qxl7r/</t>
         </is>
       </c>
     </row>
@@ -2505,71 +2505,71 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>2.61</v>
+        <v>1.87</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>2.08</v>
+        <v>1.85</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:27</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>3.05</v>
+        <v>3.32</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.11</v>
+        <v>3.44</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:22</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>2.86</v>
+        <v>4.39</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="T23" t="n">
-        <v>4.32</v>
+        <v>4.87</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:27</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-defensa-y-justicia/8U9Qxl7r/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-central-cordoba-santiago-del-estero/6LNbsUbR/</t>
         </is>
       </c>
     </row>
@@ -3609,71 +3609,71 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I35" t="n">
         <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>2.38</v>
+        <v>1.97</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>2.45</v>
+        <v>2.41</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="N35" t="n">
-        <v>2.92</v>
+        <v>3.39</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="P35" t="n">
-        <v>2.74</v>
+        <v>3.13</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="R35" t="n">
-        <v>3.56</v>
+        <v>4.13</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="T35" t="n">
-        <v>3.85</v>
+        <v>3.35</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-banfield/Wp2k24zf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-sarmiento-junin/nDnlN5CJ/</t>
         </is>
       </c>
     </row>
@@ -3701,71 +3701,71 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>1.97</v>
+        <v>2.38</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>2.41</v>
+        <v>2.45</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="N36" t="n">
-        <v>3.39</v>
+        <v>2.92</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="P36" t="n">
-        <v>3.13</v>
+        <v>2.74</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="R36" t="n">
-        <v>4.13</v>
+        <v>3.56</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="T36" t="n">
-        <v>3.35</v>
+        <v>3.85</v>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-sarmiento-junin/nDnlN5CJ/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-banfield/Wp2k24zf/</t>
         </is>
       </c>
     </row>
@@ -4989,22 +4989,22 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I50" t="n">
         <v>1</v>
       </c>
       <c r="J50" t="n">
-        <v>2.49</v>
+        <v>2.74</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -5012,15 +5012,15 @@
         </is>
       </c>
       <c r="L50" t="n">
-        <v>2.44</v>
+        <v>3.68</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>16/09/2023 01:50</t>
+          <t>16/09/2023 01:58</t>
         </is>
       </c>
       <c r="N50" t="n">
-        <v>3.13</v>
+        <v>2.93</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -5028,15 +5028,15 @@
         </is>
       </c>
       <c r="P50" t="n">
-        <v>3.2</v>
+        <v>2.98</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>16/09/2023 01:59</t>
+          <t>16/09/2023 01:58</t>
         </is>
       </c>
       <c r="R50" t="n">
-        <v>3.1</v>
+        <v>2.82</v>
       </c>
       <c r="S50" t="inlineStr">
         <is>
@@ -5044,16 +5044,16 @@
         </is>
       </c>
       <c r="T50" t="n">
-        <v>3.23</v>
+        <v>2.35</v>
       </c>
       <c r="U50" t="inlineStr">
         <is>
-          <t>16/09/2023 01:59</t>
+          <t>16/09/2023 01:58</t>
         </is>
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-rosario-central/A79Ockq8/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-argentinos-jrs/6Z2XeTDK/</t>
         </is>
       </c>
     </row>
@@ -5081,22 +5081,22 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="I51" t="n">
         <v>1</v>
       </c>
       <c r="J51" t="n">
-        <v>2.74</v>
+        <v>2.49</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -5104,15 +5104,15 @@
         </is>
       </c>
       <c r="L51" t="n">
-        <v>3.68</v>
+        <v>2.44</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>16/09/2023 01:58</t>
+          <t>16/09/2023 01:50</t>
         </is>
       </c>
       <c r="N51" t="n">
-        <v>2.93</v>
+        <v>3.13</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -5120,15 +5120,15 @@
         </is>
       </c>
       <c r="P51" t="n">
-        <v>2.98</v>
+        <v>3.2</v>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>16/09/2023 01:58</t>
+          <t>16/09/2023 01:59</t>
         </is>
       </c>
       <c r="R51" t="n">
-        <v>2.82</v>
+        <v>3.1</v>
       </c>
       <c r="S51" t="inlineStr">
         <is>
@@ -5136,16 +5136,16 @@
         </is>
       </c>
       <c r="T51" t="n">
-        <v>2.35</v>
+        <v>3.23</v>
       </c>
       <c r="U51" t="inlineStr">
         <is>
-          <t>16/09/2023 01:58</t>
+          <t>16/09/2023 01:59</t>
         </is>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-argentinos-jrs/6Z2XeTDK/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-rosario-central/A79Ockq8/</t>
         </is>
       </c>
     </row>
@@ -6277,71 +6277,71 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Velez Sarsfield</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>San Lorenzo</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J64" t="n">
-        <v>2.04</v>
+        <v>1.69</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="L64" t="n">
-        <v>2.29</v>
+        <v>1.74</v>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:23</t>
         </is>
       </c>
       <c r="N64" t="n">
-        <v>3.04</v>
+        <v>3.41</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="P64" t="n">
-        <v>2.85</v>
+        <v>3.4</v>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:23</t>
         </is>
       </c>
       <c r="R64" t="n">
-        <v>4.47</v>
+        <v>5.46</v>
       </c>
       <c r="S64" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="T64" t="n">
-        <v>4.05</v>
+        <v>6</v>
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:27</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-san-lorenzo/IZPUVZfi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-arsenal-sarandi/OEeXCLlC/</t>
         </is>
       </c>
     </row>
@@ -6369,71 +6369,71 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Velez Sarsfield</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>San Lorenzo</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J65" t="n">
-        <v>1.69</v>
+        <v>2.04</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="L65" t="n">
-        <v>1.74</v>
+        <v>2.29</v>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:23</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="N65" t="n">
-        <v>3.41</v>
+        <v>3.04</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="P65" t="n">
-        <v>3.4</v>
+        <v>2.85</v>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:23</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="R65" t="n">
-        <v>5.46</v>
+        <v>4.47</v>
       </c>
       <c r="S65" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="T65" t="n">
-        <v>6</v>
+        <v>4.05</v>
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:27</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-arsenal-sarandi/OEeXCLlC/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-san-lorenzo/IZPUVZfi/</t>
         </is>
       </c>
     </row>
@@ -6461,71 +6461,71 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Racing Club</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="I66" t="n">
         <v>1</v>
       </c>
       <c r="J66" t="n">
-        <v>2.04</v>
+        <v>2.62</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="L66" t="n">
-        <v>2.18</v>
+        <v>2.35</v>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="N66" t="n">
-        <v>3.19</v>
+        <v>2.94</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="P66" t="n">
-        <v>3</v>
+        <v>3.13</v>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="R66" t="n">
-        <v>4.18</v>
+        <v>3.12</v>
       </c>
       <c r="S66" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="T66" t="n">
-        <v>4.13</v>
+        <v>3.47</v>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-colon-santa-fe/A90iIGQi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-newells-old-boys/4Wym7jIj/</t>
         </is>
       </c>
     </row>
@@ -6553,71 +6553,71 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Racing Club</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I67" t="n">
         <v>1</v>
       </c>
       <c r="J67" t="n">
-        <v>2.62</v>
+        <v>2.04</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="L67" t="n">
-        <v>2.35</v>
+        <v>2.18</v>
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="N67" t="n">
-        <v>2.94</v>
+        <v>3.19</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="P67" t="n">
-        <v>3.13</v>
+        <v>3</v>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="R67" t="n">
-        <v>3.12</v>
+        <v>4.18</v>
       </c>
       <c r="S67" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="T67" t="n">
-        <v>3.47</v>
+        <v>4.13</v>
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-newells-old-boys/4Wym7jIj/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-colon-santa-fe/A90iIGQi/</t>
         </is>
       </c>
     </row>
@@ -7749,34 +7749,34 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="I80" t="n">
         <v>0</v>
       </c>
       <c r="J80" t="n">
-        <v>2.64</v>
+        <v>2.37</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>2.59</v>
+        <v>3.16</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="N80" t="n">
@@ -7784,11 +7784,11 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="P80" t="n">
-        <v>2.77</v>
+        <v>2.72</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
@@ -7796,24 +7796,24 @@
         </is>
       </c>
       <c r="R80" t="n">
-        <v>2.9</v>
+        <v>3.51</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="T80" t="n">
-        <v>3.5</v>
+        <v>2.86</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
         </is>
       </c>
     </row>
@@ -7841,34 +7841,34 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="I81" t="n">
         <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>2.37</v>
+        <v>2.64</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>3.16</v>
+        <v>2.59</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="N81" t="n">
@@ -7876,11 +7876,11 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="P81" t="n">
-        <v>2.72</v>
+        <v>2.77</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
@@ -7888,24 +7888,24 @@
         </is>
       </c>
       <c r="R81" t="n">
-        <v>3.51</v>
+        <v>2.9</v>
       </c>
       <c r="S81" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="T81" t="n">
-        <v>2.86</v>
+        <v>3.5</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -9229,22 +9229,22 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>2.25</v>
+        <v>2.3</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.49</v>
+        <v>2.14</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
@@ -9252,15 +9252,15 @@
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.04</v>
+        <v>3.05</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="P96" t="n">
-        <v>2.86</v>
+        <v>3.03</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
@@ -9268,15 +9268,15 @@
         </is>
       </c>
       <c r="R96" t="n">
-        <v>3.7</v>
+        <v>3.54</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="T96" t="n">
-        <v>3.54</v>
+        <v>4.22</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
         </is>
       </c>
     </row>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -9321,22 +9321,22 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>2.3</v>
+        <v>2.25</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>2.14</v>
+        <v>2.49</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
@@ -9344,15 +9344,15 @@
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.05</v>
+        <v>3.04</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>3.03</v>
+        <v>2.86</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
@@ -9360,16 +9360,16 @@
         </is>
       </c>
       <c r="R97" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>25/09/2023 22:42</t>
+        </is>
+      </c>
+      <c r="T97" t="n">
         <v>3.54</v>
       </c>
-      <c r="S97" t="inlineStr">
-        <is>
-          <t>26/09/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T97" t="n">
-        <v>4.22</v>
-      </c>
       <c r="U97" t="inlineStr">
         <is>
           <t>02/10/2023 23:29</t>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
         </is>
       </c>
     </row>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -9413,14 +9413,14 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>3.31</v>
+        <v>1.93</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
         </is>
       </c>
       <c r="L98" t="n">
-        <v>3.28</v>
+        <v>1.91</v>
       </c>
       <c r="M98" t="inlineStr">
         <is>
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="N98" t="n">
-        <v>2.97</v>
+        <v>3.29</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -9444,7 +9444,7 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>2.93</v>
+        <v>3.2</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
@@ -9452,7 +9452,7 @@
         </is>
       </c>
       <c r="R98" t="n">
-        <v>2.47</v>
+        <v>4.52</v>
       </c>
       <c r="S98" t="inlineStr">
         <is>
@@ -9460,7 +9460,7 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>2.59</v>
+        <v>5.03</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
@@ -9469,7 +9469,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
         </is>
       </c>
     </row>
@@ -9497,7 +9497,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G99" t="n">
@@ -9505,14 +9505,14 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I99" t="n">
         <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>1.93</v>
+        <v>3.31</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -9520,7 +9520,7 @@
         </is>
       </c>
       <c r="L99" t="n">
-        <v>1.91</v>
+        <v>3.28</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
@@ -9528,7 +9528,7 @@
         </is>
       </c>
       <c r="N99" t="n">
-        <v>3.29</v>
+        <v>2.97</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -9536,7 +9536,7 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>3.2</v>
+        <v>2.93</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
@@ -9544,7 +9544,7 @@
         </is>
       </c>
       <c r="R99" t="n">
-        <v>4.52</v>
+        <v>2.47</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
@@ -9552,7 +9552,7 @@
         </is>
       </c>
       <c r="T99" t="n">
-        <v>5.03</v>
+        <v>2.59</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
@@ -9561,7 +9561,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
         </is>
       </c>
     </row>
@@ -12901,7 +12901,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -12909,63 +12909,63 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J136" t="n">
-        <v>2.74</v>
+        <v>1.94</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="L136" t="n">
-        <v>2.55</v>
+        <v>1.89</v>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="N136" t="n">
-        <v>2.98</v>
+        <v>3.2</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="P136" t="n">
-        <v>3.06</v>
+        <v>3.14</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="R136" t="n">
-        <v>2.78</v>
+        <v>4.62</v>
       </c>
       <c r="S136" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="T136" t="n">
-        <v>3.18</v>
+        <v>5.29</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
         </is>
       </c>
     </row>
@@ -12993,7 +12993,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G137" t="n">
@@ -13001,63 +13001,63 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J137" t="n">
-        <v>1.94</v>
+        <v>2.74</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="L137" t="n">
-        <v>1.89</v>
+        <v>2.55</v>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="N137" t="n">
-        <v>3.2</v>
+        <v>2.98</v>
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="P137" t="n">
-        <v>3.14</v>
+        <v>3.06</v>
       </c>
       <c r="Q137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="R137" t="n">
-        <v>4.62</v>
+        <v>2.78</v>
       </c>
       <c r="S137" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="T137" t="n">
-        <v>5.29</v>
+        <v>3.18</v>
       </c>
       <c r="U137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
         </is>
       </c>
     </row>
@@ -14898,6 +14898,190 @@
       <c r="V157" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/river-plate-huracan/4denLMzd/</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E158" s="2" t="n">
+        <v>45234.79166666666</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Argentinos Jrs</t>
+        </is>
+      </c>
+      <c r="G158" t="n">
+        <v>1</v>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>Instituto</t>
+        </is>
+      </c>
+      <c r="I158" t="n">
+        <v>2</v>
+      </c>
+      <c r="J158" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>29/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L158" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>04/11/2023 18:54</t>
+        </is>
+      </c>
+      <c r="N158" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="O158" t="inlineStr">
+        <is>
+          <t>29/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P158" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="Q158" t="inlineStr">
+        <is>
+          <t>04/11/2023 18:53</t>
+        </is>
+      </c>
+      <c r="R158" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="S158" t="inlineStr">
+        <is>
+          <t>29/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T158" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="U158" t="inlineStr">
+        <is>
+          <t>04/11/2023 18:56</t>
+        </is>
+      </c>
+      <c r="V158" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-instituto/phYYrQS2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E159" s="2" t="n">
+        <v>45235.04166666666</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Atl. Tucuman</t>
+        </is>
+      </c>
+      <c r="G159" t="n">
+        <v>1</v>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>Independiente</t>
+        </is>
+      </c>
+      <c r="I159" t="n">
+        <v>2</v>
+      </c>
+      <c r="J159" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>30/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L159" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t>05/11/2023 00:55</t>
+        </is>
+      </c>
+      <c r="N159" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="O159" t="inlineStr">
+        <is>
+          <t>30/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P159" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="Q159" t="inlineStr">
+        <is>
+          <t>05/11/2023 00:55</t>
+        </is>
+      </c>
+      <c r="R159" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="S159" t="inlineStr">
+        <is>
+          <t>30/10/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T159" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="U159" t="inlineStr">
+        <is>
+          <t>05/11/2023 00:55</t>
+        </is>
+      </c>
+      <c r="V159" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-independiente/IucvNr6q/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 05-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V159"/>
+  <dimension ref="A1:V161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8117,30 +8117,30 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="I84" t="n">
         <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1.74</v>
+        <v>1.52</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="L84" t="n">
-        <v>1.72</v>
+        <v>1.67</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
@@ -8148,15 +8148,15 @@
         </is>
       </c>
       <c r="N84" t="n">
-        <v>3.47</v>
+        <v>4.1</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.54</v>
+        <v>3.69</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
@@ -8164,15 +8164,15 @@
         </is>
       </c>
       <c r="R84" t="n">
-        <v>5.5</v>
+        <v>6.9</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="T84" t="n">
-        <v>5.8</v>
+        <v>5.96</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
         </is>
       </c>
     </row>
@@ -8209,30 +8209,30 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I85" t="n">
         <v>0</v>
       </c>
       <c r="J85" t="n">
-        <v>1.52</v>
+        <v>1.74</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="L85" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
@@ -8240,15 +8240,15 @@
         </is>
       </c>
       <c r="N85" t="n">
-        <v>4.1</v>
+        <v>3.47</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.69</v>
+        <v>3.54</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
@@ -8256,15 +8256,15 @@
         </is>
       </c>
       <c r="R85" t="n">
-        <v>6.9</v>
+        <v>5.5</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="T85" t="n">
-        <v>5.96</v>
+        <v>5.8</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
@@ -8273,7 +8273,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
         </is>
       </c>
     </row>
@@ -12901,7 +12901,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -12909,63 +12909,63 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J136" t="n">
-        <v>1.94</v>
+        <v>2.74</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="L136" t="n">
-        <v>1.89</v>
+        <v>2.55</v>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="N136" t="n">
-        <v>3.2</v>
+        <v>2.98</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="P136" t="n">
-        <v>3.14</v>
+        <v>3.06</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="R136" t="n">
-        <v>4.62</v>
+        <v>2.78</v>
       </c>
       <c r="S136" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="T136" t="n">
-        <v>5.29</v>
+        <v>3.18</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
         </is>
       </c>
     </row>
@@ -12993,7 +12993,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G137" t="n">
@@ -13001,63 +13001,63 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J137" t="n">
-        <v>2.74</v>
+        <v>1.94</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="L137" t="n">
-        <v>2.55</v>
+        <v>1.89</v>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="N137" t="n">
-        <v>2.98</v>
+        <v>3.2</v>
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="P137" t="n">
-        <v>3.06</v>
+        <v>3.14</v>
       </c>
       <c r="Q137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="R137" t="n">
-        <v>2.78</v>
+        <v>4.62</v>
       </c>
       <c r="S137" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="T137" t="n">
-        <v>3.18</v>
+        <v>5.29</v>
       </c>
       <c r="U137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
         </is>
       </c>
     </row>
@@ -13269,22 +13269,22 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="G140" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="I140" t="n">
         <v>2</v>
       </c>
-      <c r="H140" t="inlineStr">
-        <is>
-          <t>Tigre</t>
-        </is>
-      </c>
-      <c r="I140" t="n">
-        <v>1</v>
-      </c>
       <c r="J140" t="n">
-        <v>2.24</v>
+        <v>2</v>
       </c>
       <c r="K140" t="inlineStr">
         <is>
@@ -13292,15 +13292,15 @@
         </is>
       </c>
       <c r="L140" t="n">
-        <v>2.6</v>
+        <v>2.15</v>
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:59</t>
+          <t>27/10/2023 01:34</t>
         </is>
       </c>
       <c r="N140" t="n">
-        <v>3.08</v>
+        <v>3.16</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -13308,15 +13308,15 @@
         </is>
       </c>
       <c r="P140" t="n">
-        <v>2.96</v>
+        <v>3.04</v>
       </c>
       <c r="Q140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:28</t>
+          <t>27/10/2023 01:34</t>
         </is>
       </c>
       <c r="R140" t="n">
-        <v>3.65</v>
+        <v>4.07</v>
       </c>
       <c r="S140" t="inlineStr">
         <is>
@@ -13324,16 +13324,16 @@
         </is>
       </c>
       <c r="T140" t="n">
-        <v>3.19</v>
+        <v>4.18</v>
       </c>
       <c r="U140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:56</t>
+          <t>27/10/2023 01:34</t>
         </is>
       </c>
       <c r="V140" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-tigre/dYdn4Ua4/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-godoy-cruz/dduZfQMj/</t>
         </is>
       </c>
     </row>
@@ -13361,22 +13361,22 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G141" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I141" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J141" t="n">
-        <v>2</v>
+        <v>2.24</v>
       </c>
       <c r="K141" t="inlineStr">
         <is>
@@ -13384,15 +13384,15 @@
         </is>
       </c>
       <c r="L141" t="n">
-        <v>2.15</v>
+        <v>2.6</v>
       </c>
       <c r="M141" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:59</t>
         </is>
       </c>
       <c r="N141" t="n">
-        <v>3.16</v>
+        <v>3.08</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -13400,15 +13400,15 @@
         </is>
       </c>
       <c r="P141" t="n">
-        <v>3.04</v>
+        <v>2.96</v>
       </c>
       <c r="Q141" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:28</t>
         </is>
       </c>
       <c r="R141" t="n">
-        <v>4.07</v>
+        <v>3.65</v>
       </c>
       <c r="S141" t="inlineStr">
         <is>
@@ -13416,16 +13416,16 @@
         </is>
       </c>
       <c r="T141" t="n">
-        <v>4.18</v>
+        <v>3.19</v>
       </c>
       <c r="U141" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:56</t>
         </is>
       </c>
       <c r="V141" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-godoy-cruz/dduZfQMj/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-tigre/dYdn4Ua4/</t>
         </is>
       </c>
     </row>
@@ -15082,6 +15082,190 @@
       <c r="V159" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-independiente/IucvNr6q/</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E160" s="2" t="n">
+        <v>45235.83333333334</v>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Velez Sarsfield</t>
+        </is>
+      </c>
+      <c r="G160" t="n">
+        <v>1</v>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>Talleres Cordoba</t>
+        </is>
+      </c>
+      <c r="I160" t="n">
+        <v>1</v>
+      </c>
+      <c r="J160" t="n">
+        <v>2.47</v>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="L160" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>05/11/2023 19:57</t>
+        </is>
+      </c>
+      <c r="N160" t="n">
+        <v>3</v>
+      </c>
+      <c r="O160" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="P160" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="Q160" t="inlineStr">
+        <is>
+          <t>05/11/2023 19:56</t>
+        </is>
+      </c>
+      <c r="R160" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="S160" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="T160" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="U160" t="inlineStr">
+        <is>
+          <t>05/11/2023 19:57</t>
+        </is>
+      </c>
+      <c r="V160" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-talleres-cordoba/beG7S4rM/</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E161" s="2" t="n">
+        <v>45235.85416666666</v>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Union de Santa Fe</t>
+        </is>
+      </c>
+      <c r="G161" t="n">
+        <v>0</v>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>Lanus</t>
+        </is>
+      </c>
+      <c r="I161" t="n">
+        <v>0</v>
+      </c>
+      <c r="J161" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>01/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L161" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="M161" t="inlineStr">
+        <is>
+          <t>05/11/2023 20:22</t>
+        </is>
+      </c>
+      <c r="N161" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="O161" t="inlineStr">
+        <is>
+          <t>01/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P161" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="Q161" t="inlineStr">
+        <is>
+          <t>05/11/2023 20:20</t>
+        </is>
+      </c>
+      <c r="R161" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="S161" t="inlineStr">
+        <is>
+          <t>01/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T161" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="U161" t="inlineStr">
+        <is>
+          <t>05/11/2023 20:22</t>
+        </is>
+      </c>
+      <c r="V161" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-lanus/hIyss4cF/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 06-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V161"/>
+  <dimension ref="A1:V164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6461,71 +6461,71 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Racing Club</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I66" t="n">
         <v>1</v>
       </c>
       <c r="J66" t="n">
-        <v>2.62</v>
+        <v>2.04</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="L66" t="n">
-        <v>2.35</v>
+        <v>2.18</v>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="N66" t="n">
-        <v>2.94</v>
+        <v>3.19</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="P66" t="n">
-        <v>3.13</v>
+        <v>3</v>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="R66" t="n">
-        <v>3.12</v>
+        <v>4.18</v>
       </c>
       <c r="S66" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="T66" t="n">
-        <v>3.47</v>
+        <v>4.13</v>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-newells-old-boys/4Wym7jIj/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-colon-santa-fe/A90iIGQi/</t>
         </is>
       </c>
     </row>
@@ -6553,71 +6553,71 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Racing Club</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="I67" t="n">
         <v>1</v>
       </c>
       <c r="J67" t="n">
-        <v>2.04</v>
+        <v>2.62</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="L67" t="n">
-        <v>2.18</v>
+        <v>2.35</v>
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="N67" t="n">
-        <v>3.19</v>
+        <v>2.94</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="P67" t="n">
-        <v>3</v>
+        <v>3.13</v>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="R67" t="n">
-        <v>4.18</v>
+        <v>3.12</v>
       </c>
       <c r="S67" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="T67" t="n">
-        <v>4.13</v>
+        <v>3.47</v>
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-colon-santa-fe/A90iIGQi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-newells-old-boys/4Wym7jIj/</t>
         </is>
       </c>
     </row>
@@ -7933,62 +7933,62 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Racing Club</t>
         </is>
       </c>
       <c r="I82" t="n">
         <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>3.03</v>
+        <v>2.34</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="L82" t="n">
-        <v>2.95</v>
+        <v>2.29</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>25/09/2023 23:25</t>
+          <t>25/09/2023 23:29</t>
         </is>
       </c>
       <c r="N82" t="n">
-        <v>3.09</v>
+        <v>3.2</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="P82" t="n">
-        <v>3.16</v>
+        <v>3.36</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>25/09/2023 23:20</t>
+          <t>25/09/2023 23:29</t>
         </is>
       </c>
       <c r="R82" t="n">
-        <v>2.46</v>
+        <v>3.3</v>
       </c>
       <c r="S82" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="T82" t="n">
-        <v>2.64</v>
+        <v>3.35</v>
       </c>
       <c r="U82" t="inlineStr">
         <is>
@@ -7997,7 +7997,7 @@
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-argentinos-jrs/0IHoSifG/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-racing-club/8OvDrDvc/</t>
         </is>
       </c>
     </row>
@@ -8025,71 +8025,71 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Racing Club</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I83" t="n">
         <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>2.34</v>
+        <v>3.03</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>24/09/2023 05:42</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>2.29</v>
+        <v>2.95</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
+          <t>25/09/2023 23:25</t>
+        </is>
+      </c>
+      <c r="N83" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>21/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P83" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>25/09/2023 23:20</t>
+        </is>
+      </c>
+      <c r="R83" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>21/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T83" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
           <t>25/09/2023 23:29</t>
         </is>
       </c>
-      <c r="N83" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>24/09/2023 05:42</t>
-        </is>
-      </c>
-      <c r="P83" t="n">
-        <v>3.36</v>
-      </c>
-      <c r="Q83" t="inlineStr">
-        <is>
-          <t>25/09/2023 23:29</t>
-        </is>
-      </c>
-      <c r="R83" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="S83" t="inlineStr">
-        <is>
-          <t>24/09/2023 05:42</t>
-        </is>
-      </c>
-      <c r="T83" t="n">
-        <v>3.35</v>
-      </c>
-      <c r="U83" t="inlineStr">
-        <is>
-          <t>25/09/2023 23:29</t>
-        </is>
-      </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-racing-club/8OvDrDvc/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-argentinos-jrs/0IHoSifG/</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -9229,22 +9229,22 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>2.3</v>
+        <v>2.25</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.14</v>
+        <v>2.49</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
@@ -9252,15 +9252,15 @@
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.05</v>
+        <v>3.04</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.03</v>
+        <v>2.86</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
@@ -9268,16 +9268,16 @@
         </is>
       </c>
       <c r="R96" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>25/09/2023 22:42</t>
+        </is>
+      </c>
+      <c r="T96" t="n">
         <v>3.54</v>
       </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>26/09/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T96" t="n">
-        <v>4.22</v>
-      </c>
       <c r="U96" t="inlineStr">
         <is>
           <t>02/10/2023 23:29</t>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
         </is>
       </c>
     </row>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -9321,22 +9321,22 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>2.25</v>
+        <v>2.3</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>2.49</v>
+        <v>2.14</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
@@ -9344,15 +9344,15 @@
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.04</v>
+        <v>3.05</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>2.86</v>
+        <v>3.03</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
@@ -9360,15 +9360,15 @@
         </is>
       </c>
       <c r="R97" t="n">
-        <v>3.7</v>
+        <v>3.54</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="T97" t="n">
-        <v>3.54</v>
+        <v>4.22</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
         </is>
       </c>
     </row>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -9413,14 +9413,14 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>1.93</v>
+        <v>3.31</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
         </is>
       </c>
       <c r="L98" t="n">
-        <v>1.91</v>
+        <v>3.28</v>
       </c>
       <c r="M98" t="inlineStr">
         <is>
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="N98" t="n">
-        <v>3.29</v>
+        <v>2.97</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -9444,7 +9444,7 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>3.2</v>
+        <v>2.93</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
@@ -9452,7 +9452,7 @@
         </is>
       </c>
       <c r="R98" t="n">
-        <v>4.52</v>
+        <v>2.47</v>
       </c>
       <c r="S98" t="inlineStr">
         <is>
@@ -9460,7 +9460,7 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>5.03</v>
+        <v>2.59</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
@@ -9469,7 +9469,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
         </is>
       </c>
     </row>
@@ -9497,7 +9497,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G99" t="n">
@@ -9505,14 +9505,14 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I99" t="n">
         <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>3.31</v>
+        <v>1.93</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -9520,7 +9520,7 @@
         </is>
       </c>
       <c r="L99" t="n">
-        <v>3.28</v>
+        <v>1.91</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
@@ -9528,7 +9528,7 @@
         </is>
       </c>
       <c r="N99" t="n">
-        <v>2.97</v>
+        <v>3.29</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -9536,7 +9536,7 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>2.93</v>
+        <v>3.2</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
@@ -9544,7 +9544,7 @@
         </is>
       </c>
       <c r="R99" t="n">
-        <v>2.47</v>
+        <v>4.52</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
@@ -9552,7 +9552,7 @@
         </is>
       </c>
       <c r="T99" t="n">
-        <v>2.59</v>
+        <v>5.03</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
@@ -9561,7 +9561,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,63 +9781,63 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J102" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>1.9</v>
+        <v>2.17</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.58</v>
+        <v>3.37</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.47</v>
+        <v>3.06</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>4.7</v>
+        <v>4.33</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>4.55</v>
+        <v>4.04</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -9873,63 +9873,63 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J103" t="n">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>2.17</v>
+        <v>1.9</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.37</v>
+        <v>3.58</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.06</v>
+        <v>3.47</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>4.33</v>
+        <v>4.7</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4.04</v>
+        <v>4.55</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
         </is>
       </c>
     </row>
@@ -10509,71 +10509,71 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G110" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J110" t="n">
-        <v>3.26</v>
+        <v>2.5</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L110" t="n">
-        <v>3.55</v>
+        <v>2.6</v>
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:59</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="N110" t="n">
-        <v>2.96</v>
+        <v>3.13</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P110" t="n">
-        <v>2.9</v>
+        <v>2.84</v>
       </c>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:58</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="R110" t="n">
-        <v>2.51</v>
+        <v>2.93</v>
       </c>
       <c r="S110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T110" t="n">
-        <v>2.46</v>
+        <v>2.91</v>
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:53</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
         </is>
       </c>
     </row>
@@ -10601,71 +10601,71 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="G111" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J111" t="n">
-        <v>2.5</v>
+        <v>3.26</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="L111" t="n">
-        <v>2.6</v>
+        <v>3.55</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:59</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>3.13</v>
+        <v>2.96</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="P111" t="n">
-        <v>2.84</v>
+        <v>2.9</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:58</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>2.93</v>
+        <v>2.51</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="T111" t="n">
-        <v>2.91</v>
+        <v>2.46</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:53</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
         </is>
       </c>
     </row>
@@ -15266,6 +15266,282 @@
       <c r="V161" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-lanus/hIyss4cF/</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E162" s="2" t="n">
+        <v>45235.9375</v>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Racing Club</t>
+        </is>
+      </c>
+      <c r="G162" t="n">
+        <v>1</v>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>Central Cordoba</t>
+        </is>
+      </c>
+      <c r="I162" t="n">
+        <v>1</v>
+      </c>
+      <c r="J162" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>02/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="L162" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>05/11/2023 22:26</t>
+        </is>
+      </c>
+      <c r="N162" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
+          <t>02/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P162" t="n">
+        <v>3.96</v>
+      </c>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>05/11/2023 22:26</t>
+        </is>
+      </c>
+      <c r="R162" t="n">
+        <v>5.15</v>
+      </c>
+      <c r="S162" t="inlineStr">
+        <is>
+          <t>02/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T162" t="n">
+        <v>6.28</v>
+      </c>
+      <c r="U162" t="inlineStr">
+        <is>
+          <t>05/11/2023 22:26</t>
+        </is>
+      </c>
+      <c r="V162" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-central-cordoba-santiago-del-estero/UsaAPySs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E163" s="2" t="n">
+        <v>45236.02083333334</v>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Estudiantes L.P.</t>
+        </is>
+      </c>
+      <c r="G163" t="n">
+        <v>2</v>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>Defensa y Justicia</t>
+        </is>
+      </c>
+      <c r="I163" t="n">
+        <v>1</v>
+      </c>
+      <c r="J163" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>02/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="L163" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>06/11/2023 00:29</t>
+        </is>
+      </c>
+      <c r="N163" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
+          <t>02/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P163" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="Q163" t="inlineStr">
+        <is>
+          <t>06/11/2023 00:29</t>
+        </is>
+      </c>
+      <c r="R163" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="S163" t="inlineStr">
+        <is>
+          <t>02/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T163" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="U163" t="inlineStr">
+        <is>
+          <t>06/11/2023 00:29</t>
+        </is>
+      </c>
+      <c r="V163" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-defensa-y-justicia/nJgFOesl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E164" s="2" t="n">
+        <v>45236.04166666666</v>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Newells Old Boys</t>
+        </is>
+      </c>
+      <c r="G164" t="n">
+        <v>0</v>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>Sarmiento Junin</t>
+        </is>
+      </c>
+      <c r="I164" t="n">
+        <v>1</v>
+      </c>
+      <c r="J164" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:42</t>
+        </is>
+      </c>
+      <c r="L164" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="M164" t="inlineStr">
+        <is>
+          <t>06/11/2023 00:59</t>
+        </is>
+      </c>
+      <c r="N164" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="O164" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:42</t>
+        </is>
+      </c>
+      <c r="P164" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="Q164" t="inlineStr">
+        <is>
+          <t>06/11/2023 00:59</t>
+        </is>
+      </c>
+      <c r="R164" t="n">
+        <v>5.83</v>
+      </c>
+      <c r="S164" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:42</t>
+        </is>
+      </c>
+      <c r="T164" t="n">
+        <v>5.96</v>
+      </c>
+      <c r="U164" t="inlineStr">
+        <is>
+          <t>06/11/2023 00:59</t>
+        </is>
+      </c>
+      <c r="V164" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-sarmiento-junin/KWiNMZB0/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 07-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V164"/>
+  <dimension ref="A1:V168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5909,30 +5909,30 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Gimnasia L.P.</t>
+          <t>Independiente</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" t="n">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>15/09/2023 01:13</t>
+          <t>16/09/2023 01:13</t>
         </is>
       </c>
       <c r="L60" t="n">
-        <v>1.9</v>
+        <v>2.78</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
@@ -5940,15 +5940,15 @@
         </is>
       </c>
       <c r="N60" t="n">
-        <v>3.3</v>
+        <v>3.12</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>15/09/2023 01:13</t>
+          <t>16/09/2023 01:13</t>
         </is>
       </c>
       <c r="P60" t="n">
-        <v>3.1</v>
+        <v>3.02</v>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
@@ -5956,15 +5956,15 @@
         </is>
       </c>
       <c r="R60" t="n">
-        <v>4.82</v>
+        <v>4.04</v>
       </c>
       <c r="S60" t="inlineStr">
         <is>
-          <t>15/09/2023 01:13</t>
+          <t>16/09/2023 01:13</t>
         </is>
       </c>
       <c r="T60" t="n">
-        <v>5.38</v>
+        <v>2.93</v>
       </c>
       <c r="U60" t="inlineStr">
         <is>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-gimnasia-l-p/IZ3aGfe4/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-independiente/vq5eHztb/</t>
         </is>
       </c>
     </row>
@@ -6001,30 +6001,30 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Independiente</t>
+          <t>Gimnasia L.P.</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>16/09/2023 01:13</t>
+          <t>15/09/2023 01:13</t>
         </is>
       </c>
       <c r="L61" t="n">
-        <v>2.78</v>
+        <v>1.9</v>
       </c>
       <c r="M61" t="inlineStr">
         <is>
@@ -6032,15 +6032,15 @@
         </is>
       </c>
       <c r="N61" t="n">
-        <v>3.12</v>
+        <v>3.3</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>16/09/2023 01:13</t>
+          <t>15/09/2023 01:13</t>
         </is>
       </c>
       <c r="P61" t="n">
-        <v>3.02</v>
+        <v>3.1</v>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
@@ -6048,15 +6048,15 @@
         </is>
       </c>
       <c r="R61" t="n">
-        <v>4.04</v>
+        <v>4.82</v>
       </c>
       <c r="S61" t="inlineStr">
         <is>
-          <t>16/09/2023 01:13</t>
+          <t>15/09/2023 01:13</t>
         </is>
       </c>
       <c r="T61" t="n">
-        <v>2.93</v>
+        <v>5.38</v>
       </c>
       <c r="U61" t="inlineStr">
         <is>
@@ -6065,7 +6065,7 @@
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-independiente/vq5eHztb/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-gimnasia-l-p/IZ3aGfe4/</t>
         </is>
       </c>
     </row>
@@ -6277,71 +6277,71 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Velez Sarsfield</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>San Lorenzo</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>1.69</v>
+        <v>2.04</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="L64" t="n">
-        <v>1.74</v>
+        <v>2.29</v>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:23</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="N64" t="n">
-        <v>3.41</v>
+        <v>3.04</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="P64" t="n">
-        <v>3.4</v>
+        <v>2.85</v>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:23</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="R64" t="n">
-        <v>5.46</v>
+        <v>4.47</v>
       </c>
       <c r="S64" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="T64" t="n">
-        <v>6</v>
+        <v>4.05</v>
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:27</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-arsenal-sarandi/OEeXCLlC/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-san-lorenzo/IZPUVZfi/</t>
         </is>
       </c>
     </row>
@@ -6369,71 +6369,71 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Velez Sarsfield</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>San Lorenzo</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J65" t="n">
-        <v>2.04</v>
+        <v>1.69</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="L65" t="n">
-        <v>2.29</v>
+        <v>1.74</v>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:23</t>
         </is>
       </c>
       <c r="N65" t="n">
-        <v>3.04</v>
+        <v>3.41</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="P65" t="n">
-        <v>2.85</v>
+        <v>3.4</v>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:23</t>
         </is>
       </c>
       <c r="R65" t="n">
-        <v>4.47</v>
+        <v>5.46</v>
       </c>
       <c r="S65" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="T65" t="n">
-        <v>4.05</v>
+        <v>6</v>
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:27</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-san-lorenzo/IZPUVZfi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-arsenal-sarandi/OEeXCLlC/</t>
         </is>
       </c>
     </row>
@@ -7749,34 +7749,34 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="I80" t="n">
         <v>0</v>
       </c>
       <c r="J80" t="n">
-        <v>2.37</v>
+        <v>2.64</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>3.16</v>
+        <v>2.59</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="N80" t="n">
@@ -7784,11 +7784,11 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="P80" t="n">
-        <v>2.72</v>
+        <v>2.77</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
@@ -7796,24 +7796,24 @@
         </is>
       </c>
       <c r="R80" t="n">
-        <v>3.51</v>
+        <v>2.9</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="T80" t="n">
-        <v>2.86</v>
+        <v>3.5</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
         </is>
       </c>
     </row>
@@ -7841,34 +7841,34 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="I81" t="n">
         <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>2.64</v>
+        <v>2.37</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>2.59</v>
+        <v>3.16</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="N81" t="n">
@@ -7876,11 +7876,11 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="P81" t="n">
-        <v>2.77</v>
+        <v>2.72</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
@@ -7888,24 +7888,24 @@
         </is>
       </c>
       <c r="R81" t="n">
-        <v>2.9</v>
+        <v>3.51</v>
       </c>
       <c r="S81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="T81" t="n">
-        <v>3.5</v>
+        <v>2.86</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
         </is>
       </c>
     </row>
@@ -7933,71 +7933,71 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Racing Club</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I82" t="n">
         <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>2.34</v>
+        <v>3.03</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>24/09/2023 05:42</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="L82" t="n">
-        <v>2.29</v>
+        <v>2.95</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
+          <t>25/09/2023 23:25</t>
+        </is>
+      </c>
+      <c r="N82" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>21/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P82" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>25/09/2023 23:20</t>
+        </is>
+      </c>
+      <c r="R82" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>21/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T82" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
           <t>25/09/2023 23:29</t>
         </is>
       </c>
-      <c r="N82" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>24/09/2023 05:42</t>
-        </is>
-      </c>
-      <c r="P82" t="n">
-        <v>3.36</v>
-      </c>
-      <c r="Q82" t="inlineStr">
-        <is>
-          <t>25/09/2023 23:29</t>
-        </is>
-      </c>
-      <c r="R82" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="S82" t="inlineStr">
-        <is>
-          <t>24/09/2023 05:42</t>
-        </is>
-      </c>
-      <c r="T82" t="n">
-        <v>3.35</v>
-      </c>
-      <c r="U82" t="inlineStr">
-        <is>
-          <t>25/09/2023 23:29</t>
-        </is>
-      </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-racing-club/8OvDrDvc/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-argentinos-jrs/0IHoSifG/</t>
         </is>
       </c>
     </row>
@@ -8025,62 +8025,62 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Racing Club</t>
         </is>
       </c>
       <c r="I83" t="n">
         <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>3.03</v>
+        <v>2.34</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>2.95</v>
+        <v>2.29</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>25/09/2023 23:25</t>
+          <t>25/09/2023 23:29</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>3.09</v>
+        <v>3.2</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="P83" t="n">
-        <v>3.16</v>
+        <v>3.36</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>25/09/2023 23:20</t>
+          <t>25/09/2023 23:29</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>2.46</v>
+        <v>3.3</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="T83" t="n">
-        <v>2.64</v>
+        <v>3.35</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
@@ -8089,7 +8089,7 @@
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-argentinos-jrs/0IHoSifG/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-racing-club/8OvDrDvc/</t>
         </is>
       </c>
     </row>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -9413,14 +9413,14 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>3.31</v>
+        <v>1.93</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
         </is>
       </c>
       <c r="L98" t="n">
-        <v>3.28</v>
+        <v>1.91</v>
       </c>
       <c r="M98" t="inlineStr">
         <is>
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="N98" t="n">
-        <v>2.97</v>
+        <v>3.29</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -9444,7 +9444,7 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>2.93</v>
+        <v>3.2</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
@@ -9452,7 +9452,7 @@
         </is>
       </c>
       <c r="R98" t="n">
-        <v>2.47</v>
+        <v>4.52</v>
       </c>
       <c r="S98" t="inlineStr">
         <is>
@@ -9460,7 +9460,7 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>2.59</v>
+        <v>5.03</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
@@ -9469,7 +9469,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
         </is>
       </c>
     </row>
@@ -9497,7 +9497,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G99" t="n">
@@ -9505,14 +9505,14 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I99" t="n">
         <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>1.93</v>
+        <v>3.31</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -9520,7 +9520,7 @@
         </is>
       </c>
       <c r="L99" t="n">
-        <v>1.91</v>
+        <v>3.28</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
@@ -9528,7 +9528,7 @@
         </is>
       </c>
       <c r="N99" t="n">
-        <v>3.29</v>
+        <v>2.97</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -9536,7 +9536,7 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>3.2</v>
+        <v>2.93</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
@@ -9544,7 +9544,7 @@
         </is>
       </c>
       <c r="R99" t="n">
-        <v>4.52</v>
+        <v>2.47</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
@@ -9552,7 +9552,7 @@
         </is>
       </c>
       <c r="T99" t="n">
-        <v>5.03</v>
+        <v>2.59</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
@@ -9561,7 +9561,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,63 +9781,63 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J102" t="n">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>2.17</v>
+        <v>1.9</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.37</v>
+        <v>3.58</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.06</v>
+        <v>3.47</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>4.33</v>
+        <v>4.7</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>4.04</v>
+        <v>4.55</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -9873,63 +9873,63 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J103" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>1.9</v>
+        <v>2.17</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.58</v>
+        <v>3.37</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.47</v>
+        <v>3.06</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>4.7</v>
+        <v>4.33</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4.55</v>
+        <v>4.04</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
         </is>
       </c>
     </row>
@@ -10509,71 +10509,71 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="G110" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J110" t="n">
-        <v>2.5</v>
+        <v>3.26</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="L110" t="n">
-        <v>2.6</v>
+        <v>3.55</v>
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:59</t>
         </is>
       </c>
       <c r="N110" t="n">
-        <v>3.13</v>
+        <v>2.96</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="P110" t="n">
-        <v>2.84</v>
+        <v>2.9</v>
       </c>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:58</t>
         </is>
       </c>
       <c r="R110" t="n">
-        <v>2.93</v>
+        <v>2.51</v>
       </c>
       <c r="S110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="T110" t="n">
-        <v>2.91</v>
+        <v>2.46</v>
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:53</t>
         </is>
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
         </is>
       </c>
     </row>
@@ -10601,71 +10601,71 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G111" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J111" t="n">
-        <v>3.26</v>
+        <v>2.5</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L111" t="n">
-        <v>3.55</v>
+        <v>2.6</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:59</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>2.96</v>
+        <v>3.13</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P111" t="n">
-        <v>2.9</v>
+        <v>2.84</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:58</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>2.51</v>
+        <v>2.93</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T111" t="n">
-        <v>2.46</v>
+        <v>2.91</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:53</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
         </is>
       </c>
     </row>
@@ -11889,7 +11889,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G125" t="n">
@@ -11897,14 +11897,14 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I125" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J125" t="n">
-        <v>2.03</v>
+        <v>1.43</v>
       </c>
       <c r="K125" t="inlineStr">
         <is>
@@ -11912,15 +11912,15 @@
         </is>
       </c>
       <c r="L125" t="n">
-        <v>2.04</v>
+        <v>1.48</v>
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:58</t>
+          <t>20/10/2023 23:52</t>
         </is>
       </c>
       <c r="N125" t="n">
-        <v>3.07</v>
+        <v>4.42</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -11928,15 +11928,15 @@
         </is>
       </c>
       <c r="P125" t="n">
-        <v>2.89</v>
+        <v>4.33</v>
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:56</t>
+          <t>20/10/2023 23:59</t>
         </is>
       </c>
       <c r="R125" t="n">
-        <v>4.41</v>
+        <v>6.91</v>
       </c>
       <c r="S125" t="inlineStr">
         <is>
@@ -11944,16 +11944,16 @@
         </is>
       </c>
       <c r="T125" t="n">
-        <v>5.06</v>
+        <v>7.59</v>
       </c>
       <c r="U125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:58</t>
+          <t>20/10/2023 23:52</t>
         </is>
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-instituto/KOmLi0As/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-arsenal-sarandi/l4uxlI96/</t>
         </is>
       </c>
     </row>
@@ -11981,7 +11981,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G126" t="n">
@@ -11989,14 +11989,14 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I126" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J126" t="n">
-        <v>1.43</v>
+        <v>2.03</v>
       </c>
       <c r="K126" t="inlineStr">
         <is>
@@ -12004,15 +12004,15 @@
         </is>
       </c>
       <c r="L126" t="n">
-        <v>1.48</v>
+        <v>2.04</v>
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:52</t>
+          <t>20/10/2023 23:58</t>
         </is>
       </c>
       <c r="N126" t="n">
-        <v>4.42</v>
+        <v>3.07</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -12020,15 +12020,15 @@
         </is>
       </c>
       <c r="P126" t="n">
-        <v>4.33</v>
+        <v>2.89</v>
       </c>
       <c r="Q126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:59</t>
+          <t>20/10/2023 23:56</t>
         </is>
       </c>
       <c r="R126" t="n">
-        <v>6.91</v>
+        <v>4.41</v>
       </c>
       <c r="S126" t="inlineStr">
         <is>
@@ -12036,16 +12036,16 @@
         </is>
       </c>
       <c r="T126" t="n">
-        <v>7.59</v>
+        <v>5.06</v>
       </c>
       <c r="U126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:52</t>
+          <t>20/10/2023 23:58</t>
         </is>
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-arsenal-sarandi/l4uxlI96/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-instituto/KOmLi0As/</t>
         </is>
       </c>
     </row>
@@ -13269,22 +13269,22 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G140" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I140" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J140" t="n">
-        <v>2</v>
+        <v>2.24</v>
       </c>
       <c r="K140" t="inlineStr">
         <is>
@@ -13292,15 +13292,15 @@
         </is>
       </c>
       <c r="L140" t="n">
-        <v>2.15</v>
+        <v>2.6</v>
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:59</t>
         </is>
       </c>
       <c r="N140" t="n">
-        <v>3.16</v>
+        <v>3.08</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -13308,15 +13308,15 @@
         </is>
       </c>
       <c r="P140" t="n">
-        <v>3.04</v>
+        <v>2.96</v>
       </c>
       <c r="Q140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:28</t>
         </is>
       </c>
       <c r="R140" t="n">
-        <v>4.07</v>
+        <v>3.65</v>
       </c>
       <c r="S140" t="inlineStr">
         <is>
@@ -13324,16 +13324,16 @@
         </is>
       </c>
       <c r="T140" t="n">
-        <v>4.18</v>
+        <v>3.19</v>
       </c>
       <c r="U140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:56</t>
         </is>
       </c>
       <c r="V140" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-godoy-cruz/dduZfQMj/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-tigre/dYdn4Ua4/</t>
         </is>
       </c>
     </row>
@@ -13361,22 +13361,22 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="G141" t="n">
+        <v>0</v>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="I141" t="n">
         <v>2</v>
       </c>
-      <c r="H141" t="inlineStr">
-        <is>
-          <t>Tigre</t>
-        </is>
-      </c>
-      <c r="I141" t="n">
-        <v>1</v>
-      </c>
       <c r="J141" t="n">
-        <v>2.24</v>
+        <v>2</v>
       </c>
       <c r="K141" t="inlineStr">
         <is>
@@ -13384,15 +13384,15 @@
         </is>
       </c>
       <c r="L141" t="n">
-        <v>2.6</v>
+        <v>2.15</v>
       </c>
       <c r="M141" t="inlineStr">
         <is>
-          <t>27/10/2023 01:59</t>
+          <t>27/10/2023 01:34</t>
         </is>
       </c>
       <c r="N141" t="n">
-        <v>3.08</v>
+        <v>3.16</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -13400,15 +13400,15 @@
         </is>
       </c>
       <c r="P141" t="n">
-        <v>2.96</v>
+        <v>3.04</v>
       </c>
       <c r="Q141" t="inlineStr">
         <is>
-          <t>27/10/2023 01:28</t>
+          <t>27/10/2023 01:34</t>
         </is>
       </c>
       <c r="R141" t="n">
-        <v>3.65</v>
+        <v>4.07</v>
       </c>
       <c r="S141" t="inlineStr">
         <is>
@@ -13416,16 +13416,16 @@
         </is>
       </c>
       <c r="T141" t="n">
-        <v>3.19</v>
+        <v>4.18</v>
       </c>
       <c r="U141" t="inlineStr">
         <is>
-          <t>27/10/2023 01:56</t>
+          <t>27/10/2023 01:34</t>
         </is>
       </c>
       <c r="V141" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-tigre/dYdn4Ua4/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-godoy-cruz/dduZfQMj/</t>
         </is>
       </c>
     </row>
@@ -15542,6 +15542,374 @@
       <c r="V164" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-sarmiento-junin/KWiNMZB0/</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E165" s="2" t="n">
+        <v>45236.9375</v>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Barracas Central</t>
+        </is>
+      </c>
+      <c r="G165" t="n">
+        <v>1</v>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>Rosario Central</t>
+        </is>
+      </c>
+      <c r="I165" t="n">
+        <v>1</v>
+      </c>
+      <c r="J165" t="n">
+        <v>2.47</v>
+      </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L165" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t>06/11/2023 22:25</t>
+        </is>
+      </c>
+      <c r="N165" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="O165" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P165" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="Q165" t="inlineStr">
+        <is>
+          <t>06/11/2023 22:25</t>
+        </is>
+      </c>
+      <c r="R165" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="S165" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T165" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="U165" t="inlineStr">
+        <is>
+          <t>06/11/2023 22:25</t>
+        </is>
+      </c>
+      <c r="V165" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-rosario-central/rmfjKtj2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E166" s="2" t="n">
+        <v>45236.9375</v>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="G166" t="n">
+        <v>2</v>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>Platense</t>
+        </is>
+      </c>
+      <c r="I166" t="n">
+        <v>0</v>
+      </c>
+      <c r="J166" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>31/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L166" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t>06/11/2023 22:02</t>
+        </is>
+      </c>
+      <c r="N166" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="O166" t="inlineStr">
+        <is>
+          <t>31/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P166" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="Q166" t="inlineStr">
+        <is>
+          <t>06/11/2023 22:02</t>
+        </is>
+      </c>
+      <c r="R166" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="S166" t="inlineStr">
+        <is>
+          <t>31/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T166" t="n">
+        <v>5.29</v>
+      </c>
+      <c r="U166" t="inlineStr">
+        <is>
+          <t>06/11/2023 22:02</t>
+        </is>
+      </c>
+      <c r="V166" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-platense/IHAQLgR6/</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E167" s="2" t="n">
+        <v>45237.04166666666</v>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Banfield</t>
+        </is>
+      </c>
+      <c r="G167" t="n">
+        <v>2</v>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>Colon Santa Fe</t>
+        </is>
+      </c>
+      <c r="I167" t="n">
+        <v>1</v>
+      </c>
+      <c r="J167" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="L167" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>07/11/2023 00:57</t>
+        </is>
+      </c>
+      <c r="N167" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="O167" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="P167" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q167" t="inlineStr">
+        <is>
+          <t>07/11/2023 00:57</t>
+        </is>
+      </c>
+      <c r="R167" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="S167" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="T167" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="U167" t="inlineStr">
+        <is>
+          <t>07/11/2023 00:46</t>
+        </is>
+      </c>
+      <c r="V167" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-colon-santa-fe/CbKBROcS/</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E168" s="2" t="n">
+        <v>45237.04166666666</v>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Belgrano</t>
+        </is>
+      </c>
+      <c r="G168" t="n">
+        <v>0</v>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>Tigre</t>
+        </is>
+      </c>
+      <c r="I168" t="n">
+        <v>3</v>
+      </c>
+      <c r="J168" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>31/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L168" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>07/11/2023 00:59</t>
+        </is>
+      </c>
+      <c r="N168" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="O168" t="inlineStr">
+        <is>
+          <t>31/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P168" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="Q168" t="inlineStr">
+        <is>
+          <t>07/11/2023 00:59</t>
+        </is>
+      </c>
+      <c r="R168" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="S168" t="inlineStr">
+        <is>
+          <t>31/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T168" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="U168" t="inlineStr">
+        <is>
+          <t>07/11/2023 00:59</t>
+        </is>
+      </c>
+      <c r="V168" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-tigre/bexwrpr9/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 09-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V168"/>
+  <dimension ref="A1:V169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15913,6 +15913,98 @@
         </is>
       </c>
     </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E169" s="2" t="n">
+        <v>45238.95833333334</v>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="G169" t="n">
+        <v>1</v>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>Boca Juniors</t>
+        </is>
+      </c>
+      <c r="I169" t="n">
+        <v>1</v>
+      </c>
+      <c r="J169" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>30/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L169" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t>08/11/2023 22:58</t>
+        </is>
+      </c>
+      <c r="N169" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="O169" t="inlineStr">
+        <is>
+          <t>30/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P169" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="Q169" t="inlineStr">
+        <is>
+          <t>08/11/2023 22:31</t>
+        </is>
+      </c>
+      <c r="R169" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="S169" t="inlineStr">
+        <is>
+          <t>30/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T169" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="U169" t="inlineStr">
+        <is>
+          <t>08/11/2023 22:56</t>
+        </is>
+      </c>
+      <c r="V169" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/san-lorenzo-boca-juniors/Q9hJNFdf/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 12-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V172"/>
+  <dimension ref="A1:V175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6093,71 +6093,71 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I62" t="n">
         <v>0</v>
       </c>
       <c r="J62" t="n">
-        <v>2.72</v>
+        <v>2.49</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="L62" t="n">
-        <v>3.41</v>
+        <v>2.67</v>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:59</t>
+          <t>20/09/2023 20:58</t>
         </is>
       </c>
       <c r="N62" t="n">
-        <v>2.92</v>
+        <v>3.2</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="P62" t="n">
-        <v>2.8</v>
+        <v>3.03</v>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:52</t>
+          <t>20/09/2023 20:53</t>
         </is>
       </c>
       <c r="R62" t="n">
-        <v>3</v>
+        <v>3.05</v>
       </c>
       <c r="S62" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="T62" t="n">
-        <v>2.61</v>
+        <v>3.04</v>
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:59</t>
+          <t>20/09/2023 20:53</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-banfield/UDN4fDYp/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-tigre/0bg4FEAA/</t>
         </is>
       </c>
     </row>
@@ -6185,71 +6185,71 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I63" t="n">
         <v>0</v>
       </c>
       <c r="J63" t="n">
-        <v>2.49</v>
+        <v>2.72</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="L63" t="n">
-        <v>2.67</v>
+        <v>3.41</v>
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:58</t>
+          <t>20/09/2023 20:59</t>
         </is>
       </c>
       <c r="N63" t="n">
-        <v>3.2</v>
+        <v>2.92</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="P63" t="n">
-        <v>3.03</v>
+        <v>2.8</v>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:53</t>
+          <t>20/09/2023 20:52</t>
         </is>
       </c>
       <c r="R63" t="n">
-        <v>3.05</v>
+        <v>3</v>
       </c>
       <c r="S63" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="T63" t="n">
-        <v>3.04</v>
+        <v>2.61</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:53</t>
+          <t>20/09/2023 20:59</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-tigre/0bg4FEAA/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-banfield/UDN4fDYp/</t>
         </is>
       </c>
     </row>
@@ -6461,71 +6461,71 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Racing Club</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I66" t="n">
         <v>1</v>
       </c>
       <c r="J66" t="n">
-        <v>2.62</v>
+        <v>2.04</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="L66" t="n">
-        <v>2.35</v>
+        <v>2.18</v>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="N66" t="n">
-        <v>2.94</v>
+        <v>3.19</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="P66" t="n">
-        <v>3.13</v>
+        <v>3</v>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="R66" t="n">
-        <v>3.12</v>
+        <v>4.18</v>
       </c>
       <c r="S66" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 01:12</t>
         </is>
       </c>
       <c r="T66" t="n">
-        <v>3.47</v>
+        <v>4.13</v>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>21/09/2023 01:55</t>
+          <t>21/09/2023 01:56</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-newells-old-boys/4Wym7jIj/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-colon-santa-fe/A90iIGQi/</t>
         </is>
       </c>
     </row>
@@ -6553,71 +6553,71 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Racing Club</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="I67" t="n">
         <v>1</v>
       </c>
       <c r="J67" t="n">
-        <v>2.04</v>
+        <v>2.62</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="L67" t="n">
-        <v>2.18</v>
+        <v>2.35</v>
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="N67" t="n">
-        <v>3.19</v>
+        <v>2.94</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="P67" t="n">
-        <v>3</v>
+        <v>3.13</v>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="R67" t="n">
-        <v>4.18</v>
+        <v>3.12</v>
       </c>
       <c r="S67" t="inlineStr">
         <is>
-          <t>17/09/2023 01:12</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="T67" t="n">
-        <v>4.13</v>
+        <v>3.47</v>
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>21/09/2023 01:56</t>
+          <t>21/09/2023 01:55</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-colon-santa-fe/A90iIGQi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-newells-old-boys/4Wym7jIj/</t>
         </is>
       </c>
     </row>
@@ -9957,22 +9957,22 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Independiente</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I104" t="n">
         <v>0</v>
       </c>
       <c r="J104" t="n">
-        <v>1.84</v>
+        <v>2.85</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -9980,7 +9980,7 @@
         </is>
       </c>
       <c r="L104" t="n">
-        <v>2.1</v>
+        <v>3.4</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
@@ -9988,7 +9988,7 @@
         </is>
       </c>
       <c r="N104" t="n">
-        <v>3.42</v>
+        <v>3.01</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -9996,32 +9996,32 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>3.09</v>
+        <v>3.02</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
+          <t>08/10/2023 02:26</t>
+        </is>
+      </c>
+      <c r="R104" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>03/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T104" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="U104" t="inlineStr">
+        <is>
           <t>08/10/2023 02:29</t>
         </is>
       </c>
-      <c r="R104" t="n">
-        <v>4.38</v>
-      </c>
-      <c r="S104" t="inlineStr">
-        <is>
-          <t>03/10/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T104" t="n">
-        <v>4.26</v>
-      </c>
-      <c r="U104" t="inlineStr">
-        <is>
-          <t>08/10/2023 02:29</t>
-        </is>
-      </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-independiente/ba6Jq3IK/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-tigre/KA8nw1el/</t>
         </is>
       </c>
     </row>
@@ -10049,22 +10049,22 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Independiente</t>
         </is>
       </c>
       <c r="I105" t="n">
         <v>0</v>
       </c>
       <c r="J105" t="n">
-        <v>2.85</v>
+        <v>1.84</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
@@ -10072,7 +10072,7 @@
         </is>
       </c>
       <c r="L105" t="n">
-        <v>3.4</v>
+        <v>2.1</v>
       </c>
       <c r="M105" t="inlineStr">
         <is>
@@ -10080,7 +10080,7 @@
         </is>
       </c>
       <c r="N105" t="n">
-        <v>3.01</v>
+        <v>3.42</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -10088,15 +10088,15 @@
         </is>
       </c>
       <c r="P105" t="n">
-        <v>3.02</v>
+        <v>3.09</v>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>08/10/2023 02:26</t>
+          <t>08/10/2023 02:29</t>
         </is>
       </c>
       <c r="R105" t="n">
-        <v>2.79</v>
+        <v>4.38</v>
       </c>
       <c r="S105" t="inlineStr">
         <is>
@@ -10104,7 +10104,7 @@
         </is>
       </c>
       <c r="T105" t="n">
-        <v>2.45</v>
+        <v>4.26</v>
       </c>
       <c r="U105" t="inlineStr">
         <is>
@@ -10113,7 +10113,7 @@
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-tigre/KA8nw1el/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-independiente/ba6Jq3IK/</t>
         </is>
       </c>
     </row>
@@ -12625,22 +12625,22 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="I133" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J133" t="n">
-        <v>2.08</v>
+        <v>1.88</v>
       </c>
       <c r="K133" t="inlineStr">
         <is>
@@ -12648,15 +12648,15 @@
         </is>
       </c>
       <c r="L133" t="n">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="N133" t="n">
-        <v>3.15</v>
+        <v>3.23</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -12664,15 +12664,15 @@
         </is>
       </c>
       <c r="P133" t="n">
-        <v>3.15</v>
+        <v>3.11</v>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:26</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="R133" t="n">
-        <v>4.07</v>
+        <v>4.51</v>
       </c>
       <c r="S133" t="inlineStr">
         <is>
@@ -12680,16 +12680,16 @@
         </is>
       </c>
       <c r="T133" t="n">
-        <v>4.84</v>
+        <v>5.33</v>
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:27</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
         </is>
       </c>
     </row>
@@ -12717,22 +12717,22 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="I134" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J134" t="n">
-        <v>1.88</v>
+        <v>2.08</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>3.23</v>
+        <v>3.15</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>3.11</v>
+        <v>3.15</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:26</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>4.51</v>
+        <v>4.07</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>5.33</v>
+        <v>4.84</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:27</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
         </is>
       </c>
     </row>
@@ -16278,6 +16278,282 @@
       <c r="V172" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-velez-sarsfield/0t0VKDtD/</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E173" s="2" t="n">
+        <v>45241.9375</v>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Rosario Central</t>
+        </is>
+      </c>
+      <c r="G173" t="n">
+        <v>3</v>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>River Plate</t>
+        </is>
+      </c>
+      <c r="I173" t="n">
+        <v>1</v>
+      </c>
+      <c r="J173" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="L173" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>11/11/2023 22:28</t>
+        </is>
+      </c>
+      <c r="N173" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="O173" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="P173" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="Q173" t="inlineStr">
+        <is>
+          <t>11/11/2023 22:28</t>
+        </is>
+      </c>
+      <c r="R173" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="S173" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="T173" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="U173" t="inlineStr">
+        <is>
+          <t>11/11/2023 22:24</t>
+        </is>
+      </c>
+      <c r="V173" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-river-plate/SnhHrHYJ/</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E174" s="2" t="n">
+        <v>45242</v>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Lanus</t>
+        </is>
+      </c>
+      <c r="G174" t="n">
+        <v>0</v>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>Racing Club</t>
+        </is>
+      </c>
+      <c r="I174" t="n">
+        <v>2</v>
+      </c>
+      <c r="J174" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="L174" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>11/11/2023 23:59</t>
+        </is>
+      </c>
+      <c r="N174" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="O174" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="P174" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="Q174" t="inlineStr">
+        <is>
+          <t>11/11/2023 23:59</t>
+        </is>
+      </c>
+      <c r="R174" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="S174" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="T174" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="U174" t="inlineStr">
+        <is>
+          <t>11/11/2023 23:59</t>
+        </is>
+      </c>
+      <c r="V174" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-racing-club/UyGku3qP/</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E175" s="2" t="n">
+        <v>45242.04166666666</v>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="G175" t="n">
+        <v>1</v>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>Arsenal Sarandi</t>
+        </is>
+      </c>
+      <c r="I175" t="n">
+        <v>0</v>
+      </c>
+      <c r="J175" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="L175" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="M175" t="inlineStr">
+        <is>
+          <t>12/11/2023 00:58</t>
+        </is>
+      </c>
+      <c r="N175" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="O175" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="P175" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="Q175" t="inlineStr">
+        <is>
+          <t>12/11/2023 00:59</t>
+        </is>
+      </c>
+      <c r="R175" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="S175" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="T175" t="n">
+        <v>7.26</v>
+      </c>
+      <c r="U175" t="inlineStr">
+        <is>
+          <t>12/11/2023 00:58</t>
+        </is>
+      </c>
+      <c r="V175" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-arsenal-sarandi/6wiLsylQ/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 12-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V175"/>
+  <dimension ref="A1:V179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6093,71 +6093,71 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I62" t="n">
         <v>0</v>
       </c>
       <c r="J62" t="n">
-        <v>2.49</v>
+        <v>2.72</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="L62" t="n">
-        <v>2.67</v>
+        <v>3.41</v>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:58</t>
+          <t>20/09/2023 20:59</t>
         </is>
       </c>
       <c r="N62" t="n">
-        <v>3.2</v>
+        <v>2.92</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="P62" t="n">
-        <v>3.03</v>
+        <v>2.8</v>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:53</t>
+          <t>20/09/2023 20:52</t>
         </is>
       </c>
       <c r="R62" t="n">
-        <v>3.05</v>
+        <v>3</v>
       </c>
       <c r="S62" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="T62" t="n">
-        <v>3.04</v>
+        <v>2.61</v>
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:53</t>
+          <t>20/09/2023 20:59</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-tigre/0bg4FEAA/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-banfield/UDN4fDYp/</t>
         </is>
       </c>
     </row>
@@ -6185,71 +6185,71 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I63" t="n">
         <v>0</v>
       </c>
       <c r="J63" t="n">
-        <v>2.72</v>
+        <v>2.49</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="L63" t="n">
-        <v>3.41</v>
+        <v>2.67</v>
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:59</t>
+          <t>20/09/2023 20:58</t>
         </is>
       </c>
       <c r="N63" t="n">
-        <v>2.92</v>
+        <v>3.2</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="P63" t="n">
-        <v>2.8</v>
+        <v>3.03</v>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:52</t>
+          <t>20/09/2023 20:53</t>
         </is>
       </c>
       <c r="R63" t="n">
-        <v>3</v>
+        <v>3.05</v>
       </c>
       <c r="S63" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="T63" t="n">
-        <v>2.61</v>
+        <v>3.04</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:59</t>
+          <t>20/09/2023 20:53</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-banfield/UDN4fDYp/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-tigre/0bg4FEAA/</t>
         </is>
       </c>
     </row>
@@ -6277,71 +6277,71 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Velez Sarsfield</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>San Lorenzo</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>1.69</v>
+        <v>2.04</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="L64" t="n">
-        <v>1.74</v>
+        <v>2.29</v>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:23</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="N64" t="n">
-        <v>3.41</v>
+        <v>3.04</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="P64" t="n">
-        <v>3.4</v>
+        <v>2.85</v>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:23</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="R64" t="n">
-        <v>5.46</v>
+        <v>4.47</v>
       </c>
       <c r="S64" t="inlineStr">
         <is>
-          <t>17/09/2023 23:43</t>
+          <t>16/09/2023 21:12</t>
         </is>
       </c>
       <c r="T64" t="n">
-        <v>6</v>
+        <v>4.05</v>
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>20/09/2023 23:27</t>
+          <t>20/09/2023 23:29</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-arsenal-sarandi/OEeXCLlC/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-san-lorenzo/IZPUVZfi/</t>
         </is>
       </c>
     </row>
@@ -6369,71 +6369,71 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Velez Sarsfield</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>San Lorenzo</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J65" t="n">
-        <v>2.04</v>
+        <v>1.69</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="L65" t="n">
-        <v>2.29</v>
+        <v>1.74</v>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:23</t>
         </is>
       </c>
       <c r="N65" t="n">
-        <v>3.04</v>
+        <v>3.41</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="P65" t="n">
-        <v>2.85</v>
+        <v>3.4</v>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:23</t>
         </is>
       </c>
       <c r="R65" t="n">
-        <v>4.47</v>
+        <v>5.46</v>
       </c>
       <c r="S65" t="inlineStr">
         <is>
-          <t>16/09/2023 21:12</t>
+          <t>17/09/2023 23:43</t>
         </is>
       </c>
       <c r="T65" t="n">
-        <v>4.05</v>
+        <v>6</v>
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>20/09/2023 23:29</t>
+          <t>20/09/2023 23:27</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-san-lorenzo/IZPUVZfi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-arsenal-sarandi/OEeXCLlC/</t>
         </is>
       </c>
     </row>
@@ -7749,34 +7749,34 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="I80" t="n">
         <v>0</v>
       </c>
       <c r="J80" t="n">
-        <v>2.37</v>
+        <v>2.64</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>3.16</v>
+        <v>2.59</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="N80" t="n">
@@ -7784,11 +7784,11 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="P80" t="n">
-        <v>2.72</v>
+        <v>2.77</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
@@ -7796,24 +7796,24 @@
         </is>
       </c>
       <c r="R80" t="n">
-        <v>3.51</v>
+        <v>2.9</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="T80" t="n">
-        <v>2.86</v>
+        <v>3.5</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
         </is>
       </c>
     </row>
@@ -7841,34 +7841,34 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="I81" t="n">
         <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>2.64</v>
+        <v>2.37</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>2.59</v>
+        <v>3.16</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="N81" t="n">
@@ -7876,11 +7876,11 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="P81" t="n">
-        <v>2.77</v>
+        <v>2.72</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
@@ -7888,24 +7888,24 @@
         </is>
       </c>
       <c r="R81" t="n">
-        <v>2.9</v>
+        <v>3.51</v>
       </c>
       <c r="S81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="T81" t="n">
-        <v>3.5</v>
+        <v>2.86</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
         </is>
       </c>
     </row>
@@ -8117,30 +8117,30 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="I84" t="n">
         <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1.74</v>
+        <v>1.52</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="L84" t="n">
-        <v>1.72</v>
+        <v>1.67</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
@@ -8148,15 +8148,15 @@
         </is>
       </c>
       <c r="N84" t="n">
-        <v>3.47</v>
+        <v>4.1</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.54</v>
+        <v>3.69</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
@@ -8164,15 +8164,15 @@
         </is>
       </c>
       <c r="R84" t="n">
-        <v>5.5</v>
+        <v>6.9</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="T84" t="n">
-        <v>5.8</v>
+        <v>5.96</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
         </is>
       </c>
     </row>
@@ -8209,30 +8209,30 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I85" t="n">
         <v>0</v>
       </c>
       <c r="J85" t="n">
-        <v>1.52</v>
+        <v>1.74</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="L85" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
@@ -8240,15 +8240,15 @@
         </is>
       </c>
       <c r="N85" t="n">
-        <v>4.1</v>
+        <v>3.47</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.69</v>
+        <v>3.54</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
@@ -8256,15 +8256,15 @@
         </is>
       </c>
       <c r="R85" t="n">
-        <v>6.9</v>
+        <v>5.5</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="T85" t="n">
-        <v>5.96</v>
+        <v>5.8</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
@@ -8273,7 +8273,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,63 +9781,63 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J102" t="n">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>2.17</v>
+        <v>1.9</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.37</v>
+        <v>3.58</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.06</v>
+        <v>3.47</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>4.33</v>
+        <v>4.7</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>4.04</v>
+        <v>4.55</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -9873,63 +9873,63 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J103" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>1.9</v>
+        <v>2.17</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.58</v>
+        <v>3.37</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.47</v>
+        <v>3.06</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>4.7</v>
+        <v>4.33</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4.55</v>
+        <v>4.04</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
         </is>
       </c>
     </row>
@@ -12901,7 +12901,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -12909,63 +12909,63 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J136" t="n">
-        <v>2.74</v>
+        <v>1.94</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="L136" t="n">
-        <v>2.55</v>
+        <v>1.89</v>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="N136" t="n">
-        <v>2.98</v>
+        <v>3.2</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="P136" t="n">
-        <v>3.06</v>
+        <v>3.14</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="R136" t="n">
-        <v>2.78</v>
+        <v>4.62</v>
       </c>
       <c r="S136" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="T136" t="n">
-        <v>3.18</v>
+        <v>5.29</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
         </is>
       </c>
     </row>
@@ -12993,7 +12993,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G137" t="n">
@@ -13001,63 +13001,63 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J137" t="n">
-        <v>1.94</v>
+        <v>2.74</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="L137" t="n">
-        <v>1.89</v>
+        <v>2.55</v>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="N137" t="n">
-        <v>3.2</v>
+        <v>2.98</v>
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="P137" t="n">
-        <v>3.14</v>
+        <v>3.06</v>
       </c>
       <c r="Q137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="R137" t="n">
-        <v>4.62</v>
+        <v>2.78</v>
       </c>
       <c r="S137" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="T137" t="n">
-        <v>5.29</v>
+        <v>3.18</v>
       </c>
       <c r="U137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
         </is>
       </c>
     </row>
@@ -16554,6 +16554,374 @@
       <c r="V175" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-arsenal-sarandi/6wiLsylQ/</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E176" s="2" t="n">
+        <v>45242.77083333334</v>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>Colon Santa Fe</t>
+        </is>
+      </c>
+      <c r="G176" t="n">
+        <v>3</v>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>Talleres Cordoba</t>
+        </is>
+      </c>
+      <c r="I176" t="n">
+        <v>0</v>
+      </c>
+      <c r="J176" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="L176" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="M176" t="inlineStr">
+        <is>
+          <t>12/11/2023 18:21</t>
+        </is>
+      </c>
+      <c r="N176" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="O176" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="P176" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="Q176" t="inlineStr">
+        <is>
+          <t>12/11/2023 18:21</t>
+        </is>
+      </c>
+      <c r="R176" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="S176" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="T176" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="U176" t="inlineStr">
+        <is>
+          <t>12/11/2023 18:21</t>
+        </is>
+      </c>
+      <c r="V176" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-talleres-cordoba/KpXeyZQg/</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E177" s="2" t="n">
+        <v>45242.77083333334</v>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>Defensa y Justicia</t>
+        </is>
+      </c>
+      <c r="G177" t="n">
+        <v>0</v>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="I177" t="n">
+        <v>1</v>
+      </c>
+      <c r="J177" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:13</t>
+        </is>
+      </c>
+      <c r="L177" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="M177" t="inlineStr">
+        <is>
+          <t>12/11/2023 18:24</t>
+        </is>
+      </c>
+      <c r="N177" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="O177" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:13</t>
+        </is>
+      </c>
+      <c r="P177" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="Q177" t="inlineStr">
+        <is>
+          <t>12/11/2023 18:24</t>
+        </is>
+      </c>
+      <c r="R177" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="S177" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:13</t>
+        </is>
+      </c>
+      <c r="T177" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="U177" t="inlineStr">
+        <is>
+          <t>12/11/2023 18:24</t>
+        </is>
+      </c>
+      <c r="V177" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-san-lorenzo/C0o5XjQI/</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E178" s="2" t="n">
+        <v>45242.86458333334</v>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>Boca Juniors</t>
+        </is>
+      </c>
+      <c r="G178" t="n">
+        <v>1</v>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>Newells Old Boys</t>
+        </is>
+      </c>
+      <c r="I178" t="n">
+        <v>0</v>
+      </c>
+      <c r="J178" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L178" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="M178" t="inlineStr">
+        <is>
+          <t>12/11/2023 20:41</t>
+        </is>
+      </c>
+      <c r="N178" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="O178" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P178" t="n">
+        <v>3.03</v>
+      </c>
+      <c r="Q178" t="inlineStr">
+        <is>
+          <t>12/11/2023 20:41</t>
+        </is>
+      </c>
+      <c r="R178" t="n">
+        <v>4.24</v>
+      </c>
+      <c r="S178" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T178" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="U178" t="inlineStr">
+        <is>
+          <t>12/11/2023 20:41</t>
+        </is>
+      </c>
+      <c r="V178" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/boca-juniors-newells-old-boys/Iwn1YWAC/</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E179" s="2" t="n">
+        <v>45242.86458333334</v>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>Tigre</t>
+        </is>
+      </c>
+      <c r="G179" t="n">
+        <v>1</v>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>Platense</t>
+        </is>
+      </c>
+      <c r="I179" t="n">
+        <v>1</v>
+      </c>
+      <c r="J179" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="L179" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="M179" t="inlineStr">
+        <is>
+          <t>12/11/2023 20:43</t>
+        </is>
+      </c>
+      <c r="N179" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O179" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="P179" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="Q179" t="inlineStr">
+        <is>
+          <t>12/11/2023 20:40</t>
+        </is>
+      </c>
+      <c r="R179" t="n">
+        <v>4.31</v>
+      </c>
+      <c r="S179" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="T179" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="U179" t="inlineStr">
+        <is>
+          <t>12/11/2023 20:43</t>
+        </is>
+      </c>
+      <c r="V179" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/tigre-platense/byWazgt0/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 13-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V179"/>
+  <dimension ref="A1:V181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7749,34 +7749,34 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="I80" t="n">
         <v>0</v>
       </c>
       <c r="J80" t="n">
-        <v>2.64</v>
+        <v>2.37</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>2.59</v>
+        <v>3.16</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="N80" t="n">
@@ -7784,11 +7784,11 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="P80" t="n">
-        <v>2.77</v>
+        <v>2.72</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
@@ -7796,24 +7796,24 @@
         </is>
       </c>
       <c r="R80" t="n">
-        <v>2.9</v>
+        <v>3.51</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="T80" t="n">
-        <v>3.5</v>
+        <v>2.86</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
         </is>
       </c>
     </row>
@@ -7841,34 +7841,34 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="I81" t="n">
         <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>2.37</v>
+        <v>2.64</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>3.16</v>
+        <v>2.59</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="N81" t="n">
@@ -7876,11 +7876,11 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="P81" t="n">
-        <v>2.72</v>
+        <v>2.77</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
@@ -7888,24 +7888,24 @@
         </is>
       </c>
       <c r="R81" t="n">
-        <v>3.51</v>
+        <v>2.9</v>
       </c>
       <c r="S81" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="T81" t="n">
-        <v>2.86</v>
+        <v>3.5</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
         </is>
       </c>
     </row>
@@ -7933,62 +7933,62 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Racing Club</t>
         </is>
       </c>
       <c r="I82" t="n">
         <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>3.03</v>
+        <v>2.34</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="L82" t="n">
-        <v>2.95</v>
+        <v>2.29</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>25/09/2023 23:25</t>
+          <t>25/09/2023 23:29</t>
         </is>
       </c>
       <c r="N82" t="n">
-        <v>3.09</v>
+        <v>3.2</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="P82" t="n">
-        <v>3.16</v>
+        <v>3.36</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>25/09/2023 23:20</t>
+          <t>25/09/2023 23:29</t>
         </is>
       </c>
       <c r="R82" t="n">
-        <v>2.46</v>
+        <v>3.3</v>
       </c>
       <c r="S82" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="T82" t="n">
-        <v>2.64</v>
+        <v>3.35</v>
       </c>
       <c r="U82" t="inlineStr">
         <is>
@@ -7997,7 +7997,7 @@
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-argentinos-jrs/0IHoSifG/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-racing-club/8OvDrDvc/</t>
         </is>
       </c>
     </row>
@@ -8025,71 +8025,71 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Racing Club</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I83" t="n">
         <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>2.34</v>
+        <v>3.03</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>24/09/2023 05:42</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>2.29</v>
+        <v>2.95</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
+          <t>25/09/2023 23:25</t>
+        </is>
+      </c>
+      <c r="N83" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>21/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P83" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>25/09/2023 23:20</t>
+        </is>
+      </c>
+      <c r="R83" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>21/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T83" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
           <t>25/09/2023 23:29</t>
         </is>
       </c>
-      <c r="N83" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>24/09/2023 05:42</t>
-        </is>
-      </c>
-      <c r="P83" t="n">
-        <v>3.36</v>
-      </c>
-      <c r="Q83" t="inlineStr">
-        <is>
-          <t>25/09/2023 23:29</t>
-        </is>
-      </c>
-      <c r="R83" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="S83" t="inlineStr">
-        <is>
-          <t>24/09/2023 05:42</t>
-        </is>
-      </c>
-      <c r="T83" t="n">
-        <v>3.35</v>
-      </c>
-      <c r="U83" t="inlineStr">
-        <is>
-          <t>25/09/2023 23:29</t>
-        </is>
-      </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-racing-club/8OvDrDvc/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-argentinos-jrs/0IHoSifG/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,63 +9781,63 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J102" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>1.9</v>
+        <v>2.17</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.58</v>
+        <v>3.37</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.47</v>
+        <v>3.06</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>4.7</v>
+        <v>4.33</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>4.55</v>
+        <v>4.04</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -9873,63 +9873,63 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J103" t="n">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>2.17</v>
+        <v>1.9</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.37</v>
+        <v>3.58</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.06</v>
+        <v>3.47</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>4.33</v>
+        <v>4.7</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4.04</v>
+        <v>4.55</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
         </is>
       </c>
     </row>
@@ -9957,22 +9957,22 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Independiente</t>
         </is>
       </c>
       <c r="I104" t="n">
         <v>0</v>
       </c>
       <c r="J104" t="n">
-        <v>2.85</v>
+        <v>1.84</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -9980,7 +9980,7 @@
         </is>
       </c>
       <c r="L104" t="n">
-        <v>3.4</v>
+        <v>2.1</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
@@ -9988,7 +9988,7 @@
         </is>
       </c>
       <c r="N104" t="n">
-        <v>3.01</v>
+        <v>3.42</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -9996,15 +9996,15 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>3.02</v>
+        <v>3.09</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>08/10/2023 02:26</t>
+          <t>08/10/2023 02:29</t>
         </is>
       </c>
       <c r="R104" t="n">
-        <v>2.79</v>
+        <v>4.38</v>
       </c>
       <c r="S104" t="inlineStr">
         <is>
@@ -10012,7 +10012,7 @@
         </is>
       </c>
       <c r="T104" t="n">
-        <v>2.45</v>
+        <v>4.26</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
@@ -10021,7 +10021,7 @@
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-tigre/KA8nw1el/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-independiente/ba6Jq3IK/</t>
         </is>
       </c>
     </row>
@@ -10049,22 +10049,22 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="G105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Independiente</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I105" t="n">
         <v>0</v>
       </c>
       <c r="J105" t="n">
-        <v>1.84</v>
+        <v>2.85</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
@@ -10072,7 +10072,7 @@
         </is>
       </c>
       <c r="L105" t="n">
-        <v>2.1</v>
+        <v>3.4</v>
       </c>
       <c r="M105" t="inlineStr">
         <is>
@@ -10080,7 +10080,7 @@
         </is>
       </c>
       <c r="N105" t="n">
-        <v>3.42</v>
+        <v>3.01</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -10088,32 +10088,32 @@
         </is>
       </c>
       <c r="P105" t="n">
-        <v>3.09</v>
+        <v>3.02</v>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
+          <t>08/10/2023 02:26</t>
+        </is>
+      </c>
+      <c r="R105" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>03/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T105" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="U105" t="inlineStr">
+        <is>
           <t>08/10/2023 02:29</t>
         </is>
       </c>
-      <c r="R105" t="n">
-        <v>4.38</v>
-      </c>
-      <c r="S105" t="inlineStr">
-        <is>
-          <t>03/10/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T105" t="n">
-        <v>4.26</v>
-      </c>
-      <c r="U105" t="inlineStr">
-        <is>
-          <t>08/10/2023 02:29</t>
-        </is>
-      </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-independiente/ba6Jq3IK/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-tigre/KA8nw1el/</t>
         </is>
       </c>
     </row>
@@ -11889,7 +11889,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G125" t="n">
@@ -11897,14 +11897,14 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I125" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J125" t="n">
-        <v>2.03</v>
+        <v>1.43</v>
       </c>
       <c r="K125" t="inlineStr">
         <is>
@@ -11912,15 +11912,15 @@
         </is>
       </c>
       <c r="L125" t="n">
-        <v>2.04</v>
+        <v>1.48</v>
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:58</t>
+          <t>20/10/2023 23:52</t>
         </is>
       </c>
       <c r="N125" t="n">
-        <v>3.07</v>
+        <v>4.42</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -11928,15 +11928,15 @@
         </is>
       </c>
       <c r="P125" t="n">
-        <v>2.89</v>
+        <v>4.33</v>
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:56</t>
+          <t>20/10/2023 23:59</t>
         </is>
       </c>
       <c r="R125" t="n">
-        <v>4.41</v>
+        <v>6.91</v>
       </c>
       <c r="S125" t="inlineStr">
         <is>
@@ -11944,16 +11944,16 @@
         </is>
       </c>
       <c r="T125" t="n">
-        <v>5.06</v>
+        <v>7.59</v>
       </c>
       <c r="U125" t="inlineStr">
         <is>
-          <t>20/10/2023 23:58</t>
+          <t>20/10/2023 23:52</t>
         </is>
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-instituto/KOmLi0As/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-arsenal-sarandi/l4uxlI96/</t>
         </is>
       </c>
     </row>
@@ -11981,7 +11981,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G126" t="n">
@@ -11989,14 +11989,14 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I126" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J126" t="n">
-        <v>1.43</v>
+        <v>2.03</v>
       </c>
       <c r="K126" t="inlineStr">
         <is>
@@ -12004,15 +12004,15 @@
         </is>
       </c>
       <c r="L126" t="n">
-        <v>1.48</v>
+        <v>2.04</v>
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:52</t>
+          <t>20/10/2023 23:58</t>
         </is>
       </c>
       <c r="N126" t="n">
-        <v>4.42</v>
+        <v>3.07</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -12020,15 +12020,15 @@
         </is>
       </c>
       <c r="P126" t="n">
-        <v>4.33</v>
+        <v>2.89</v>
       </c>
       <c r="Q126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:59</t>
+          <t>20/10/2023 23:56</t>
         </is>
       </c>
       <c r="R126" t="n">
-        <v>6.91</v>
+        <v>4.41</v>
       </c>
       <c r="S126" t="inlineStr">
         <is>
@@ -12036,16 +12036,16 @@
         </is>
       </c>
       <c r="T126" t="n">
-        <v>7.59</v>
+        <v>5.06</v>
       </c>
       <c r="U126" t="inlineStr">
         <is>
-          <t>20/10/2023 23:52</t>
+          <t>20/10/2023 23:58</t>
         </is>
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-arsenal-sarandi/l4uxlI96/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-instituto/KOmLi0As/</t>
         </is>
       </c>
     </row>
@@ -16922,6 +16922,190 @@
       <c r="V179" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/tigre-platense/byWazgt0/</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E180" s="2" t="n">
+        <v>45242.95833333334</v>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>Belgrano</t>
+        </is>
+      </c>
+      <c r="G180" t="n">
+        <v>4</v>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>Union de Santa Fe</t>
+        </is>
+      </c>
+      <c r="I180" t="n">
+        <v>1</v>
+      </c>
+      <c r="J180" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="L180" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="M180" t="inlineStr">
+        <is>
+          <t>12/11/2023 22:59</t>
+        </is>
+      </c>
+      <c r="N180" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O180" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="P180" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="Q180" t="inlineStr">
+        <is>
+          <t>12/11/2023 22:52</t>
+        </is>
+      </c>
+      <c r="R180" t="n">
+        <v>4.31</v>
+      </c>
+      <c r="S180" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="T180" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="U180" t="inlineStr">
+        <is>
+          <t>12/11/2023 22:59</t>
+        </is>
+      </c>
+      <c r="V180" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-union-de-santa-fe/Wp2HzNit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E181" s="2" t="n">
+        <v>45242.95833333334</v>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>Independiente</t>
+        </is>
+      </c>
+      <c r="G181" t="n">
+        <v>0</v>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>Banfield</t>
+        </is>
+      </c>
+      <c r="I181" t="n">
+        <v>0</v>
+      </c>
+      <c r="J181" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="L181" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="M181" t="inlineStr">
+        <is>
+          <t>12/11/2023 22:52</t>
+        </is>
+      </c>
+      <c r="N181" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="O181" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="P181" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="Q181" t="inlineStr">
+        <is>
+          <t>12/11/2023 22:52</t>
+        </is>
+      </c>
+      <c r="R181" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="S181" t="inlineStr">
+        <is>
+          <t>08/11/2023 14:42</t>
+        </is>
+      </c>
+      <c r="T181" t="n">
+        <v>5.17</v>
+      </c>
+      <c r="U181" t="inlineStr">
+        <is>
+          <t>12/11/2023 22:52</t>
+        </is>
+      </c>
+      <c r="V181" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/independiente-banfield/QNXixFBm/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 13-11-2023 22:16
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V181"/>
+  <dimension ref="A1:V182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7749,34 +7749,34 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="I80" t="n">
         <v>0</v>
       </c>
       <c r="J80" t="n">
-        <v>2.37</v>
+        <v>2.64</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>3.16</v>
+        <v>2.59</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="N80" t="n">
@@ -7784,11 +7784,11 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="P80" t="n">
-        <v>2.72</v>
+        <v>2.77</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
@@ -7796,24 +7796,24 @@
         </is>
       </c>
       <c r="R80" t="n">
-        <v>3.51</v>
+        <v>2.9</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="T80" t="n">
-        <v>2.86</v>
+        <v>3.5</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
         </is>
       </c>
     </row>
@@ -7841,34 +7841,34 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="I81" t="n">
         <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>2.64</v>
+        <v>2.37</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>2.59</v>
+        <v>3.16</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="N81" t="n">
@@ -7876,11 +7876,11 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="P81" t="n">
-        <v>2.77</v>
+        <v>2.72</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
@@ -7888,24 +7888,24 @@
         </is>
       </c>
       <c r="R81" t="n">
-        <v>2.9</v>
+        <v>3.51</v>
       </c>
       <c r="S81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="T81" t="n">
-        <v>3.5</v>
+        <v>2.86</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
         </is>
       </c>
     </row>
@@ -7933,71 +7933,71 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Racing Club</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I82" t="n">
         <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>2.34</v>
+        <v>3.03</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>24/09/2023 05:42</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="L82" t="n">
-        <v>2.29</v>
+        <v>2.95</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
+          <t>25/09/2023 23:25</t>
+        </is>
+      </c>
+      <c r="N82" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>21/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P82" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>25/09/2023 23:20</t>
+        </is>
+      </c>
+      <c r="R82" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>21/09/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T82" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
           <t>25/09/2023 23:29</t>
         </is>
       </c>
-      <c r="N82" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>24/09/2023 05:42</t>
-        </is>
-      </c>
-      <c r="P82" t="n">
-        <v>3.36</v>
-      </c>
-      <c r="Q82" t="inlineStr">
-        <is>
-          <t>25/09/2023 23:29</t>
-        </is>
-      </c>
-      <c r="R82" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="S82" t="inlineStr">
-        <is>
-          <t>24/09/2023 05:42</t>
-        </is>
-      </c>
-      <c r="T82" t="n">
-        <v>3.35</v>
-      </c>
-      <c r="U82" t="inlineStr">
-        <is>
-          <t>25/09/2023 23:29</t>
-        </is>
-      </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-racing-club/8OvDrDvc/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-argentinos-jrs/0IHoSifG/</t>
         </is>
       </c>
     </row>
@@ -8025,62 +8025,62 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Racing Club</t>
         </is>
       </c>
       <c r="I83" t="n">
         <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>3.03</v>
+        <v>2.34</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>2.95</v>
+        <v>2.29</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>25/09/2023 23:25</t>
+          <t>25/09/2023 23:29</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>3.09</v>
+        <v>3.2</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="P83" t="n">
-        <v>3.16</v>
+        <v>3.36</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>25/09/2023 23:20</t>
+          <t>25/09/2023 23:29</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>2.46</v>
+        <v>3.3</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>24/09/2023 05:42</t>
         </is>
       </c>
       <c r="T83" t="n">
-        <v>2.64</v>
+        <v>3.35</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
@@ -8089,7 +8089,7 @@
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-argentinos-jrs/0IHoSifG/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-racing-club/8OvDrDvc/</t>
         </is>
       </c>
     </row>
@@ -8117,30 +8117,30 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I84" t="n">
         <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1.52</v>
+        <v>1.74</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="L84" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
@@ -8148,15 +8148,15 @@
         </is>
       </c>
       <c r="N84" t="n">
-        <v>4.1</v>
+        <v>3.47</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.69</v>
+        <v>3.54</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
@@ -8164,15 +8164,15 @@
         </is>
       </c>
       <c r="R84" t="n">
-        <v>6.9</v>
+        <v>5.5</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="T84" t="n">
-        <v>5.96</v>
+        <v>5.8</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
         </is>
       </c>
     </row>
@@ -8209,30 +8209,30 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="I85" t="n">
         <v>0</v>
       </c>
       <c r="J85" t="n">
-        <v>1.74</v>
+        <v>1.52</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="L85" t="n">
-        <v>1.72</v>
+        <v>1.67</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
@@ -8240,15 +8240,15 @@
         </is>
       </c>
       <c r="N85" t="n">
-        <v>3.47</v>
+        <v>4.1</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.54</v>
+        <v>3.69</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
@@ -8256,15 +8256,15 @@
         </is>
       </c>
       <c r="R85" t="n">
-        <v>5.5</v>
+        <v>6.9</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="T85" t="n">
-        <v>5.8</v>
+        <v>5.96</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
@@ -8273,7 +8273,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,63 +9781,63 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J102" t="n">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>2.17</v>
+        <v>1.9</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.37</v>
+        <v>3.58</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.06</v>
+        <v>3.47</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>4.33</v>
+        <v>4.7</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>4.04</v>
+        <v>4.55</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -9873,63 +9873,63 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J103" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>1.9</v>
+        <v>2.17</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.58</v>
+        <v>3.37</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.47</v>
+        <v>3.06</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>4.7</v>
+        <v>4.33</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4.55</v>
+        <v>4.04</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
         </is>
       </c>
     </row>
@@ -10509,71 +10509,71 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G110" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J110" t="n">
-        <v>3.26</v>
+        <v>2.5</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L110" t="n">
-        <v>3.55</v>
+        <v>2.6</v>
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:59</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="N110" t="n">
-        <v>2.96</v>
+        <v>3.13</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P110" t="n">
-        <v>2.9</v>
+        <v>2.84</v>
       </c>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:58</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="R110" t="n">
-        <v>2.51</v>
+        <v>2.93</v>
       </c>
       <c r="S110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T110" t="n">
-        <v>2.46</v>
+        <v>2.91</v>
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:53</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
         </is>
       </c>
     </row>
@@ -10601,71 +10601,71 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="G111" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J111" t="n">
-        <v>2.5</v>
+        <v>3.26</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="L111" t="n">
-        <v>2.6</v>
+        <v>3.55</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:59</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>3.13</v>
+        <v>2.96</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="P111" t="n">
-        <v>2.84</v>
+        <v>2.9</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:58</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>2.93</v>
+        <v>2.51</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="T111" t="n">
-        <v>2.91</v>
+        <v>2.46</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:53</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
         </is>
       </c>
     </row>
@@ -17106,6 +17106,98 @@
       <c r="V181" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/independiente-banfield/QNXixFBm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E182" s="2" t="n">
+        <v>45243.95833333334</v>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>Sarmiento Junin</t>
+        </is>
+      </c>
+      <c r="G182" t="n">
+        <v>0</v>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="I182" t="n">
+        <v>0</v>
+      </c>
+      <c r="J182" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:11</t>
+        </is>
+      </c>
+      <c r="L182" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="M182" t="inlineStr">
+        <is>
+          <t>13/11/2023 22:57</t>
+        </is>
+      </c>
+      <c r="N182" t="n">
+        <v>3.02</v>
+      </c>
+      <c r="O182" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:11</t>
+        </is>
+      </c>
+      <c r="P182" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="Q182" t="inlineStr">
+        <is>
+          <t>13/11/2023 22:59</t>
+        </is>
+      </c>
+      <c r="R182" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="S182" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:11</t>
+        </is>
+      </c>
+      <c r="T182" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="U182" t="inlineStr">
+        <is>
+          <t>13/11/2023 22:57</t>
+        </is>
+      </c>
+      <c r="V182" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-godoy-cruz/vmmcZCe6/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 14-11-2023 08:46
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V182"/>
+  <dimension ref="A1:V183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,63 +9781,63 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J102" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>1.9</v>
+        <v>2.17</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.58</v>
+        <v>3.37</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.47</v>
+        <v>3.06</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>4.7</v>
+        <v>4.33</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>4.55</v>
+        <v>4.04</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -9873,63 +9873,63 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J103" t="n">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>2.17</v>
+        <v>1.9</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.37</v>
+        <v>3.58</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.06</v>
+        <v>3.47</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>4.33</v>
+        <v>4.7</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4.04</v>
+        <v>4.55</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
         </is>
       </c>
     </row>
@@ -10509,71 +10509,71 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="G110" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J110" t="n">
-        <v>2.5</v>
+        <v>3.26</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="L110" t="n">
-        <v>2.6</v>
+        <v>3.55</v>
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:59</t>
         </is>
       </c>
       <c r="N110" t="n">
-        <v>3.13</v>
+        <v>2.96</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="P110" t="n">
-        <v>2.84</v>
+        <v>2.9</v>
       </c>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:58</t>
         </is>
       </c>
       <c r="R110" t="n">
-        <v>2.93</v>
+        <v>2.51</v>
       </c>
       <c r="S110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="T110" t="n">
-        <v>2.91</v>
+        <v>2.46</v>
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:53</t>
         </is>
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
         </is>
       </c>
     </row>
@@ -10601,71 +10601,71 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G111" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J111" t="n">
-        <v>3.26</v>
+        <v>2.5</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L111" t="n">
-        <v>3.55</v>
+        <v>2.6</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:59</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>2.96</v>
+        <v>3.13</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P111" t="n">
-        <v>2.9</v>
+        <v>2.84</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:58</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>2.51</v>
+        <v>2.93</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T111" t="n">
-        <v>2.46</v>
+        <v>2.91</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:53</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
         </is>
       </c>
     </row>
@@ -17198,6 +17198,98 @@
       <c r="V182" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-godoy-cruz/vmmcZCe6/</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E183" s="2" t="n">
+        <v>45244.04166666666</v>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Instituto</t>
+        </is>
+      </c>
+      <c r="G183" t="n">
+        <v>0</v>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>Barracas Central</t>
+        </is>
+      </c>
+      <c r="I183" t="n">
+        <v>0</v>
+      </c>
+      <c r="J183" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:11</t>
+        </is>
+      </c>
+      <c r="L183" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="M183" t="inlineStr">
+        <is>
+          <t>14/11/2023 00:34</t>
+        </is>
+      </c>
+      <c r="N183" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="O183" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:11</t>
+        </is>
+      </c>
+      <c r="P183" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="Q183" t="inlineStr">
+        <is>
+          <t>14/11/2023 00:33</t>
+        </is>
+      </c>
+      <c r="R183" t="n">
+        <v>5.77</v>
+      </c>
+      <c r="S183" t="inlineStr">
+        <is>
+          <t>07/11/2023 05:11</t>
+        </is>
+      </c>
+      <c r="T183" t="n">
+        <v>6.16</v>
+      </c>
+      <c r="U183" t="inlineStr">
+        <is>
+          <t>14/11/2023 00:48</t>
+        </is>
+      </c>
+      <c r="V183" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-barracas-central/vXbZJXeJ/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 27-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V187"/>
+  <dimension ref="A1:V192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2413,71 +2413,71 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>1.87</v>
+        <v>2.61</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>1.85</v>
+        <v>2.08</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:27</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.32</v>
+        <v>3.05</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.44</v>
+        <v>3.11</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:22</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>4.39</v>
+        <v>2.86</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="T22" t="n">
-        <v>4.87</v>
+        <v>4.32</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:27</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-central-cordoba-santiago-del-estero/6LNbsUbR/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-defensa-y-justicia/8U9Qxl7r/</t>
         </is>
       </c>
     </row>
@@ -2505,71 +2505,71 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>2.61</v>
+        <v>1.87</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>2.08</v>
+        <v>1.85</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:27</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>3.05</v>
+        <v>3.32</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.11</v>
+        <v>3.44</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:22</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>2.86</v>
+        <v>4.39</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="T23" t="n">
-        <v>4.32</v>
+        <v>4.87</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:27</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-defensa-y-justicia/8U9Qxl7r/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-central-cordoba-santiago-del-estero/6LNbsUbR/</t>
         </is>
       </c>
     </row>
@@ -3333,22 +3333,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I32" t="n">
         <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>2.74</v>
+        <v>1.98</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -3356,15 +3356,15 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>2.85</v>
+        <v>2.12</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>2.8</v>
+        <v>3.19</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3372,15 +3372,15 @@
         </is>
       </c>
       <c r="P32" t="n">
-        <v>2.67</v>
+        <v>2.93</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>3.12</v>
+        <v>4.44</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
@@ -3388,16 +3388,16 @@
         </is>
       </c>
       <c r="T32" t="n">
-        <v>3.25</v>
+        <v>4.54</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>02/09/2023 23:51</t>
+          <t>02/09/2023 23:56</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-newells-old-boys/plSOG3km/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-colon-santa-fe/xr5c0r56/</t>
         </is>
       </c>
     </row>
@@ -3425,22 +3425,22 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="I33" t="n">
         <v>1</v>
       </c>
       <c r="J33" t="n">
-        <v>1.98</v>
+        <v>2.74</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -3448,15 +3448,15 @@
         </is>
       </c>
       <c r="L33" t="n">
-        <v>2.12</v>
+        <v>2.85</v>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="N33" t="n">
-        <v>3.19</v>
+        <v>2.8</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -3464,15 +3464,15 @@
         </is>
       </c>
       <c r="P33" t="n">
-        <v>2.93</v>
+        <v>2.67</v>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="R33" t="n">
-        <v>4.44</v>
+        <v>3.12</v>
       </c>
       <c r="S33" t="inlineStr">
         <is>
@@ -3480,16 +3480,16 @@
         </is>
       </c>
       <c r="T33" t="n">
-        <v>4.54</v>
+        <v>3.25</v>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>02/09/2023 23:56</t>
+          <t>02/09/2023 23:51</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-colon-santa-fe/xr5c0r56/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-newells-old-boys/plSOG3km/</t>
         </is>
       </c>
     </row>
@@ -3609,71 +3609,71 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I35" t="n">
         <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>1.97</v>
+        <v>2.38</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>2.41</v>
+        <v>2.45</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="N35" t="n">
-        <v>3.39</v>
+        <v>2.92</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="P35" t="n">
-        <v>3.13</v>
+        <v>2.74</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="R35" t="n">
-        <v>4.13</v>
+        <v>3.56</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>27/08/2023 21:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="T35" t="n">
-        <v>3.35</v>
+        <v>3.85</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>03/09/2023 18:59</t>
+          <t>03/09/2023 18:54</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-sarmiento-junin/nDnlN5CJ/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-banfield/Wp2k24zf/</t>
         </is>
       </c>
     </row>
@@ -3701,71 +3701,71 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>2.38</v>
+        <v>1.97</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>2.45</v>
+        <v>2.41</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="N36" t="n">
-        <v>2.92</v>
+        <v>3.39</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="P36" t="n">
-        <v>2.74</v>
+        <v>3.13</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="R36" t="n">
-        <v>3.56</v>
+        <v>4.13</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>27/08/2023 21:12</t>
         </is>
       </c>
       <c r="T36" t="n">
-        <v>3.85</v>
+        <v>3.35</v>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>03/09/2023 18:54</t>
+          <t>03/09/2023 18:59</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-banfield/Wp2k24zf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-sarmiento-junin/nDnlN5CJ/</t>
         </is>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -3801,38 +3801,38 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J37" t="n">
-        <v>2.67</v>
+        <v>1.76</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>3.38</v>
+        <v>1.75</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>03/09/2023 21:07</t>
+          <t>03/09/2023 21:13</t>
         </is>
       </c>
       <c r="N37" t="n">
-        <v>3.13</v>
+        <v>3.56</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="P37" t="n">
-        <v>3.18</v>
+        <v>3.46</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
@@ -3840,15 +3840,15 @@
         </is>
       </c>
       <c r="R37" t="n">
-        <v>2.73</v>
+        <v>5.34</v>
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="T37" t="n">
-        <v>2.36</v>
+        <v>5.63</v>
       </c>
       <c r="U37" t="inlineStr">
         <is>
@@ -3857,7 +3857,7 @@
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
         </is>
       </c>
     </row>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -3893,63 +3893,63 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>1.76</v>
+        <v>2.67</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>29/08/2023 00:12</t>
         </is>
       </c>
       <c r="L38" t="n">
-        <v>1.75</v>
+        <v>3.38</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
+          <t>03/09/2023 21:07</t>
+        </is>
+      </c>
+      <c r="N38" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P38" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="N38" t="n">
-        <v>3.56</v>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="P38" t="n">
-        <v>3.46</v>
-      </c>
-      <c r="Q38" t="inlineStr">
+      <c r="R38" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T38" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="U38" t="inlineStr">
         <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="R38" t="n">
-        <v>5.34</v>
-      </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="T38" t="n">
-        <v>5.63</v>
-      </c>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>03/09/2023 21:13</t>
-        </is>
-      </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
         </is>
       </c>
     </row>
@@ -7197,71 +7197,71 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Velez Sarsfield</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J74" t="n">
-        <v>2.27</v>
+        <v>2.13</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>20/09/2023 22:42</t>
+          <t>20/09/2023 20:12</t>
         </is>
       </c>
       <c r="L74" t="n">
-        <v>2.49</v>
+        <v>2.02</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>24/09/2023 01:59</t>
+          <t>24/09/2023 01:52</t>
         </is>
       </c>
       <c r="N74" t="n">
-        <v>2.92</v>
+        <v>3.27</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>20/09/2023 22:42</t>
+          <t>20/09/2023 20:12</t>
         </is>
       </c>
       <c r="P74" t="n">
-        <v>2.71</v>
+        <v>3.32</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>24/09/2023 01:59</t>
+          <t>24/09/2023 01:35</t>
         </is>
       </c>
       <c r="R74" t="n">
-        <v>3.84</v>
+        <v>3.5</v>
       </c>
       <c r="S74" t="inlineStr">
         <is>
-          <t>20/09/2023 22:42</t>
+          <t>20/09/2023 20:12</t>
         </is>
       </c>
       <c r="T74" t="n">
-        <v>3.81</v>
+        <v>4.23</v>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>24/09/2023 01:59</t>
+          <t>24/09/2023 01:52</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-velez-sarsfield/WxUYUgAc/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-defensa-y-justicia/MooTvVwM/</t>
         </is>
       </c>
     </row>
@@ -7289,71 +7289,71 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Velez Sarsfield</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J75" t="n">
-        <v>2.13</v>
+        <v>2.27</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>20/09/2023 20:12</t>
+          <t>20/09/2023 22:42</t>
         </is>
       </c>
       <c r="L75" t="n">
-        <v>2.02</v>
+        <v>2.49</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>24/09/2023 01:52</t>
+          <t>24/09/2023 01:59</t>
         </is>
       </c>
       <c r="N75" t="n">
-        <v>3.27</v>
+        <v>2.92</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>20/09/2023 20:12</t>
+          <t>20/09/2023 22:42</t>
         </is>
       </c>
       <c r="P75" t="n">
-        <v>3.32</v>
+        <v>2.71</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>24/09/2023 01:35</t>
+          <t>24/09/2023 01:59</t>
         </is>
       </c>
       <c r="R75" t="n">
-        <v>3.5</v>
+        <v>3.84</v>
       </c>
       <c r="S75" t="inlineStr">
         <is>
-          <t>20/09/2023 20:12</t>
+          <t>20/09/2023 22:42</t>
         </is>
       </c>
       <c r="T75" t="n">
-        <v>4.23</v>
+        <v>3.81</v>
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>24/09/2023 01:52</t>
+          <t>24/09/2023 01:59</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-defensa-y-justicia/MooTvVwM/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-velez-sarsfield/WxUYUgAc/</t>
         </is>
       </c>
     </row>
@@ -7749,34 +7749,34 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="I80" t="n">
         <v>0</v>
       </c>
       <c r="J80" t="n">
-        <v>2.37</v>
+        <v>2.64</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>3.16</v>
+        <v>2.59</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="N80" t="n">
@@ -7784,11 +7784,11 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="P80" t="n">
-        <v>2.72</v>
+        <v>2.77</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
@@ -7796,24 +7796,24 @@
         </is>
       </c>
       <c r="R80" t="n">
-        <v>3.51</v>
+        <v>2.9</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>21/09/2023 21:12</t>
+          <t>21/09/2023 22:42</t>
         </is>
       </c>
       <c r="T80" t="n">
-        <v>2.86</v>
+        <v>3.5</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>25/09/2023 20:58</t>
+          <t>25/09/2023 20:59</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
         </is>
       </c>
     </row>
@@ -7841,34 +7841,34 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="I81" t="n">
         <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>2.64</v>
+        <v>2.37</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>2.59</v>
+        <v>3.16</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="N81" t="n">
@@ -7876,11 +7876,11 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="P81" t="n">
-        <v>2.77</v>
+        <v>2.72</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
@@ -7888,24 +7888,24 @@
         </is>
       </c>
       <c r="R81" t="n">
-        <v>2.9</v>
+        <v>3.51</v>
       </c>
       <c r="S81" t="inlineStr">
         <is>
-          <t>21/09/2023 22:42</t>
+          <t>21/09/2023 21:12</t>
         </is>
       </c>
       <c r="T81" t="n">
-        <v>3.5</v>
+        <v>2.86</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>25/09/2023 20:59</t>
+          <t>25/09/2023 20:58</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-union-de-santa-fe/nFwHsXg3/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/sarmiento-junin-ca-belgrano-de-cordoba/txwLti99/</t>
         </is>
       </c>
     </row>
@@ -8117,30 +8117,30 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="I84" t="n">
         <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1.74</v>
+        <v>1.52</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="L84" t="n">
-        <v>1.72</v>
+        <v>1.67</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
@@ -8148,15 +8148,15 @@
         </is>
       </c>
       <c r="N84" t="n">
-        <v>3.47</v>
+        <v>4.1</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.54</v>
+        <v>3.69</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
@@ -8164,15 +8164,15 @@
         </is>
       </c>
       <c r="R84" t="n">
-        <v>5.5</v>
+        <v>6.9</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="T84" t="n">
-        <v>5.8</v>
+        <v>5.96</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
         </is>
       </c>
     </row>
@@ -8209,30 +8209,30 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I85" t="n">
         <v>0</v>
       </c>
       <c r="J85" t="n">
-        <v>1.52</v>
+        <v>1.74</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="L85" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
@@ -8240,15 +8240,15 @@
         </is>
       </c>
       <c r="N85" t="n">
-        <v>4.1</v>
+        <v>3.47</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.69</v>
+        <v>3.54</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
@@ -8256,15 +8256,15 @@
         </is>
       </c>
       <c r="R85" t="n">
-        <v>6.9</v>
+        <v>5.5</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="T85" t="n">
-        <v>5.96</v>
+        <v>5.8</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
@@ -8273,7 +8273,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -9229,22 +9229,22 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>2.3</v>
+        <v>2.25</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.14</v>
+        <v>2.49</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
@@ -9252,15 +9252,15 @@
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.05</v>
+        <v>3.04</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.03</v>
+        <v>2.86</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
@@ -9268,16 +9268,16 @@
         </is>
       </c>
       <c r="R96" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>25/09/2023 22:42</t>
+        </is>
+      </c>
+      <c r="T96" t="n">
         <v>3.54</v>
       </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>26/09/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T96" t="n">
-        <v>4.22</v>
-      </c>
       <c r="U96" t="inlineStr">
         <is>
           <t>02/10/2023 23:29</t>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
         </is>
       </c>
     </row>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -9321,22 +9321,22 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>2.25</v>
+        <v>2.3</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>2.49</v>
+        <v>2.14</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
@@ -9344,15 +9344,15 @@
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.04</v>
+        <v>3.05</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>2.86</v>
+        <v>3.03</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
@@ -9360,15 +9360,15 @@
         </is>
       </c>
       <c r="R97" t="n">
-        <v>3.7</v>
+        <v>3.54</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="T97" t="n">
-        <v>3.54</v>
+        <v>4.22</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
         </is>
       </c>
     </row>
@@ -12901,7 +12901,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -12909,63 +12909,63 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J136" t="n">
-        <v>1.94</v>
+        <v>2.74</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="L136" t="n">
-        <v>1.89</v>
+        <v>2.55</v>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="N136" t="n">
-        <v>3.2</v>
+        <v>2.98</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="P136" t="n">
-        <v>3.14</v>
+        <v>3.06</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="R136" t="n">
-        <v>4.62</v>
+        <v>2.78</v>
       </c>
       <c r="S136" t="inlineStr">
         <is>
-          <t>18/10/2023 22:42</t>
+          <t>20/10/2023 23:12</t>
         </is>
       </c>
       <c r="T136" t="n">
-        <v>5.29</v>
+        <v>3.18</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>25/10/2023 23:26</t>
+          <t>25/10/2023 23:27</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
         </is>
       </c>
     </row>
@@ -12993,7 +12993,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G137" t="n">
@@ -13001,63 +13001,63 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J137" t="n">
-        <v>2.74</v>
+        <v>1.94</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="L137" t="n">
-        <v>2.55</v>
+        <v>1.89</v>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="N137" t="n">
-        <v>2.98</v>
+        <v>3.2</v>
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="P137" t="n">
-        <v>3.06</v>
+        <v>3.14</v>
       </c>
       <c r="Q137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="R137" t="n">
-        <v>2.78</v>
+        <v>4.62</v>
       </c>
       <c r="S137" t="inlineStr">
         <is>
-          <t>20/10/2023 23:12</t>
+          <t>18/10/2023 22:42</t>
         </is>
       </c>
       <c r="T137" t="n">
-        <v>3.18</v>
+        <v>5.29</v>
       </c>
       <c r="U137" t="inlineStr">
         <is>
-          <t>25/10/2023 23:27</t>
+          <t>25/10/2023 23:26</t>
         </is>
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-talleres-cordoba/jezLm9FN/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-central-cordoba-santiago-del-estero/Q71j3lFA/</t>
         </is>
       </c>
     </row>
@@ -15569,71 +15569,71 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="I165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J165" t="n">
-        <v>2.47</v>
+        <v>1.98</v>
       </c>
       <c r="K165" t="inlineStr">
         <is>
-          <t>31/10/2023 01:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="L165" t="n">
-        <v>2.37</v>
+        <v>1.87</v>
       </c>
       <c r="M165" t="inlineStr">
         <is>
-          <t>06/11/2023 22:25</t>
+          <t>06/11/2023 22:02</t>
         </is>
       </c>
       <c r="N165" t="n">
-        <v>3.12</v>
+        <v>3.2</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
-          <t>31/10/2023 01:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="P165" t="n">
-        <v>2.99</v>
+        <v>3.2</v>
       </c>
       <c r="Q165" t="inlineStr">
         <is>
-          <t>06/11/2023 22:25</t>
+          <t>06/11/2023 22:02</t>
         </is>
       </c>
       <c r="R165" t="n">
-        <v>3.15</v>
+        <v>4.43</v>
       </c>
       <c r="S165" t="inlineStr">
         <is>
-          <t>31/10/2023 01:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="T165" t="n">
-        <v>3.61</v>
+        <v>5.29</v>
       </c>
       <c r="U165" t="inlineStr">
         <is>
-          <t>06/11/2023 22:25</t>
+          <t>06/11/2023 22:02</t>
         </is>
       </c>
       <c r="V165" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-rosario-central/rmfjKtj2/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-platense/IHAQLgR6/</t>
         </is>
       </c>
     </row>
@@ -15661,71 +15661,71 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="I166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J166" t="n">
-        <v>1.98</v>
+        <v>2.47</v>
       </c>
       <c r="K166" t="inlineStr">
         <is>
-          <t>31/10/2023 23:12</t>
+          <t>31/10/2023 01:12</t>
         </is>
       </c>
       <c r="L166" t="n">
-        <v>1.87</v>
+        <v>2.37</v>
       </c>
       <c r="M166" t="inlineStr">
         <is>
-          <t>06/11/2023 22:02</t>
+          <t>06/11/2023 22:25</t>
         </is>
       </c>
       <c r="N166" t="n">
-        <v>3.2</v>
+        <v>3.12</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
-          <t>31/10/2023 23:12</t>
+          <t>31/10/2023 01:12</t>
         </is>
       </c>
       <c r="P166" t="n">
-        <v>3.2</v>
+        <v>2.99</v>
       </c>
       <c r="Q166" t="inlineStr">
         <is>
-          <t>06/11/2023 22:02</t>
+          <t>06/11/2023 22:25</t>
         </is>
       </c>
       <c r="R166" t="n">
-        <v>4.43</v>
+        <v>3.15</v>
       </c>
       <c r="S166" t="inlineStr">
         <is>
-          <t>31/10/2023 23:12</t>
+          <t>31/10/2023 01:12</t>
         </is>
       </c>
       <c r="T166" t="n">
-        <v>5.29</v>
+        <v>3.61</v>
       </c>
       <c r="U166" t="inlineStr">
         <is>
-          <t>06/11/2023 22:02</t>
+          <t>06/11/2023 22:25</t>
         </is>
       </c>
       <c r="V166" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-platense/IHAQLgR6/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-rosario-central/rmfjKtj2/</t>
         </is>
       </c>
     </row>
@@ -15753,71 +15753,71 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G167" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I167" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J167" t="n">
-        <v>2.01</v>
+        <v>2.22</v>
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t>30/10/2023 20:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="L167" t="n">
-        <v>2.23</v>
+        <v>2.57</v>
       </c>
       <c r="M167" t="inlineStr">
         <is>
-          <t>07/11/2023 00:57</t>
+          <t>07/11/2023 00:59</t>
         </is>
       </c>
       <c r="N167" t="n">
-        <v>3.25</v>
+        <v>3.05</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
-          <t>30/10/2023 20:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="P167" t="n">
-        <v>3</v>
+        <v>2.79</v>
       </c>
       <c r="Q167" t="inlineStr">
         <is>
-          <t>07/11/2023 00:57</t>
+          <t>07/11/2023 00:59</t>
         </is>
       </c>
       <c r="R167" t="n">
-        <v>4.19</v>
+        <v>3.53</v>
       </c>
       <c r="S167" t="inlineStr">
         <is>
-          <t>30/10/2023 20:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="T167" t="n">
-        <v>3.98</v>
+        <v>3.5</v>
       </c>
       <c r="U167" t="inlineStr">
         <is>
-          <t>07/11/2023 00:46</t>
+          <t>07/11/2023 00:59</t>
         </is>
       </c>
       <c r="V167" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-colon-santa-fe/CbKBROcS/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-tigre/bexwrpr9/</t>
         </is>
       </c>
     </row>
@@ -15845,71 +15845,71 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="G168" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I168" t="n">
+        <v>1</v>
+      </c>
+      <c r="J168" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="L168" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>07/11/2023 00:57</t>
+        </is>
+      </c>
+      <c r="N168" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="O168" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="P168" t="n">
         <v>3</v>
       </c>
-      <c r="J168" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="K168" t="inlineStr">
-        <is>
-          <t>31/10/2023 23:12</t>
-        </is>
-      </c>
-      <c r="L168" t="n">
-        <v>2.57</v>
-      </c>
-      <c r="M168" t="inlineStr">
-        <is>
-          <t>07/11/2023 00:59</t>
-        </is>
-      </c>
-      <c r="N168" t="n">
-        <v>3.05</v>
-      </c>
-      <c r="O168" t="inlineStr">
-        <is>
-          <t>31/10/2023 23:12</t>
-        </is>
-      </c>
-      <c r="P168" t="n">
-        <v>2.79</v>
-      </c>
       <c r="Q168" t="inlineStr">
         <is>
-          <t>07/11/2023 00:59</t>
+          <t>07/11/2023 00:57</t>
         </is>
       </c>
       <c r="R168" t="n">
-        <v>3.53</v>
+        <v>4.19</v>
       </c>
       <c r="S168" t="inlineStr">
         <is>
-          <t>31/10/2023 23:12</t>
+          <t>30/10/2023 20:12</t>
         </is>
       </c>
       <c r="T168" t="n">
-        <v>3.5</v>
+        <v>3.98</v>
       </c>
       <c r="U168" t="inlineStr">
         <is>
-          <t>07/11/2023 00:59</t>
+          <t>07/11/2023 00:46</t>
         </is>
       </c>
       <c r="V168" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-tigre/bexwrpr9/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-colon-santa-fe/CbKBROcS/</t>
         </is>
       </c>
     </row>
@@ -16581,71 +16581,71 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="G176" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>San Lorenzo</t>
         </is>
       </c>
       <c r="I176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J176" t="n">
-        <v>2.64</v>
+        <v>2.65</v>
       </c>
       <c r="K176" t="inlineStr">
         <is>
-          <t>07/11/2023 05:42</t>
+          <t>08/11/2023 23:13</t>
         </is>
       </c>
       <c r="L176" t="n">
-        <v>2.39</v>
+        <v>2.73</v>
       </c>
       <c r="M176" t="inlineStr">
         <is>
-          <t>12/11/2023 18:21</t>
+          <t>12/11/2023 18:24</t>
         </is>
       </c>
       <c r="N176" t="n">
-        <v>3.15</v>
+        <v>2.86</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
-          <t>07/11/2023 05:42</t>
+          <t>08/11/2023 23:13</t>
         </is>
       </c>
       <c r="P176" t="n">
-        <v>3.22</v>
+        <v>2.85</v>
       </c>
       <c r="Q176" t="inlineStr">
         <is>
-          <t>12/11/2023 18:21</t>
+          <t>12/11/2023 18:24</t>
         </is>
       </c>
       <c r="R176" t="n">
-        <v>2.88</v>
+        <v>3.16</v>
       </c>
       <c r="S176" t="inlineStr">
         <is>
-          <t>07/11/2023 05:42</t>
+          <t>08/11/2023 23:13</t>
         </is>
       </c>
       <c r="T176" t="n">
-        <v>3.3</v>
+        <v>3.17</v>
       </c>
       <c r="U176" t="inlineStr">
         <is>
-          <t>12/11/2023 18:21</t>
+          <t>12/11/2023 18:24</t>
         </is>
       </c>
       <c r="V176" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-talleres-cordoba/KpXeyZQg/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-san-lorenzo/C0o5XjQI/</t>
         </is>
       </c>
     </row>
@@ -16673,71 +16673,71 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="G177" t="n">
+        <v>3</v>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>Talleres Cordoba</t>
+        </is>
+      </c>
+      <c r="I177" t="n">
         <v>0</v>
       </c>
-      <c r="H177" t="inlineStr">
-        <is>
-          <t>San Lorenzo</t>
-        </is>
-      </c>
-      <c r="I177" t="n">
-        <v>1</v>
-      </c>
       <c r="J177" t="n">
-        <v>2.65</v>
+        <v>2.64</v>
       </c>
       <c r="K177" t="inlineStr">
         <is>
-          <t>08/11/2023 23:13</t>
+          <t>07/11/2023 05:42</t>
         </is>
       </c>
       <c r="L177" t="n">
-        <v>2.73</v>
+        <v>2.39</v>
       </c>
       <c r="M177" t="inlineStr">
         <is>
-          <t>12/11/2023 18:24</t>
+          <t>12/11/2023 18:21</t>
         </is>
       </c>
       <c r="N177" t="n">
-        <v>2.86</v>
+        <v>3.15</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
-          <t>08/11/2023 23:13</t>
+          <t>07/11/2023 05:42</t>
         </is>
       </c>
       <c r="P177" t="n">
-        <v>2.85</v>
+        <v>3.22</v>
       </c>
       <c r="Q177" t="inlineStr">
         <is>
-          <t>12/11/2023 18:24</t>
+          <t>12/11/2023 18:21</t>
         </is>
       </c>
       <c r="R177" t="n">
-        <v>3.16</v>
+        <v>2.88</v>
       </c>
       <c r="S177" t="inlineStr">
         <is>
-          <t>08/11/2023 23:13</t>
+          <t>07/11/2023 05:42</t>
         </is>
       </c>
       <c r="T177" t="n">
-        <v>3.17</v>
+        <v>3.3</v>
       </c>
       <c r="U177" t="inlineStr">
         <is>
-          <t>12/11/2023 18:24</t>
+          <t>12/11/2023 18:21</t>
         </is>
       </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-san-lorenzo/C0o5XjQI/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-talleres-cordoba/KpXeyZQg/</t>
         </is>
       </c>
     </row>
@@ -16765,7 +16765,7 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>Boca Juniors</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="G178" t="n">
@@ -16773,63 +16773,63 @@
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="I178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J178" t="n">
-        <v>1.96</v>
+        <v>2.03</v>
       </c>
       <c r="K178" t="inlineStr">
         <is>
-          <t>08/11/2023 23:12</t>
+          <t>07/11/2023 05:42</t>
         </is>
       </c>
       <c r="L178" t="n">
-        <v>2.06</v>
+        <v>1.93</v>
       </c>
       <c r="M178" t="inlineStr">
         <is>
-          <t>12/11/2023 20:41</t>
+          <t>12/11/2023 20:43</t>
         </is>
       </c>
       <c r="N178" t="n">
-        <v>3.14</v>
+        <v>3.13</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
-          <t>08/11/2023 23:12</t>
+          <t>07/11/2023 05:42</t>
         </is>
       </c>
       <c r="P178" t="n">
-        <v>3.03</v>
+        <v>3.21</v>
       </c>
       <c r="Q178" t="inlineStr">
         <is>
-          <t>12/11/2023 20:41</t>
+          <t>12/11/2023 20:40</t>
         </is>
       </c>
       <c r="R178" t="n">
-        <v>4.24</v>
+        <v>4.31</v>
       </c>
       <c r="S178" t="inlineStr">
         <is>
-          <t>08/11/2023 23:12</t>
+          <t>07/11/2023 05:42</t>
         </is>
       </c>
       <c r="T178" t="n">
-        <v>4.57</v>
+        <v>4.83</v>
       </c>
       <c r="U178" t="inlineStr">
         <is>
-          <t>12/11/2023 20:41</t>
+          <t>12/11/2023 20:43</t>
         </is>
       </c>
       <c r="V178" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/boca-juniors-newells-old-boys/Iwn1YWAC/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/tigre-platense/byWazgt0/</t>
         </is>
       </c>
     </row>
@@ -16857,7 +16857,7 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Boca Juniors</t>
         </is>
       </c>
       <c r="G179" t="n">
@@ -16865,63 +16865,63 @@
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="I179" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J179" t="n">
-        <v>2.03</v>
+        <v>1.96</v>
       </c>
       <c r="K179" t="inlineStr">
         <is>
-          <t>07/11/2023 05:42</t>
+          <t>08/11/2023 23:12</t>
         </is>
       </c>
       <c r="L179" t="n">
-        <v>1.93</v>
+        <v>2.06</v>
       </c>
       <c r="M179" t="inlineStr">
         <is>
-          <t>12/11/2023 20:43</t>
+          <t>12/11/2023 20:41</t>
         </is>
       </c>
       <c r="N179" t="n">
-        <v>3.13</v>
+        <v>3.14</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
-          <t>07/11/2023 05:42</t>
+          <t>08/11/2023 23:12</t>
         </is>
       </c>
       <c r="P179" t="n">
-        <v>3.21</v>
+        <v>3.03</v>
       </c>
       <c r="Q179" t="inlineStr">
         <is>
-          <t>12/11/2023 20:40</t>
+          <t>12/11/2023 20:41</t>
         </is>
       </c>
       <c r="R179" t="n">
-        <v>4.31</v>
+        <v>4.24</v>
       </c>
       <c r="S179" t="inlineStr">
         <is>
-          <t>07/11/2023 05:42</t>
+          <t>08/11/2023 23:12</t>
         </is>
       </c>
       <c r="T179" t="n">
-        <v>4.83</v>
+        <v>4.57</v>
       </c>
       <c r="U179" t="inlineStr">
         <is>
-          <t>12/11/2023 20:43</t>
+          <t>12/11/2023 20:41</t>
         </is>
       </c>
       <c r="V179" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/tigre-platense/byWazgt0/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/boca-juniors-newells-old-boys/Iwn1YWAC/</t>
         </is>
       </c>
     </row>
@@ -17317,7 +17317,7 @@
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="G184" t="n">
@@ -17325,14 +17325,14 @@
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I184" t="n">
         <v>0</v>
       </c>
       <c r="J184" t="n">
-        <v>1.97</v>
+        <v>2.47</v>
       </c>
       <c r="K184" t="inlineStr">
         <is>
@@ -17340,48 +17340,48 @@
         </is>
       </c>
       <c r="L184" t="n">
-        <v>2.28</v>
+        <v>2.11</v>
       </c>
       <c r="M184" t="inlineStr">
         <is>
+          <t>25/11/2023 21:55</t>
+        </is>
+      </c>
+      <c r="N184" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="O184" t="inlineStr">
+        <is>
+          <t>18/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P184" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="Q184" t="inlineStr">
+        <is>
           <t>25/11/2023 21:58</t>
         </is>
       </c>
-      <c r="N184" t="n">
-        <v>3.16</v>
-      </c>
-      <c r="O184" t="inlineStr">
+      <c r="R184" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="S184" t="inlineStr">
         <is>
           <t>18/11/2023 22:12</t>
         </is>
       </c>
-      <c r="P184" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="Q184" t="inlineStr">
-        <is>
-          <t>25/11/2023 21:58</t>
-        </is>
-      </c>
-      <c r="R184" t="n">
-        <v>4.56</v>
-      </c>
-      <c r="S184" t="inlineStr">
-        <is>
-          <t>18/11/2023 22:12</t>
-        </is>
-      </c>
       <c r="T184" t="n">
-        <v>4</v>
+        <v>4.28</v>
       </c>
       <c r="U184" t="inlineStr">
         <is>
-          <t>25/11/2023 21:58</t>
+          <t>25/11/2023 21:55</t>
         </is>
       </c>
       <c r="V184" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-sarmiento-junin/neXEqIzB/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-tigre/2kjkTdjU/</t>
         </is>
       </c>
     </row>
@@ -17409,58 +17409,58 @@
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Velez Sarsfield</t>
         </is>
       </c>
       <c r="G185" t="n">
+        <v>3</v>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>Colon Santa Fe</t>
+        </is>
+      </c>
+      <c r="I185" t="n">
         <v>1</v>
       </c>
-      <c r="H185" t="inlineStr">
-        <is>
-          <t>Tigre</t>
-        </is>
-      </c>
-      <c r="I185" t="n">
-        <v>0</v>
-      </c>
       <c r="J185" t="n">
-        <v>2.47</v>
+        <v>1.87</v>
       </c>
       <c r="K185" t="inlineStr">
         <is>
-          <t>18/11/2023 22:12</t>
+          <t>12/11/2023 21:12</t>
         </is>
       </c>
       <c r="L185" t="n">
-        <v>2.11</v>
+        <v>2.2</v>
       </c>
       <c r="M185" t="inlineStr">
         <is>
-          <t>25/11/2023 21:55</t>
+          <t>25/11/2023 21:51</t>
         </is>
       </c>
       <c r="N185" t="n">
-        <v>3.01</v>
+        <v>3.32</v>
       </c>
       <c r="O185" t="inlineStr">
         <is>
-          <t>18/11/2023 22:12</t>
+          <t>12/11/2023 21:12</t>
         </is>
       </c>
       <c r="P185" t="n">
-        <v>3.06</v>
+        <v>2.9</v>
       </c>
       <c r="Q185" t="inlineStr">
         <is>
-          <t>25/11/2023 21:58</t>
+          <t>25/11/2023 21:51</t>
         </is>
       </c>
       <c r="R185" t="n">
-        <v>3.28</v>
+        <v>4.81</v>
       </c>
       <c r="S185" t="inlineStr">
         <is>
-          <t>18/11/2023 22:12</t>
+          <t>12/11/2023 21:12</t>
         </is>
       </c>
       <c r="T185" t="n">
@@ -17468,12 +17468,12 @@
       </c>
       <c r="U185" t="inlineStr">
         <is>
-          <t>25/11/2023 21:55</t>
+          <t>25/11/2023 21:58</t>
         </is>
       </c>
       <c r="V185" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-tigre/2kjkTdjU/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-colon-santa-fe/0K6LZt7n/</t>
         </is>
       </c>
     </row>
@@ -17593,42 +17593,42 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>Velez Sarsfield</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G187" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I187" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J187" t="n">
-        <v>1.87</v>
+        <v>1.97</v>
       </c>
       <c r="K187" t="inlineStr">
         <is>
-          <t>12/11/2023 21:12</t>
+          <t>18/11/2023 22:12</t>
         </is>
       </c>
       <c r="L187" t="n">
-        <v>2.2</v>
+        <v>2.28</v>
       </c>
       <c r="M187" t="inlineStr">
         <is>
-          <t>25/11/2023 21:51</t>
+          <t>25/11/2023 21:58</t>
         </is>
       </c>
       <c r="N187" t="n">
-        <v>3.32</v>
+        <v>3.16</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
-          <t>12/11/2023 21:12</t>
+          <t>18/11/2023 22:12</t>
         </is>
       </c>
       <c r="P187" t="n">
@@ -17636,28 +17636,488 @@
       </c>
       <c r="Q187" t="inlineStr">
         <is>
-          <t>25/11/2023 21:51</t>
+          <t>25/11/2023 21:58</t>
         </is>
       </c>
       <c r="R187" t="n">
-        <v>4.81</v>
+        <v>4.56</v>
       </c>
       <c r="S187" t="inlineStr">
         <is>
+          <t>18/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="T187" t="n">
+        <v>4</v>
+      </c>
+      <c r="U187" t="inlineStr">
+        <is>
+          <t>25/11/2023 21:58</t>
+        </is>
+      </c>
+      <c r="V187" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-sarmiento-junin/neXEqIzB/</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E188" s="2" t="n">
+        <v>45256.91666666666</v>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>Atl. Tucuman</t>
+        </is>
+      </c>
+      <c r="G188" t="n">
+        <v>0</v>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="I188" t="n">
+        <v>2</v>
+      </c>
+      <c r="J188" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="K188" t="inlineStr">
+        <is>
           <t>12/11/2023 21:12</t>
         </is>
       </c>
-      <c r="T187" t="n">
-        <v>4.28</v>
-      </c>
-      <c r="U187" t="inlineStr">
-        <is>
-          <t>25/11/2023 21:58</t>
-        </is>
-      </c>
-      <c r="V187" t="inlineStr">
-        <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-colon-santa-fe/0K6LZt7n/</t>
+      <c r="L188" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="M188" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="N188" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="O188" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P188" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="Q188" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="R188" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="S188" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T188" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="U188" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="V188" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-huracan/Y9bYWvi5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E189" s="2" t="n">
+        <v>45256.91666666666</v>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>River Plate</t>
+        </is>
+      </c>
+      <c r="G189" t="n">
+        <v>0</v>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>Instituto</t>
+        </is>
+      </c>
+      <c r="I189" t="n">
+        <v>0</v>
+      </c>
+      <c r="J189" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>19/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="L189" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="M189" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="N189" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="O189" t="inlineStr">
+        <is>
+          <t>19/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P189" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="Q189" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="R189" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="S189" t="inlineStr">
+        <is>
+          <t>19/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="T189" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="U189" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="V189" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/river-plate-instituto/6NdtVILH/</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E190" s="2" t="n">
+        <v>45256.91666666666</v>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>Arsenal Sarandi</t>
+        </is>
+      </c>
+      <c r="G190" t="n">
+        <v>1</v>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>Rosario Central</t>
+        </is>
+      </c>
+      <c r="I190" t="n">
+        <v>2</v>
+      </c>
+      <c r="J190" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L190" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="M190" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="N190" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="O190" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P190" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="Q190" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="R190" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="S190" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T190" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="U190" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="V190" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-rosario-central/SWcxWb6B/</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E191" s="2" t="n">
+        <v>45256.91666666666</v>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Talleres Cordoba</t>
+        </is>
+      </c>
+      <c r="G191" t="n">
+        <v>3</v>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>Independiente</t>
+        </is>
+      </c>
+      <c r="I191" t="n">
+        <v>2</v>
+      </c>
+      <c r="J191" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>19/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="L191" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="M191" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="N191" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="O191" t="inlineStr">
+        <is>
+          <t>19/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P191" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="Q191" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="R191" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="S191" t="inlineStr">
+        <is>
+          <t>19/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="T191" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="U191" t="inlineStr">
+        <is>
+          <t>26/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="V191" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-independiente/vB5PY0Mh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E192" s="2" t="n">
+        <v>45257.0625</v>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="G192" t="n">
+        <v>1</v>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>Boca Juniors</t>
+        </is>
+      </c>
+      <c r="I192" t="n">
+        <v>2</v>
+      </c>
+      <c r="J192" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>20/11/2023 01:41</t>
+        </is>
+      </c>
+      <c r="L192" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="M192" t="inlineStr">
+        <is>
+          <t>27/11/2023 01:24</t>
+        </is>
+      </c>
+      <c r="N192" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="O192" t="inlineStr">
+        <is>
+          <t>20/11/2023 01:41</t>
+        </is>
+      </c>
+      <c r="P192" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="Q192" t="inlineStr">
+        <is>
+          <t>27/11/2023 01:24</t>
+        </is>
+      </c>
+      <c r="R192" t="n">
+        <v>3.91</v>
+      </c>
+      <c r="S192" t="inlineStr">
+        <is>
+          <t>20/11/2023 01:41</t>
+        </is>
+      </c>
+      <c r="T192" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="U192" t="inlineStr">
+        <is>
+          <t>27/11/2023 01:24</t>
+        </is>
+      </c>
+      <c r="V192" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-boca-juniors/84YApbL4/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 28-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V192"/>
+  <dimension ref="A1:V196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2137,71 +2137,71 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>1.74</v>
+        <v>2.19</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>1.94</v>
+        <v>2.09</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:43</t>
         </is>
       </c>
       <c r="N19" t="n">
-        <v>3.44</v>
+        <v>2.94</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="P19" t="n">
-        <v>3.23</v>
+        <v>3.01</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:43</t>
         </is>
       </c>
       <c r="R19" t="n">
-        <v>5.57</v>
+        <v>3.79</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="T19" t="n">
-        <v>4.73</v>
+        <v>4.48</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:42</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-huracan/l4ycuMBq/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-lanus/OdYgrAqL/</t>
         </is>
       </c>
     </row>
@@ -2229,71 +2229,71 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G20" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
         <v>1</v>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Lanus</t>
-        </is>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
       <c r="J20" t="n">
-        <v>2.19</v>
+        <v>1.74</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>2.09</v>
+        <v>1.94</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:43</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="N20" t="n">
-        <v>2.94</v>
+        <v>3.44</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="P20" t="n">
-        <v>3.01</v>
+        <v>3.23</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:43</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="R20" t="n">
-        <v>3.79</v>
+        <v>5.57</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="T20" t="n">
-        <v>4.48</v>
+        <v>4.73</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:42</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-lanus/OdYgrAqL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-huracan/l4ycuMBq/</t>
         </is>
       </c>
     </row>
@@ -2413,71 +2413,71 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>2.61</v>
+        <v>1.87</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>2.08</v>
+        <v>1.85</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:27</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.05</v>
+        <v>3.32</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.11</v>
+        <v>3.44</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:22</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>2.86</v>
+        <v>4.39</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="T22" t="n">
-        <v>4.32</v>
+        <v>4.87</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:27</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-defensa-y-justicia/8U9Qxl7r/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-central-cordoba-santiago-del-estero/6LNbsUbR/</t>
         </is>
       </c>
     </row>
@@ -2505,71 +2505,71 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>1.87</v>
+        <v>2.61</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>1.85</v>
+        <v>2.08</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:27</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>3.32</v>
+        <v>3.05</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.44</v>
+        <v>3.11</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:22</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>4.39</v>
+        <v>2.86</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="T23" t="n">
-        <v>4.87</v>
+        <v>4.32</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:27</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-central-cordoba-santiago-del-estero/6LNbsUbR/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-defensa-y-justicia/8U9Qxl7r/</t>
         </is>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -3801,63 +3801,63 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>1.76</v>
+        <v>2.67</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>29/08/2023 00:12</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>1.75</v>
+        <v>3.38</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
+          <t>03/09/2023 21:07</t>
+        </is>
+      </c>
+      <c r="N37" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P37" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="N37" t="n">
-        <v>3.56</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="P37" t="n">
-        <v>3.46</v>
-      </c>
-      <c r="Q37" t="inlineStr">
+      <c r="R37" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T37" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="U37" t="inlineStr">
         <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="R37" t="n">
-        <v>5.34</v>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="T37" t="n">
-        <v>5.63</v>
-      </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>03/09/2023 21:13</t>
-        </is>
-      </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
         </is>
       </c>
     </row>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -3893,38 +3893,38 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J38" t="n">
-        <v>2.67</v>
+        <v>1.76</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="L38" t="n">
-        <v>3.38</v>
+        <v>1.75</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>03/09/2023 21:07</t>
+          <t>03/09/2023 21:13</t>
         </is>
       </c>
       <c r="N38" t="n">
-        <v>3.13</v>
+        <v>3.56</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="P38" t="n">
-        <v>3.18</v>
+        <v>3.46</v>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
@@ -3932,15 +3932,15 @@
         </is>
       </c>
       <c r="R38" t="n">
-        <v>2.73</v>
+        <v>5.34</v>
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="T38" t="n">
-        <v>2.36</v>
+        <v>5.63</v>
       </c>
       <c r="U38" t="inlineStr">
         <is>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
         </is>
       </c>
     </row>
@@ -6093,71 +6093,71 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I62" t="n">
         <v>0</v>
       </c>
       <c r="J62" t="n">
-        <v>2.49</v>
+        <v>2.72</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="L62" t="n">
-        <v>2.67</v>
+        <v>3.41</v>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:58</t>
+          <t>20/09/2023 20:59</t>
         </is>
       </c>
       <c r="N62" t="n">
-        <v>3.2</v>
+        <v>2.92</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="P62" t="n">
-        <v>3.03</v>
+        <v>2.8</v>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:53</t>
+          <t>20/09/2023 20:52</t>
         </is>
       </c>
       <c r="R62" t="n">
-        <v>3.05</v>
+        <v>3</v>
       </c>
       <c r="S62" t="inlineStr">
         <is>
-          <t>15/09/2023 23:13</t>
+          <t>16/09/2023 23:12</t>
         </is>
       </c>
       <c r="T62" t="n">
-        <v>3.04</v>
+        <v>2.61</v>
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>20/09/2023 20:53</t>
+          <t>20/09/2023 20:59</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-tigre/0bg4FEAA/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-banfield/UDN4fDYp/</t>
         </is>
       </c>
     </row>
@@ -6185,71 +6185,71 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I63" t="n">
         <v>0</v>
       </c>
       <c r="J63" t="n">
-        <v>2.72</v>
+        <v>2.49</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="L63" t="n">
-        <v>3.41</v>
+        <v>2.67</v>
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:59</t>
+          <t>20/09/2023 20:58</t>
         </is>
       </c>
       <c r="N63" t="n">
-        <v>2.92</v>
+        <v>3.2</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="P63" t="n">
-        <v>2.8</v>
+        <v>3.03</v>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:52</t>
+          <t>20/09/2023 20:53</t>
         </is>
       </c>
       <c r="R63" t="n">
-        <v>3</v>
+        <v>3.05</v>
       </c>
       <c r="S63" t="inlineStr">
         <is>
-          <t>16/09/2023 23:12</t>
+          <t>15/09/2023 23:13</t>
         </is>
       </c>
       <c r="T63" t="n">
-        <v>2.61</v>
+        <v>3.04</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>20/09/2023 20:59</t>
+          <t>20/09/2023 20:53</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-banfield/UDN4fDYp/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-tigre/0bg4FEAA/</t>
         </is>
       </c>
     </row>
@@ -7197,71 +7197,71 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Velez Sarsfield</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J74" t="n">
-        <v>2.13</v>
+        <v>2.27</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>20/09/2023 20:12</t>
+          <t>20/09/2023 22:42</t>
         </is>
       </c>
       <c r="L74" t="n">
-        <v>2.02</v>
+        <v>2.49</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>24/09/2023 01:52</t>
+          <t>24/09/2023 01:59</t>
         </is>
       </c>
       <c r="N74" t="n">
-        <v>3.27</v>
+        <v>2.92</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>20/09/2023 20:12</t>
+          <t>20/09/2023 22:42</t>
         </is>
       </c>
       <c r="P74" t="n">
-        <v>3.32</v>
+        <v>2.71</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>24/09/2023 01:35</t>
+          <t>24/09/2023 01:59</t>
         </is>
       </c>
       <c r="R74" t="n">
-        <v>3.5</v>
+        <v>3.84</v>
       </c>
       <c r="S74" t="inlineStr">
         <is>
-          <t>20/09/2023 20:12</t>
+          <t>20/09/2023 22:42</t>
         </is>
       </c>
       <c r="T74" t="n">
-        <v>4.23</v>
+        <v>3.81</v>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>24/09/2023 01:52</t>
+          <t>24/09/2023 01:59</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-defensa-y-justicia/MooTvVwM/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-velez-sarsfield/WxUYUgAc/</t>
         </is>
       </c>
     </row>
@@ -7289,71 +7289,71 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Velez Sarsfield</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J75" t="n">
-        <v>2.27</v>
+        <v>2.13</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>20/09/2023 22:42</t>
+          <t>20/09/2023 20:12</t>
         </is>
       </c>
       <c r="L75" t="n">
-        <v>2.49</v>
+        <v>2.02</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>24/09/2023 01:59</t>
+          <t>24/09/2023 01:52</t>
         </is>
       </c>
       <c r="N75" t="n">
-        <v>2.92</v>
+        <v>3.27</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>20/09/2023 22:42</t>
+          <t>20/09/2023 20:12</t>
         </is>
       </c>
       <c r="P75" t="n">
-        <v>2.71</v>
+        <v>3.32</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>24/09/2023 01:59</t>
+          <t>24/09/2023 01:35</t>
         </is>
       </c>
       <c r="R75" t="n">
-        <v>3.84</v>
+        <v>3.5</v>
       </c>
       <c r="S75" t="inlineStr">
         <is>
-          <t>20/09/2023 22:42</t>
+          <t>20/09/2023 20:12</t>
         </is>
       </c>
       <c r="T75" t="n">
-        <v>3.81</v>
+        <v>4.23</v>
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>24/09/2023 01:59</t>
+          <t>24/09/2023 01:52</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-velez-sarsfield/WxUYUgAc/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-defensa-y-justicia/MooTvVwM/</t>
         </is>
       </c>
     </row>
@@ -8117,30 +8117,30 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="I84" t="n">
         <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1.52</v>
+        <v>1.74</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="L84" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
@@ -8148,15 +8148,15 @@
         </is>
       </c>
       <c r="N84" t="n">
-        <v>4.1</v>
+        <v>3.47</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.69</v>
+        <v>3.54</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
@@ -8164,15 +8164,15 @@
         </is>
       </c>
       <c r="R84" t="n">
-        <v>6.9</v>
+        <v>5.5</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
-          <t>21/09/2023 23:42</t>
+          <t>22/09/2023 01:12</t>
         </is>
       </c>
       <c r="T84" t="n">
-        <v>5.96</v>
+        <v>5.8</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
         </is>
       </c>
     </row>
@@ -8209,30 +8209,30 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="I85" t="n">
         <v>0</v>
       </c>
       <c r="J85" t="n">
-        <v>1.74</v>
+        <v>1.52</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="L85" t="n">
-        <v>1.72</v>
+        <v>1.67</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
@@ -8240,15 +8240,15 @@
         </is>
       </c>
       <c r="N85" t="n">
-        <v>3.47</v>
+        <v>4.1</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.54</v>
+        <v>3.69</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
@@ -8256,15 +8256,15 @@
         </is>
       </c>
       <c r="R85" t="n">
-        <v>5.5</v>
+        <v>6.9</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
-          <t>22/09/2023 01:12</t>
+          <t>21/09/2023 23:42</t>
         </is>
       </c>
       <c r="T85" t="n">
-        <v>5.8</v>
+        <v>5.96</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
@@ -8273,7 +8273,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-arsenal-sarandi/bgcMLkXq/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-barracas-central/v9GkRB9M/</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -9229,22 +9229,22 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>2.25</v>
+        <v>2.3</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.49</v>
+        <v>2.14</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
@@ -9252,15 +9252,15 @@
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.04</v>
+        <v>3.05</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="P96" t="n">
-        <v>2.86</v>
+        <v>3.03</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
@@ -9268,15 +9268,15 @@
         </is>
       </c>
       <c r="R96" t="n">
-        <v>3.7</v>
+        <v>3.54</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="T96" t="n">
-        <v>3.54</v>
+        <v>4.22</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
         </is>
       </c>
     </row>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -9321,22 +9321,22 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>2.3</v>
+        <v>2.25</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>2.14</v>
+        <v>2.49</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
@@ -9344,15 +9344,15 @@
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.05</v>
+        <v>3.04</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>3.03</v>
+        <v>2.86</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
@@ -9360,16 +9360,16 @@
         </is>
       </c>
       <c r="R97" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>25/09/2023 22:42</t>
+        </is>
+      </c>
+      <c r="T97" t="n">
         <v>3.54</v>
       </c>
-      <c r="S97" t="inlineStr">
-        <is>
-          <t>26/09/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T97" t="n">
-        <v>4.22</v>
-      </c>
       <c r="U97" t="inlineStr">
         <is>
           <t>02/10/2023 23:29</t>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
         </is>
       </c>
     </row>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -9413,14 +9413,14 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>1.93</v>
+        <v>3.31</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
         </is>
       </c>
       <c r="L98" t="n">
-        <v>1.91</v>
+        <v>3.28</v>
       </c>
       <c r="M98" t="inlineStr">
         <is>
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="N98" t="n">
-        <v>3.29</v>
+        <v>2.97</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -9444,7 +9444,7 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>3.2</v>
+        <v>2.93</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
@@ -9452,7 +9452,7 @@
         </is>
       </c>
       <c r="R98" t="n">
-        <v>4.52</v>
+        <v>2.47</v>
       </c>
       <c r="S98" t="inlineStr">
         <is>
@@ -9460,7 +9460,7 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>5.03</v>
+        <v>2.59</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
@@ -9469,7 +9469,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
         </is>
       </c>
     </row>
@@ -9497,7 +9497,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G99" t="n">
@@ -9505,14 +9505,14 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I99" t="n">
         <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>3.31</v>
+        <v>1.93</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -9520,7 +9520,7 @@
         </is>
       </c>
       <c r="L99" t="n">
-        <v>3.28</v>
+        <v>1.91</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
@@ -9528,7 +9528,7 @@
         </is>
       </c>
       <c r="N99" t="n">
-        <v>2.97</v>
+        <v>3.29</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -9536,7 +9536,7 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>2.93</v>
+        <v>3.2</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
@@ -9544,7 +9544,7 @@
         </is>
       </c>
       <c r="R99" t="n">
-        <v>2.47</v>
+        <v>4.52</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
@@ -9552,7 +9552,7 @@
         </is>
       </c>
       <c r="T99" t="n">
-        <v>2.59</v>
+        <v>5.03</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
@@ -9561,7 +9561,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
         </is>
       </c>
     </row>
@@ -10141,7 +10141,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="G106" t="n">
@@ -10149,14 +10149,14 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Gimnasia L.P.</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J106" t="n">
-        <v>1.93</v>
+        <v>1.96</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
@@ -10164,15 +10164,15 @@
         </is>
       </c>
       <c r="L106" t="n">
-        <v>2.08</v>
+        <v>1.88</v>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:05</t>
         </is>
       </c>
       <c r="N106" t="n">
-        <v>3.23</v>
+        <v>3.24</v>
       </c>
       <c r="O106" t="inlineStr">
         <is>
@@ -10180,15 +10180,15 @@
         </is>
       </c>
       <c r="P106" t="n">
-        <v>2.95</v>
+        <v>3.14</v>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:05</t>
         </is>
       </c>
       <c r="R106" t="n">
-        <v>4.21</v>
+        <v>4.4</v>
       </c>
       <c r="S106" t="inlineStr">
         <is>
@@ -10196,16 +10196,16 @@
         </is>
       </c>
       <c r="T106" t="n">
-        <v>4.67</v>
+        <v>5.34</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:06</t>
         </is>
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-gimnasia-l-p/xj5NrNXQ/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-sarmiento-junin/Aa1azau7/</t>
         </is>
       </c>
     </row>
@@ -10233,7 +10233,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -10241,14 +10241,14 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Gimnasia L.P.</t>
         </is>
       </c>
       <c r="I107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J107" t="n">
-        <v>1.96</v>
+        <v>1.93</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -10256,15 +10256,15 @@
         </is>
       </c>
       <c r="L107" t="n">
-        <v>1.88</v>
+        <v>2.08</v>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:05</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>3.24</v>
+        <v>3.23</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -10272,15 +10272,15 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>3.14</v>
+        <v>2.95</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:05</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="R107" t="n">
-        <v>4.4</v>
+        <v>4.21</v>
       </c>
       <c r="S107" t="inlineStr">
         <is>
@@ -10288,16 +10288,16 @@
         </is>
       </c>
       <c r="T107" t="n">
-        <v>5.34</v>
+        <v>4.67</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:06</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-sarmiento-junin/Aa1azau7/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-gimnasia-l-p/xj5NrNXQ/</t>
         </is>
       </c>
     </row>
@@ -10509,71 +10509,71 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G110" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J110" t="n">
-        <v>3.26</v>
+        <v>2.5</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L110" t="n">
-        <v>3.55</v>
+        <v>2.6</v>
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:59</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="N110" t="n">
-        <v>2.96</v>
+        <v>3.13</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P110" t="n">
-        <v>2.9</v>
+        <v>2.84</v>
       </c>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:58</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="R110" t="n">
-        <v>2.51</v>
+        <v>2.93</v>
       </c>
       <c r="S110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T110" t="n">
-        <v>2.46</v>
+        <v>2.91</v>
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:53</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
         </is>
       </c>
     </row>
@@ -10601,71 +10601,71 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="G111" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J111" t="n">
-        <v>2.5</v>
+        <v>3.26</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="L111" t="n">
-        <v>2.6</v>
+        <v>3.55</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:59</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>3.13</v>
+        <v>2.96</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="P111" t="n">
-        <v>2.84</v>
+        <v>2.9</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:58</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>2.93</v>
+        <v>2.51</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="T111" t="n">
-        <v>2.91</v>
+        <v>2.46</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:53</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
         </is>
       </c>
     </row>
@@ -12625,22 +12625,22 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="I133" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J133" t="n">
-        <v>1.88</v>
+        <v>2.08</v>
       </c>
       <c r="K133" t="inlineStr">
         <is>
@@ -12648,15 +12648,15 @@
         </is>
       </c>
       <c r="L133" t="n">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="N133" t="n">
-        <v>3.23</v>
+        <v>3.15</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -12664,15 +12664,15 @@
         </is>
       </c>
       <c r="P133" t="n">
-        <v>3.11</v>
+        <v>3.15</v>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:26</t>
         </is>
       </c>
       <c r="R133" t="n">
-        <v>4.51</v>
+        <v>4.07</v>
       </c>
       <c r="S133" t="inlineStr">
         <is>
@@ -12680,16 +12680,16 @@
         </is>
       </c>
       <c r="T133" t="n">
-        <v>5.33</v>
+        <v>4.84</v>
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:27</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
         </is>
       </c>
     </row>
@@ -12717,22 +12717,22 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="I134" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J134" t="n">
-        <v>2.08</v>
+        <v>1.88</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>3.15</v>
+        <v>3.23</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>3.15</v>
+        <v>3.11</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:26</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>4.07</v>
+        <v>4.51</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>4.84</v>
+        <v>5.33</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:27</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
         </is>
       </c>
     </row>
@@ -15753,71 +15753,71 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="G167" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I167" t="n">
+        <v>1</v>
+      </c>
+      <c r="J167" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="L167" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>07/11/2023 00:57</t>
+        </is>
+      </c>
+      <c r="N167" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="O167" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="P167" t="n">
         <v>3</v>
       </c>
-      <c r="J167" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="K167" t="inlineStr">
-        <is>
-          <t>31/10/2023 23:12</t>
-        </is>
-      </c>
-      <c r="L167" t="n">
-        <v>2.57</v>
-      </c>
-      <c r="M167" t="inlineStr">
-        <is>
-          <t>07/11/2023 00:59</t>
-        </is>
-      </c>
-      <c r="N167" t="n">
-        <v>3.05</v>
-      </c>
-      <c r="O167" t="inlineStr">
-        <is>
-          <t>31/10/2023 23:12</t>
-        </is>
-      </c>
-      <c r="P167" t="n">
-        <v>2.79</v>
-      </c>
       <c r="Q167" t="inlineStr">
         <is>
-          <t>07/11/2023 00:59</t>
+          <t>07/11/2023 00:57</t>
         </is>
       </c>
       <c r="R167" t="n">
-        <v>3.53</v>
+        <v>4.19</v>
       </c>
       <c r="S167" t="inlineStr">
         <is>
-          <t>31/10/2023 23:12</t>
+          <t>30/10/2023 20:12</t>
         </is>
       </c>
       <c r="T167" t="n">
-        <v>3.5</v>
+        <v>3.98</v>
       </c>
       <c r="U167" t="inlineStr">
         <is>
-          <t>07/11/2023 00:59</t>
+          <t>07/11/2023 00:46</t>
         </is>
       </c>
       <c r="V167" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-tigre/bexwrpr9/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-colon-santa-fe/CbKBROcS/</t>
         </is>
       </c>
     </row>
@@ -15845,71 +15845,71 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G168" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I168" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J168" t="n">
-        <v>2.01</v>
+        <v>2.22</v>
       </c>
       <c r="K168" t="inlineStr">
         <is>
-          <t>30/10/2023 20:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="L168" t="n">
-        <v>2.23</v>
+        <v>2.57</v>
       </c>
       <c r="M168" t="inlineStr">
         <is>
-          <t>07/11/2023 00:57</t>
+          <t>07/11/2023 00:59</t>
         </is>
       </c>
       <c r="N168" t="n">
-        <v>3.25</v>
+        <v>3.05</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
-          <t>30/10/2023 20:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="P168" t="n">
-        <v>3</v>
+        <v>2.79</v>
       </c>
       <c r="Q168" t="inlineStr">
         <is>
-          <t>07/11/2023 00:57</t>
+          <t>07/11/2023 00:59</t>
         </is>
       </c>
       <c r="R168" t="n">
-        <v>4.19</v>
+        <v>3.53</v>
       </c>
       <c r="S168" t="inlineStr">
         <is>
-          <t>30/10/2023 20:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="T168" t="n">
-        <v>3.98</v>
+        <v>3.5</v>
       </c>
       <c r="U168" t="inlineStr">
         <is>
-          <t>07/11/2023 00:46</t>
+          <t>07/11/2023 00:59</t>
         </is>
       </c>
       <c r="V168" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-colon-santa-fe/CbKBROcS/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-tigre/bexwrpr9/</t>
         </is>
       </c>
     </row>
@@ -16581,71 +16581,71 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="G176" t="n">
+        <v>3</v>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>Talleres Cordoba</t>
+        </is>
+      </c>
+      <c r="I176" t="n">
         <v>0</v>
       </c>
-      <c r="H176" t="inlineStr">
-        <is>
-          <t>San Lorenzo</t>
-        </is>
-      </c>
-      <c r="I176" t="n">
-        <v>1</v>
-      </c>
       <c r="J176" t="n">
-        <v>2.65</v>
+        <v>2.64</v>
       </c>
       <c r="K176" t="inlineStr">
         <is>
-          <t>08/11/2023 23:13</t>
+          <t>07/11/2023 05:42</t>
         </is>
       </c>
       <c r="L176" t="n">
-        <v>2.73</v>
+        <v>2.39</v>
       </c>
       <c r="M176" t="inlineStr">
         <is>
-          <t>12/11/2023 18:24</t>
+          <t>12/11/2023 18:21</t>
         </is>
       </c>
       <c r="N176" t="n">
-        <v>2.86</v>
+        <v>3.15</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
-          <t>08/11/2023 23:13</t>
+          <t>07/11/2023 05:42</t>
         </is>
       </c>
       <c r="P176" t="n">
-        <v>2.85</v>
+        <v>3.22</v>
       </c>
       <c r="Q176" t="inlineStr">
         <is>
-          <t>12/11/2023 18:24</t>
+          <t>12/11/2023 18:21</t>
         </is>
       </c>
       <c r="R176" t="n">
-        <v>3.16</v>
+        <v>2.88</v>
       </c>
       <c r="S176" t="inlineStr">
         <is>
-          <t>08/11/2023 23:13</t>
+          <t>07/11/2023 05:42</t>
         </is>
       </c>
       <c r="T176" t="n">
-        <v>3.17</v>
+        <v>3.3</v>
       </c>
       <c r="U176" t="inlineStr">
         <is>
-          <t>12/11/2023 18:24</t>
+          <t>12/11/2023 18:21</t>
         </is>
       </c>
       <c r="V176" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-san-lorenzo/C0o5XjQI/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-talleres-cordoba/KpXeyZQg/</t>
         </is>
       </c>
     </row>
@@ -16673,71 +16673,71 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="G177" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>San Lorenzo</t>
         </is>
       </c>
       <c r="I177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J177" t="n">
-        <v>2.64</v>
+        <v>2.65</v>
       </c>
       <c r="K177" t="inlineStr">
         <is>
-          <t>07/11/2023 05:42</t>
+          <t>08/11/2023 23:13</t>
         </is>
       </c>
       <c r="L177" t="n">
-        <v>2.39</v>
+        <v>2.73</v>
       </c>
       <c r="M177" t="inlineStr">
         <is>
-          <t>12/11/2023 18:21</t>
+          <t>12/11/2023 18:24</t>
         </is>
       </c>
       <c r="N177" t="n">
-        <v>3.15</v>
+        <v>2.86</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
-          <t>07/11/2023 05:42</t>
+          <t>08/11/2023 23:13</t>
         </is>
       </c>
       <c r="P177" t="n">
-        <v>3.22</v>
+        <v>2.85</v>
       </c>
       <c r="Q177" t="inlineStr">
         <is>
-          <t>12/11/2023 18:21</t>
+          <t>12/11/2023 18:24</t>
         </is>
       </c>
       <c r="R177" t="n">
-        <v>2.88</v>
+        <v>3.16</v>
       </c>
       <c r="S177" t="inlineStr">
         <is>
-          <t>07/11/2023 05:42</t>
+          <t>08/11/2023 23:13</t>
         </is>
       </c>
       <c r="T177" t="n">
-        <v>3.3</v>
+        <v>3.17</v>
       </c>
       <c r="U177" t="inlineStr">
         <is>
-          <t>12/11/2023 18:21</t>
+          <t>12/11/2023 18:24</t>
         </is>
       </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/colon-santa-fe-talleres-cordoba/KpXeyZQg/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/defensa-y-justicia-san-lorenzo/C0o5XjQI/</t>
         </is>
       </c>
     </row>
@@ -18118,6 +18118,374 @@
       <c r="V192" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-boca-juniors/84YApbL4/</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E193" s="2" t="n">
+        <v>45257.95833333334</v>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>Estudiantes L.P.</t>
+        </is>
+      </c>
+      <c r="G193" t="n">
+        <v>1</v>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>Lanus</t>
+        </is>
+      </c>
+      <c r="I193" t="n">
+        <v>1</v>
+      </c>
+      <c r="J193" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L193" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="M193" t="inlineStr">
+        <is>
+          <t>27/11/2023 22:58</t>
+        </is>
+      </c>
+      <c r="N193" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="O193" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P193" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="Q193" t="inlineStr">
+        <is>
+          <t>27/11/2023 22:58</t>
+        </is>
+      </c>
+      <c r="R193" t="n">
+        <v>5.02</v>
+      </c>
+      <c r="S193" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T193" t="n">
+        <v>5.37</v>
+      </c>
+      <c r="U193" t="inlineStr">
+        <is>
+          <t>27/11/2023 22:59</t>
+        </is>
+      </c>
+      <c r="V193" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-lanus/hEVbm0yn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E194" s="2" t="n">
+        <v>45257.95833333334</v>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="G194" t="n">
+        <v>2</v>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>Central Cordoba</t>
+        </is>
+      </c>
+      <c r="I194" t="n">
+        <v>0</v>
+      </c>
+      <c r="J194" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L194" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="M194" t="inlineStr">
+        <is>
+          <t>27/11/2023 22:58</t>
+        </is>
+      </c>
+      <c r="N194" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="O194" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P194" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="Q194" t="inlineStr">
+        <is>
+          <t>27/11/2023 22:58</t>
+        </is>
+      </c>
+      <c r="R194" t="n">
+        <v>5.02</v>
+      </c>
+      <c r="S194" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T194" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="U194" t="inlineStr">
+        <is>
+          <t>27/11/2023 22:58</t>
+        </is>
+      </c>
+      <c r="V194" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/san-lorenzo-central-cordoba-santiago-del-estero/zwL3nKjh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E195" s="2" t="n">
+        <v>45258.0625</v>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Racing Club</t>
+        </is>
+      </c>
+      <c r="G195" t="n">
+        <v>4</v>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>Belgrano</t>
+        </is>
+      </c>
+      <c r="I195" t="n">
+        <v>1</v>
+      </c>
+      <c r="J195" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>21/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="L195" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="M195" t="inlineStr">
+        <is>
+          <t>28/11/2023 01:22</t>
+        </is>
+      </c>
+      <c r="N195" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="O195" t="inlineStr">
+        <is>
+          <t>21/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="P195" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="Q195" t="inlineStr">
+        <is>
+          <t>28/11/2023 01:21</t>
+        </is>
+      </c>
+      <c r="R195" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="S195" t="inlineStr">
+        <is>
+          <t>21/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="T195" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="U195" t="inlineStr">
+        <is>
+          <t>28/11/2023 00:58</t>
+        </is>
+      </c>
+      <c r="V195" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-ca-belgrano-de-cordoba/vBRfltMu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E196" s="2" t="n">
+        <v>45258.0625</v>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Newells Old Boys</t>
+        </is>
+      </c>
+      <c r="G196" t="n">
+        <v>3</v>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>Defensa y Justicia</t>
+        </is>
+      </c>
+      <c r="I196" t="n">
+        <v>0</v>
+      </c>
+      <c r="J196" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L196" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="M196" t="inlineStr">
+        <is>
+          <t>28/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="N196" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="O196" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P196" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="Q196" t="inlineStr">
+        <is>
+          <t>28/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="R196" t="n">
+        <v>5</v>
+      </c>
+      <c r="S196" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T196" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="U196" t="inlineStr">
+        <is>
+          <t>28/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="V196" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-defensa-y-justicia/ETJ7ov6b/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 19-12-2023 18:56
</commit_message>
<xml_diff>
--- a/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
+++ b/2023/argentina_copa-de-la-liga-profesional_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V196"/>
+  <dimension ref="A1:V203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2137,71 +2137,71 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G19" t="n">
+        <v>2</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
         <v>1</v>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Lanus</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
       <c r="J19" t="n">
-        <v>2.19</v>
+        <v>1.74</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>2.09</v>
+        <v>1.94</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:43</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="N19" t="n">
-        <v>2.94</v>
+        <v>3.44</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="P19" t="n">
-        <v>3.01</v>
+        <v>3.23</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:43</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="R19" t="n">
-        <v>3.79</v>
+        <v>5.57</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 23:12</t>
         </is>
       </c>
       <c r="T19" t="n">
-        <v>4.48</v>
+        <v>4.73</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>26/08/2023 23:42</t>
+          <t>26/08/2023 23:50</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-lanus/OdYgrAqL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-huracan/l4ycuMBq/</t>
         </is>
       </c>
     </row>
@@ -2229,71 +2229,71 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>1.74</v>
+        <v>2.19</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>1.94</v>
+        <v>2.09</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:43</t>
         </is>
       </c>
       <c r="N20" t="n">
-        <v>3.44</v>
+        <v>2.94</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="P20" t="n">
-        <v>3.23</v>
+        <v>3.01</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:43</t>
         </is>
       </c>
       <c r="R20" t="n">
-        <v>5.57</v>
+        <v>3.79</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>21/08/2023 23:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="T20" t="n">
-        <v>4.73</v>
+        <v>4.48</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>26/08/2023 23:50</t>
+          <t>26/08/2023 23:42</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-huracan/l4ycuMBq/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-lanus/OdYgrAqL/</t>
         </is>
       </c>
     </row>
@@ -2413,71 +2413,71 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>1.87</v>
+        <v>2.61</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>1.85</v>
+        <v>2.08</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:27</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.32</v>
+        <v>3.05</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.44</v>
+        <v>3.11</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:22</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>4.39</v>
+        <v>2.86</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>22/08/2023 01:42</t>
+          <t>21/08/2023 08:12</t>
         </is>
       </c>
       <c r="T22" t="n">
-        <v>4.87</v>
+        <v>4.32</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>27/08/2023 19:26</t>
+          <t>27/08/2023 19:27</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-central-cordoba-santiago-del-estero/6LNbsUbR/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-defensa-y-justicia/8U9Qxl7r/</t>
         </is>
       </c>
     </row>
@@ -2505,71 +2505,71 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>2.61</v>
+        <v>1.87</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>2.08</v>
+        <v>1.85</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:27</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>3.05</v>
+        <v>3.32</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.11</v>
+        <v>3.44</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:22</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>2.86</v>
+        <v>4.39</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>21/08/2023 08:12</t>
+          <t>22/08/2023 01:42</t>
         </is>
       </c>
       <c r="T23" t="n">
-        <v>4.32</v>
+        <v>4.87</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>27/08/2023 19:27</t>
+          <t>27/08/2023 19:26</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-defensa-y-justicia/8U9Qxl7r/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-central-cordoba-santiago-del-estero/6LNbsUbR/</t>
         </is>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -3801,38 +3801,38 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J37" t="n">
-        <v>2.67</v>
+        <v>1.76</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>3.38</v>
+        <v>1.75</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>03/09/2023 21:07</t>
+          <t>03/09/2023 21:13</t>
         </is>
       </c>
       <c r="N37" t="n">
-        <v>3.13</v>
+        <v>3.56</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="P37" t="n">
-        <v>3.18</v>
+        <v>3.46</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
@@ -3840,15 +3840,15 @@
         </is>
       </c>
       <c r="R37" t="n">
-        <v>2.73</v>
+        <v>5.34</v>
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>29/08/2023 00:12</t>
+          <t>29/08/2023 01:42</t>
         </is>
       </c>
       <c r="T37" t="n">
-        <v>2.36</v>
+        <v>5.63</v>
       </c>
       <c r="U37" t="inlineStr">
         <is>
@@ -3857,7 +3857,7 @@
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
         </is>
       </c>
     </row>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -3893,63 +3893,63 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>1.76</v>
+        <v>2.67</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>29/08/2023 01:42</t>
+          <t>29/08/2023 00:12</t>
         </is>
       </c>
       <c r="L38" t="n">
-        <v>1.75</v>
+        <v>3.38</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
+          <t>03/09/2023 21:07</t>
+        </is>
+      </c>
+      <c r="N38" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P38" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="N38" t="n">
-        <v>3.56</v>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="P38" t="n">
-        <v>3.46</v>
-      </c>
-      <c r="Q38" t="inlineStr">
+      <c r="R38" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>29/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T38" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="U38" t="inlineStr">
         <is>
           <t>03/09/2023 21:13</t>
         </is>
       </c>
-      <c r="R38" t="n">
-        <v>5.34</v>
-      </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>29/08/2023 01:42</t>
-        </is>
-      </c>
-      <c r="T38" t="n">
-        <v>5.63</v>
-      </c>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>03/09/2023 21:13</t>
-        </is>
-      </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-atl-tucuman/hf3o3pLm/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-talleres-cordoba/Q71g1Ok0/</t>
         </is>
       </c>
     </row>
@@ -7197,71 +7197,71 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Velez Sarsfield</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J74" t="n">
-        <v>2.27</v>
+        <v>2.13</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>20/09/2023 22:42</t>
+          <t>20/09/2023 20:12</t>
         </is>
       </c>
       <c r="L74" t="n">
-        <v>2.49</v>
+        <v>2.02</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>24/09/2023 01:59</t>
+          <t>24/09/2023 01:52</t>
         </is>
       </c>
       <c r="N74" t="n">
-        <v>2.92</v>
+        <v>3.27</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>20/09/2023 22:42</t>
+          <t>20/09/2023 20:12</t>
         </is>
       </c>
       <c r="P74" t="n">
-        <v>2.71</v>
+        <v>3.32</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>24/09/2023 01:59</t>
+          <t>24/09/2023 01:35</t>
         </is>
       </c>
       <c r="R74" t="n">
-        <v>3.84</v>
+        <v>3.5</v>
       </c>
       <c r="S74" t="inlineStr">
         <is>
-          <t>20/09/2023 22:42</t>
+          <t>20/09/2023 20:12</t>
         </is>
       </c>
       <c r="T74" t="n">
-        <v>3.81</v>
+        <v>4.23</v>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>24/09/2023 01:59</t>
+          <t>24/09/2023 01:52</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-velez-sarsfield/WxUYUgAc/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-defensa-y-justicia/MooTvVwM/</t>
         </is>
       </c>
     </row>
@@ -7289,71 +7289,71 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Velez Sarsfield</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J75" t="n">
-        <v>2.13</v>
+        <v>2.27</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>20/09/2023 20:12</t>
+          <t>20/09/2023 22:42</t>
         </is>
       </c>
       <c r="L75" t="n">
-        <v>2.02</v>
+        <v>2.49</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>24/09/2023 01:52</t>
+          <t>24/09/2023 01:59</t>
         </is>
       </c>
       <c r="N75" t="n">
-        <v>3.27</v>
+        <v>2.92</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>20/09/2023 20:12</t>
+          <t>20/09/2023 22:42</t>
         </is>
       </c>
       <c r="P75" t="n">
-        <v>3.32</v>
+        <v>2.71</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>24/09/2023 01:35</t>
+          <t>24/09/2023 01:59</t>
         </is>
       </c>
       <c r="R75" t="n">
-        <v>3.5</v>
+        <v>3.84</v>
       </c>
       <c r="S75" t="inlineStr">
         <is>
-          <t>20/09/2023 20:12</t>
+          <t>20/09/2023 22:42</t>
         </is>
       </c>
       <c r="T75" t="n">
-        <v>4.23</v>
+        <v>3.81</v>
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>24/09/2023 01:52</t>
+          <t>24/09/2023 01:59</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/central-cordoba-santiago-del-estero-defensa-y-justicia/MooTvVwM/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-velez-sarsfield/WxUYUgAc/</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -9229,22 +9229,22 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>2.3</v>
+        <v>2.25</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.14</v>
+        <v>2.49</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
@@ -9252,15 +9252,15 @@
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.05</v>
+        <v>3.04</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>26/09/2023 01:12</t>
+          <t>25/09/2023 22:42</t>
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.03</v>
+        <v>2.86</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
@@ -9268,16 +9268,16 @@
         </is>
       </c>
       <c r="R96" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>25/09/2023 22:42</t>
+        </is>
+      </c>
+      <c r="T96" t="n">
         <v>3.54</v>
       </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>26/09/2023 01:12</t>
-        </is>
-      </c>
-      <c r="T96" t="n">
-        <v>4.22</v>
-      </c>
       <c r="U96" t="inlineStr">
         <is>
           <t>02/10/2023 23:29</t>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
         </is>
       </c>
     </row>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -9321,22 +9321,22 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>2.25</v>
+        <v>2.3</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>2.49</v>
+        <v>2.14</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
@@ -9344,15 +9344,15 @@
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.04</v>
+        <v>3.05</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>2.86</v>
+        <v>3.03</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
@@ -9360,15 +9360,15 @@
         </is>
       </c>
       <c r="R97" t="n">
-        <v>3.7</v>
+        <v>3.54</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
-          <t>25/09/2023 22:42</t>
+          <t>26/09/2023 01:12</t>
         </is>
       </c>
       <c r="T97" t="n">
-        <v>3.54</v>
+        <v>4.22</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-instituto/t4LKO1te/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-sarmiento-junin/WA73IQJL/</t>
         </is>
       </c>
     </row>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -9413,14 +9413,14 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Central Cordoba</t>
         </is>
       </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>3.31</v>
+        <v>1.93</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
         </is>
       </c>
       <c r="L98" t="n">
-        <v>3.28</v>
+        <v>1.91</v>
       </c>
       <c r="M98" t="inlineStr">
         <is>
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="N98" t="n">
-        <v>2.97</v>
+        <v>3.29</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -9444,7 +9444,7 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>2.93</v>
+        <v>3.2</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
@@ -9452,7 +9452,7 @@
         </is>
       </c>
       <c r="R98" t="n">
-        <v>2.47</v>
+        <v>4.52</v>
       </c>
       <c r="S98" t="inlineStr">
         <is>
@@ -9460,7 +9460,7 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>2.59</v>
+        <v>5.03</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
@@ -9469,7 +9469,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
         </is>
       </c>
     </row>
@@ -9497,7 +9497,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G99" t="n">
@@ -9505,14 +9505,14 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Central Cordoba</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="I99" t="n">
         <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>1.93</v>
+        <v>3.31</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -9520,7 +9520,7 @@
         </is>
       </c>
       <c r="L99" t="n">
-        <v>1.91</v>
+        <v>3.28</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
@@ -9528,7 +9528,7 @@
         </is>
       </c>
       <c r="N99" t="n">
-        <v>3.29</v>
+        <v>2.97</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -9536,7 +9536,7 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>3.2</v>
+        <v>2.93</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
@@ -9544,7 +9544,7 @@
         </is>
       </c>
       <c r="R99" t="n">
-        <v>4.52</v>
+        <v>2.47</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
@@ -9552,7 +9552,7 @@
         </is>
       </c>
       <c r="T99" t="n">
-        <v>5.03</v>
+        <v>2.59</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
@@ -9561,7 +9561,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-central-cordoba-santiago-del-estero/2DMGPsRl/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-argentinos-jrs/CrrxXPYE/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Estudiantes L.P.</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,63 +9781,63 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J102" t="n">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>2.17</v>
+        <v>1.9</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.37</v>
+        <v>3.58</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.06</v>
+        <v>3.47</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>4.33</v>
+        <v>4.7</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>01/10/2023 02:42</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>4.04</v>
+        <v>4.55</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>07/10/2023 23:59</t>
+          <t>07/10/2023 23:58</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Estudiantes L.P.</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -9873,63 +9873,63 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Godoy Cruz</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J103" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>1.9</v>
+        <v>2.17</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>3.58</v>
+        <v>3.37</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>3.47</v>
+        <v>3.06</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>4.7</v>
+        <v>4.33</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>01/10/2023 02:42</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>4.55</v>
+        <v>4.04</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>07/10/2023 23:58</t>
+          <t>07/10/2023 23:59</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-defensa-y-justicia/EX7jxLAf/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/estudiantes-l-p-godoy-cruz/x6gob2XD/</t>
         </is>
       </c>
     </row>
@@ -10141,7 +10141,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G106" t="n">
@@ -10149,14 +10149,14 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Sarmiento Junin</t>
+          <t>Gimnasia L.P.</t>
         </is>
       </c>
       <c r="I106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J106" t="n">
-        <v>1.96</v>
+        <v>1.93</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
@@ -10164,15 +10164,15 @@
         </is>
       </c>
       <c r="L106" t="n">
-        <v>1.88</v>
+        <v>2.08</v>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:05</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="N106" t="n">
-        <v>3.24</v>
+        <v>3.23</v>
       </c>
       <c r="O106" t="inlineStr">
         <is>
@@ -10180,15 +10180,15 @@
         </is>
       </c>
       <c r="P106" t="n">
-        <v>3.14</v>
+        <v>2.95</v>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:05</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="R106" t="n">
-        <v>4.4</v>
+        <v>4.21</v>
       </c>
       <c r="S106" t="inlineStr">
         <is>
@@ -10196,16 +10196,16 @@
         </is>
       </c>
       <c r="T106" t="n">
-        <v>5.34</v>
+        <v>4.67</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>08/10/2023 19:06</t>
+          <t>08/10/2023 19:27</t>
         </is>
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-sarmiento-junin/Aa1azau7/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-gimnasia-l-p/xj5NrNXQ/</t>
         </is>
       </c>
     </row>
@@ -10233,7 +10233,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -10241,14 +10241,14 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Gimnasia L.P.</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J107" t="n">
-        <v>1.93</v>
+        <v>1.96</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -10256,15 +10256,15 @@
         </is>
       </c>
       <c r="L107" t="n">
-        <v>2.08</v>
+        <v>1.88</v>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:05</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>3.23</v>
+        <v>3.24</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -10272,15 +10272,15 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>2.95</v>
+        <v>3.14</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:05</t>
         </is>
       </c>
       <c r="R107" t="n">
-        <v>4.21</v>
+        <v>4.4</v>
       </c>
       <c r="S107" t="inlineStr">
         <is>
@@ -10288,16 +10288,16 @@
         </is>
       </c>
       <c r="T107" t="n">
-        <v>4.67</v>
+        <v>5.34</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>08/10/2023 19:27</t>
+          <t>08/10/2023 19:06</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-gimnasia-l-p/xj5NrNXQ/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-sarmiento-junin/Aa1azau7/</t>
         </is>
       </c>
     </row>
@@ -10509,71 +10509,71 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Barracas Central</t>
+          <t>Arsenal Sarandi</t>
         </is>
       </c>
       <c r="G110" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="I110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J110" t="n">
-        <v>2.5</v>
+        <v>3.26</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="L110" t="n">
-        <v>2.6</v>
+        <v>3.55</v>
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:59</t>
         </is>
       </c>
       <c r="N110" t="n">
-        <v>3.13</v>
+        <v>2.96</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="P110" t="n">
-        <v>2.84</v>
+        <v>2.9</v>
       </c>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:58</t>
         </is>
       </c>
       <c r="R110" t="n">
-        <v>2.93</v>
+        <v>2.51</v>
       </c>
       <c r="S110" t="inlineStr">
         <is>
-          <t>02/10/2023 22:42</t>
+          <t>02/10/2023 22:12</t>
         </is>
       </c>
       <c r="T110" t="n">
-        <v>2.91</v>
+        <v>2.46</v>
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>09/10/2023 22:36</t>
+          <t>09/10/2023 22:53</t>
         </is>
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
         </is>
       </c>
     </row>
@@ -10601,71 +10601,71 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Arsenal Sarandi</t>
+          <t>Barracas Central</t>
         </is>
       </c>
       <c r="G111" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J111" t="n">
-        <v>3.26</v>
+        <v>2.5</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="L111" t="n">
-        <v>3.55</v>
+        <v>2.6</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:59</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>2.96</v>
+        <v>3.13</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="P111" t="n">
-        <v>2.9</v>
+        <v>2.84</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:58</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>2.51</v>
+        <v>2.93</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>02/10/2023 22:12</t>
+          <t>02/10/2023 22:42</t>
         </is>
       </c>
       <c r="T111" t="n">
-        <v>2.46</v>
+        <v>2.91</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>09/10/2023 22:53</t>
+          <t>09/10/2023 22:36</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/arsenal-sarandi-banfield/lUOSMuB7/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/barracas-central-colon-santa-fe/4x7Fpq3E/</t>
         </is>
       </c>
     </row>
@@ -12625,22 +12625,22 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Instituto</t>
+          <t>Argentinos Jrs</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Rosario Central</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="I133" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J133" t="n">
-        <v>2.08</v>
+        <v>1.88</v>
       </c>
       <c r="K133" t="inlineStr">
         <is>
@@ -12648,15 +12648,15 @@
         </is>
       </c>
       <c r="L133" t="n">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="N133" t="n">
-        <v>3.15</v>
+        <v>3.23</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -12664,15 +12664,15 @@
         </is>
       </c>
       <c r="P133" t="n">
-        <v>3.15</v>
+        <v>3.11</v>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:26</t>
+          <t>25/10/2023 02:23</t>
         </is>
       </c>
       <c r="R133" t="n">
-        <v>4.07</v>
+        <v>4.51</v>
       </c>
       <c r="S133" t="inlineStr">
         <is>
@@ -12680,16 +12680,16 @@
         </is>
       </c>
       <c r="T133" t="n">
-        <v>4.84</v>
+        <v>5.33</v>
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>25/10/2023 02:29</t>
+          <t>25/10/2023 02:27</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
         </is>
       </c>
     </row>
@@ -12717,22 +12717,22 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Argentinos Jrs</t>
+          <t>Instituto</t>
         </is>
       </c>
       <c r="G134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Rosario Central</t>
         </is>
       </c>
       <c r="I134" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J134" t="n">
-        <v>1.88</v>
+        <v>2.08</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>3.23</v>
+        <v>3.15</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>3.11</v>
+        <v>3.15</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:23</t>
+          <t>25/10/2023 02:26</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>4.51</v>
+        <v>4.07</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>5.33</v>
+        <v>4.84</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>25/10/2023 02:27</t>
+          <t>25/10/2023 02:29</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/argentinos-jrs-huracan/zJ8w6jVi/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/instituto-rosario-central/Isbr5Apb/</t>
         </is>
       </c>
     </row>
@@ -13269,22 +13269,22 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Lanus</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="G140" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="I140" t="n">
         <v>2</v>
       </c>
-      <c r="H140" t="inlineStr">
-        <is>
-          <t>Tigre</t>
-        </is>
-      </c>
-      <c r="I140" t="n">
-        <v>1</v>
-      </c>
       <c r="J140" t="n">
-        <v>2.24</v>
+        <v>2</v>
       </c>
       <c r="K140" t="inlineStr">
         <is>
@@ -13292,15 +13292,15 @@
         </is>
       </c>
       <c r="L140" t="n">
-        <v>2.6</v>
+        <v>2.15</v>
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:59</t>
+          <t>27/10/2023 01:34</t>
         </is>
       </c>
       <c r="N140" t="n">
-        <v>3.08</v>
+        <v>3.16</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -13308,15 +13308,15 @@
         </is>
       </c>
       <c r="P140" t="n">
-        <v>2.96</v>
+        <v>3.04</v>
       </c>
       <c r="Q140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:28</t>
+          <t>27/10/2023 01:34</t>
         </is>
       </c>
       <c r="R140" t="n">
-        <v>3.65</v>
+        <v>4.07</v>
       </c>
       <c r="S140" t="inlineStr">
         <is>
@@ -13324,16 +13324,16 @@
         </is>
       </c>
       <c r="T140" t="n">
-        <v>3.19</v>
+        <v>4.18</v>
       </c>
       <c r="U140" t="inlineStr">
         <is>
-          <t>27/10/2023 01:56</t>
+          <t>27/10/2023 01:34</t>
         </is>
       </c>
       <c r="V140" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-tigre/dYdn4Ua4/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-godoy-cruz/dduZfQMj/</t>
         </is>
       </c>
     </row>
@@ -13361,22 +13361,22 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Lanus</t>
         </is>
       </c>
       <c r="G141" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>Godoy Cruz</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I141" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J141" t="n">
-        <v>2</v>
+        <v>2.24</v>
       </c>
       <c r="K141" t="inlineStr">
         <is>
@@ -13384,15 +13384,15 @@
         </is>
       </c>
       <c r="L141" t="n">
-        <v>2.15</v>
+        <v>2.6</v>
       </c>
       <c r="M141" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:59</t>
         </is>
       </c>
       <c r="N141" t="n">
-        <v>3.16</v>
+        <v>3.08</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -13400,15 +13400,15 @@
         </is>
       </c>
       <c r="P141" t="n">
-        <v>3.04</v>
+        <v>2.96</v>
       </c>
       <c r="Q141" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:28</t>
         </is>
       </c>
       <c r="R141" t="n">
-        <v>4.07</v>
+        <v>3.65</v>
       </c>
       <c r="S141" t="inlineStr">
         <is>
@@ -13416,16 +13416,16 @@
         </is>
       </c>
       <c r="T141" t="n">
-        <v>4.18</v>
+        <v>3.19</v>
       </c>
       <c r="U141" t="inlineStr">
         <is>
-          <t>27/10/2023 01:34</t>
+          <t>27/10/2023 01:56</t>
         </is>
       </c>
       <c r="V141" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-godoy-cruz/dduZfQMj/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/lanus-tigre/dYdn4Ua4/</t>
         </is>
       </c>
     </row>
@@ -15753,71 +15753,71 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="G167" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I167" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J167" t="n">
-        <v>2.01</v>
+        <v>2.22</v>
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t>30/10/2023 20:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="L167" t="n">
-        <v>2.23</v>
+        <v>2.57</v>
       </c>
       <c r="M167" t="inlineStr">
         <is>
-          <t>07/11/2023 00:57</t>
+          <t>07/11/2023 00:59</t>
         </is>
       </c>
       <c r="N167" t="n">
-        <v>3.25</v>
+        <v>3.05</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
-          <t>30/10/2023 20:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="P167" t="n">
-        <v>3</v>
+        <v>2.79</v>
       </c>
       <c r="Q167" t="inlineStr">
         <is>
-          <t>07/11/2023 00:57</t>
+          <t>07/11/2023 00:59</t>
         </is>
       </c>
       <c r="R167" t="n">
-        <v>4.19</v>
+        <v>3.53</v>
       </c>
       <c r="S167" t="inlineStr">
         <is>
-          <t>30/10/2023 20:12</t>
+          <t>31/10/2023 23:12</t>
         </is>
       </c>
       <c r="T167" t="n">
-        <v>3.98</v>
+        <v>3.5</v>
       </c>
       <c r="U167" t="inlineStr">
         <is>
-          <t>07/11/2023 00:46</t>
+          <t>07/11/2023 00:59</t>
         </is>
       </c>
       <c r="V167" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-colon-santa-fe/CbKBROcS/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-tigre/bexwrpr9/</t>
         </is>
       </c>
     </row>
@@ -15845,71 +15845,71 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="G168" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Colon Santa Fe</t>
         </is>
       </c>
       <c r="I168" t="n">
+        <v>1</v>
+      </c>
+      <c r="J168" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="L168" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>07/11/2023 00:57</t>
+        </is>
+      </c>
+      <c r="N168" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="O168" t="inlineStr">
+        <is>
+          <t>30/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="P168" t="n">
         <v>3</v>
       </c>
-      <c r="J168" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="K168" t="inlineStr">
-        <is>
-          <t>31/10/2023 23:12</t>
-        </is>
-      </c>
-      <c r="L168" t="n">
-        <v>2.57</v>
-      </c>
-      <c r="M168" t="inlineStr">
-        <is>
-          <t>07/11/2023 00:59</t>
-        </is>
-      </c>
-      <c r="N168" t="n">
-        <v>3.05</v>
-      </c>
-      <c r="O168" t="inlineStr">
-        <is>
-          <t>31/10/2023 23:12</t>
-        </is>
-      </c>
-      <c r="P168" t="n">
-        <v>2.79</v>
-      </c>
       <c r="Q168" t="inlineStr">
         <is>
-          <t>07/11/2023 00:59</t>
+          <t>07/11/2023 00:57</t>
         </is>
       </c>
       <c r="R168" t="n">
-        <v>3.53</v>
+        <v>4.19</v>
       </c>
       <c r="S168" t="inlineStr">
         <is>
-          <t>31/10/2023 23:12</t>
+          <t>30/10/2023 20:12</t>
         </is>
       </c>
       <c r="T168" t="n">
-        <v>3.5</v>
+        <v>3.98</v>
       </c>
       <c r="U168" t="inlineStr">
         <is>
-          <t>07/11/2023 00:59</t>
+          <t>07/11/2023 00:46</t>
         </is>
       </c>
       <c r="V168" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/ca-belgrano-de-cordoba-tigre/bexwrpr9/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-colon-santa-fe/CbKBROcS/</t>
         </is>
       </c>
     </row>
@@ -17317,22 +17317,22 @@
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>Union de Santa Fe</t>
+          <t>Banfield</t>
         </is>
       </c>
       <c r="G184" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>Tigre</t>
+          <t>Gimnasia L.P.</t>
         </is>
       </c>
       <c r="I184" t="n">
         <v>0</v>
       </c>
       <c r="J184" t="n">
-        <v>2.47</v>
+        <v>1.98</v>
       </c>
       <c r="K184" t="inlineStr">
         <is>
@@ -17340,15 +17340,15 @@
         </is>
       </c>
       <c r="L184" t="n">
-        <v>2.11</v>
+        <v>2.27</v>
       </c>
       <c r="M184" t="inlineStr">
         <is>
-          <t>25/11/2023 21:55</t>
+          <t>25/11/2023 21:51</t>
         </is>
       </c>
       <c r="N184" t="n">
-        <v>3.01</v>
+        <v>3.2</v>
       </c>
       <c r="O184" t="inlineStr">
         <is>
@@ -17356,15 +17356,15 @@
         </is>
       </c>
       <c r="P184" t="n">
-        <v>3.06</v>
+        <v>3.1</v>
       </c>
       <c r="Q184" t="inlineStr">
         <is>
-          <t>25/11/2023 21:58</t>
+          <t>25/11/2023 21:51</t>
         </is>
       </c>
       <c r="R184" t="n">
-        <v>3.28</v>
+        <v>4.4</v>
       </c>
       <c r="S184" t="inlineStr">
         <is>
@@ -17372,16 +17372,16 @@
         </is>
       </c>
       <c r="T184" t="n">
-        <v>4.28</v>
+        <v>3.71</v>
       </c>
       <c r="U184" t="inlineStr">
         <is>
-          <t>25/11/2023 21:55</t>
+          <t>25/11/2023 21:51</t>
         </is>
       </c>
       <c r="V184" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-tigre/2kjkTdjU/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-gimnasia-l-p/MZfUXKya/</t>
         </is>
       </c>
     </row>
@@ -17409,42 +17409,42 @@
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>Velez Sarsfield</t>
+          <t>Platense</t>
         </is>
       </c>
       <c r="G185" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>Colon Santa Fe</t>
+          <t>Sarmiento Junin</t>
         </is>
       </c>
       <c r="I185" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J185" t="n">
-        <v>1.87</v>
+        <v>1.97</v>
       </c>
       <c r="K185" t="inlineStr">
         <is>
-          <t>12/11/2023 21:12</t>
+          <t>18/11/2023 22:12</t>
         </is>
       </c>
       <c r="L185" t="n">
-        <v>2.2</v>
+        <v>2.28</v>
       </c>
       <c r="M185" t="inlineStr">
         <is>
-          <t>25/11/2023 21:51</t>
+          <t>25/11/2023 21:58</t>
         </is>
       </c>
       <c r="N185" t="n">
-        <v>3.32</v>
+        <v>3.16</v>
       </c>
       <c r="O185" t="inlineStr">
         <is>
-          <t>12/11/2023 21:12</t>
+          <t>18/11/2023 22:12</t>
         </is>
       </c>
       <c r="P185" t="n">
@@ -17452,19 +17452,19 @@
       </c>
       <c r="Q185" t="inlineStr">
         <is>
-          <t>25/11/2023 21:51</t>
+          <t>25/11/2023 21:58</t>
         </is>
       </c>
       <c r="R185" t="n">
-        <v>4.81</v>
+        <v>4.56</v>
       </c>
       <c r="S185" t="inlineStr">
         <is>
-          <t>12/11/2023 21:12</t>
+          <t>18/11/2023 22:12</t>
         </is>
       </c>
       <c r="T185" t="n">
-        <v>4.28</v>
+        <v>4</v>
       </c>
       <c r="U185" t="inlineStr">
         <is>
@@ -17473,7 +17473,7 @@
       </c>
       <c r="V185" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-colon-santa-fe/0K6LZt7n/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-sarmiento-junin/neXEqIzB/</t>
         </is>
       </c>
     </row>
@@ -17501,22 +17501,22 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>Banfield</t>
+          <t>Union de Santa Fe</t>
         </is>
       </c>
       <c r="G186" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>Gimnasia L.P.</t>
+          <t>Tigre</t>
         </is>
       </c>
       <c r="I186" t="n">
         <v>0</v>
       </c>
       <c r="J186" t="n">
-        <v>1.98</v>
+        <v>2.47</v>
       </c>
       <c r="K186" t="inlineStr">
         <is>
@@ -17524,15 +17524,15 @@
         </is>
       </c>
       <c r="L186" t="n">
-        <v>2.27</v>
+        <v>2.11</v>
       </c>
       <c r="M186" t="inlineStr">
         <is>
-          <t>25/11/2023 21:51</t>
+          <t>25/11/2023 21:55</t>
         </is>
       </c>
       <c r="N186" t="n">
-        <v>3.2</v>
+        <v>3.01</v>
       </c>
       <c r="O186" t="inlineStr">
         <is>
@@ -17540,15 +17540,15 @@
         </is>
       </c>
       <c r="P186" t="n">
-        <v>3.1</v>
+        <v>3.06</v>
       </c>
       <c r="Q186" t="inlineStr">
         <is>
-          <t>25/11/2023 21:51</t>
+          <t>25/11/2023 21:58</t>
         </is>
       </c>
       <c r="R186" t="n">
-        <v>4.4</v>
+        <v>3.28</v>
       </c>
       <c r="S186" t="inlineStr">
         <is>
@@ -17556,16 +17556,16 @@
         </is>
       </c>
       <c r="T186" t="n">
-        <v>3.71</v>
+        <v>4.28</v>
       </c>
       <c r="U186" t="inlineStr">
         <is>
-          <t>25/11/2023 21:51</t>
+          <t>25/11/2023 21:55</t>
         </is>
       </c>
       <c r="V186" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/banfield-gimnasia-l-p/MZfUXKya/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/union-de-santa-fe-tigre/2kjkTdjU/</t>
         </is>
       </c>
     </row>
@@ -17593,42 +17593,42 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>Platense</t>
+          <t>Velez Sarsfield</t>
         </is>
       </c>
       <c r="G187" t="n">
+        <v>3</v>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>Colon Santa Fe</t>
+        </is>
+      </c>
+      <c r="I187" t="n">
         <v>1</v>
       </c>
-      <c r="H187" t="inlineStr">
-        <is>
-          <t>Sarmiento Junin</t>
-        </is>
-      </c>
-      <c r="I187" t="n">
-        <v>0</v>
-      </c>
       <c r="J187" t="n">
-        <v>1.97</v>
+        <v>1.87</v>
       </c>
       <c r="K187" t="inlineStr">
         <is>
-          <t>18/11/2023 22:12</t>
+          <t>12/11/2023 21:12</t>
         </is>
       </c>
       <c r="L187" t="n">
-        <v>2.28</v>
+        <v>2.2</v>
       </c>
       <c r="M187" t="inlineStr">
         <is>
-          <t>25/11/2023 21:58</t>
+          <t>25/11/2023 21:51</t>
         </is>
       </c>
       <c r="N187" t="n">
-        <v>3.16</v>
+        <v>3.32</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
-          <t>18/11/2023 22:12</t>
+          <t>12/11/2023 21:12</t>
         </is>
       </c>
       <c r="P187" t="n">
@@ -17636,28 +17636,28 @@
       </c>
       <c r="Q187" t="inlineStr">
         <is>
+          <t>25/11/2023 21:51</t>
+        </is>
+      </c>
+      <c r="R187" t="n">
+        <v>4.81</v>
+      </c>
+      <c r="S187" t="inlineStr">
+        <is>
+          <t>12/11/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T187" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="U187" t="inlineStr">
+        <is>
           <t>25/11/2023 21:58</t>
         </is>
       </c>
-      <c r="R187" t="n">
-        <v>4.56</v>
-      </c>
-      <c r="S187" t="inlineStr">
-        <is>
-          <t>18/11/2023 22:12</t>
-        </is>
-      </c>
-      <c r="T187" t="n">
-        <v>4</v>
-      </c>
-      <c r="U187" t="inlineStr">
-        <is>
-          <t>25/11/2023 21:58</t>
-        </is>
-      </c>
       <c r="V187" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/platense-sarmiento-junin/neXEqIzB/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/velez-sarsfield-colon-santa-fe/0K6LZt7n/</t>
         </is>
       </c>
     </row>
@@ -17685,30 +17685,30 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>Atl. Tucuman</t>
+          <t>Talleres Cordoba</t>
         </is>
       </c>
       <c r="G188" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>Huracan</t>
+          <t>Independiente</t>
         </is>
       </c>
       <c r="I188" t="n">
         <v>2</v>
       </c>
       <c r="J188" t="n">
-        <v>2.46</v>
+        <v>2.13</v>
       </c>
       <c r="K188" t="inlineStr">
         <is>
-          <t>12/11/2023 21:12</t>
+          <t>19/11/2023 22:12</t>
         </is>
       </c>
       <c r="L188" t="n">
-        <v>2.57</v>
+        <v>2.68</v>
       </c>
       <c r="M188" t="inlineStr">
         <is>
@@ -17716,15 +17716,15 @@
         </is>
       </c>
       <c r="N188" t="n">
-        <v>2.95</v>
+        <v>3.12</v>
       </c>
       <c r="O188" t="inlineStr">
         <is>
-          <t>12/11/2023 21:12</t>
+          <t>19/11/2023 22:12</t>
         </is>
       </c>
       <c r="P188" t="n">
-        <v>2.76</v>
+        <v>2.44</v>
       </c>
       <c r="Q188" t="inlineStr">
         <is>
@@ -17732,15 +17732,15 @@
         </is>
       </c>
       <c r="R188" t="n">
-        <v>3.35</v>
+        <v>3.67</v>
       </c>
       <c r="S188" t="inlineStr">
         <is>
-          <t>12/11/2023 21:12</t>
+          <t>19/11/2023 22:12</t>
         </is>
       </c>
       <c r="T188" t="n">
-        <v>3.56</v>
+        <v>3.98</v>
       </c>
       <c r="U188" t="inlineStr">
         <is>
@@ -17749,7 +17749,7 @@
       </c>
       <c r="V188" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-huracan/Y9bYWvi5/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-independiente/vB5PY0Mh/</t>
         </is>
       </c>
     </row>
@@ -17961,30 +17961,30 @@
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>Talleres Cordoba</t>
+          <t>Atl. Tucuman</t>
         </is>
       </c>
       <c r="G191" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>Independiente</t>
+          <t>Huracan</t>
         </is>
       </c>
       <c r="I191" t="n">
         <v>2</v>
       </c>
       <c r="J191" t="n">
-        <v>2.13</v>
+        <v>2.46</v>
       </c>
       <c r="K191" t="inlineStr">
         <is>
-          <t>19/11/2023 22:12</t>
+          <t>12/11/2023 21:12</t>
         </is>
       </c>
       <c r="L191" t="n">
-        <v>2.68</v>
+        <v>2.57</v>
       </c>
       <c r="M191" t="inlineStr">
         <is>
@@ -17992,15 +17992,15 @@
         </is>
       </c>
       <c r="N191" t="n">
-        <v>3.12</v>
+        <v>2.95</v>
       </c>
       <c r="O191" t="inlineStr">
         <is>
-          <t>19/11/2023 22:12</t>
+          <t>12/11/2023 21:12</t>
         </is>
       </c>
       <c r="P191" t="n">
-        <v>2.44</v>
+        <v>2.76</v>
       </c>
       <c r="Q191" t="inlineStr">
         <is>
@@ -18008,15 +18008,15 @@
         </is>
       </c>
       <c r="R191" t="n">
-        <v>3.67</v>
+        <v>3.35</v>
       </c>
       <c r="S191" t="inlineStr">
         <is>
-          <t>19/11/2023 22:12</t>
+          <t>12/11/2023 21:12</t>
         </is>
       </c>
       <c r="T191" t="n">
-        <v>3.98</v>
+        <v>3.56</v>
       </c>
       <c r="U191" t="inlineStr">
         <is>
@@ -18025,7 +18025,7 @@
       </c>
       <c r="V191" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/talleres-cordoba-independiente/vB5PY0Mh/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/atl-tucuman-huracan/Y9bYWvi5/</t>
         </is>
       </c>
     </row>
@@ -18329,71 +18329,71 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>Racing Club</t>
+          <t>Newells Old Boys</t>
         </is>
       </c>
       <c r="G195" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Defensa y Justicia</t>
         </is>
       </c>
       <c r="I195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J195" t="n">
-        <v>1.92</v>
+        <v>1.78</v>
       </c>
       <c r="K195" t="inlineStr">
         <is>
-          <t>21/11/2023 01:42</t>
+          <t>12/11/2023 21:12</t>
         </is>
       </c>
       <c r="L195" t="n">
-        <v>2.06</v>
+        <v>1.69</v>
       </c>
       <c r="M195" t="inlineStr">
         <is>
-          <t>28/11/2023 01:22</t>
+          <t>28/11/2023 01:28</t>
         </is>
       </c>
       <c r="N195" t="n">
-        <v>3.34</v>
+        <v>3.5</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
-          <t>21/11/2023 01:42</t>
+          <t>12/11/2023 21:12</t>
         </is>
       </c>
       <c r="P195" t="n">
-        <v>3.21</v>
+        <v>3.64</v>
       </c>
       <c r="Q195" t="inlineStr">
         <is>
-          <t>28/11/2023 01:21</t>
+          <t>28/11/2023 01:28</t>
         </is>
       </c>
       <c r="R195" t="n">
-        <v>4.13</v>
+        <v>5</v>
       </c>
       <c r="S195" t="inlineStr">
         <is>
-          <t>21/11/2023 01:42</t>
+          <t>12/11/2023 21:12</t>
         </is>
       </c>
       <c r="T195" t="n">
-        <v>4.14</v>
+        <v>5.85</v>
       </c>
       <c r="U195" t="inlineStr">
         <is>
-          <t>28/11/2023 00:58</t>
+          <t>28/11/2023 01:28</t>
         </is>
       </c>
       <c r="V195" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-ca-belgrano-de-cordoba/vBRfltMu/</t>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-defensa-y-justicia/ETJ7ov6b/</t>
         </is>
       </c>
     </row>
@@ -18421,71 +18421,715 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>Newells Old Boys</t>
+          <t>Racing Club</t>
         </is>
       </c>
       <c r="G196" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>Defensa y Justicia</t>
+          <t>Belgrano</t>
         </is>
       </c>
       <c r="I196" t="n">
+        <v>1</v>
+      </c>
+      <c r="J196" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>21/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="L196" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="M196" t="inlineStr">
+        <is>
+          <t>28/11/2023 01:22</t>
+        </is>
+      </c>
+      <c r="N196" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="O196" t="inlineStr">
+        <is>
+          <t>21/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="P196" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="Q196" t="inlineStr">
+        <is>
+          <t>28/11/2023 01:21</t>
+        </is>
+      </c>
+      <c r="R196" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="S196" t="inlineStr">
+        <is>
+          <t>21/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="T196" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="U196" t="inlineStr">
+        <is>
+          <t>28/11/2023 00:58</t>
+        </is>
+      </c>
+      <c r="V196" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-ca-belgrano-de-cordoba/vBRfltMu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E197" s="2" t="n">
+        <v>45262.9375</v>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Huracan</t>
+        </is>
+      </c>
+      <c r="G197" t="n">
+        <v>1</v>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>Platense</t>
+        </is>
+      </c>
+      <c r="I197" t="n">
+        <v>1</v>
+      </c>
+      <c r="J197" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="L197" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="M197" t="inlineStr">
+        <is>
+          <t>02/12/2023 22:29</t>
+        </is>
+      </c>
+      <c r="N197" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="O197" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="P197" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="Q197" t="inlineStr">
+        <is>
+          <t>02/12/2023 22:29</t>
+        </is>
+      </c>
+      <c r="R197" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="S197" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="T197" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="U197" t="inlineStr">
+        <is>
+          <t>02/12/2023 22:29</t>
+        </is>
+      </c>
+      <c r="V197" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/huracan-platense/SzIUwiaU/</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E198" s="2" t="n">
+        <v>45263.0625</v>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="G198" t="n">
         <v>0</v>
       </c>
-      <c r="J196" t="n">
-        <v>1.78</v>
-      </c>
-      <c r="K196" t="inlineStr">
-        <is>
-          <t>12/11/2023 21:12</t>
-        </is>
-      </c>
-      <c r="L196" t="n">
-        <v>1.69</v>
-      </c>
-      <c r="M196" t="inlineStr">
-        <is>
-          <t>28/11/2023 01:28</t>
-        </is>
-      </c>
-      <c r="N196" t="n">
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>Banfield</t>
+        </is>
+      </c>
+      <c r="I198" t="n">
+        <v>0</v>
+      </c>
+      <c r="J198" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="L198" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="M198" t="inlineStr">
+        <is>
+          <t>03/12/2023 01:29</t>
+        </is>
+      </c>
+      <c r="N198" t="n">
+        <v>2.94</v>
+      </c>
+      <c r="O198" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="P198" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="Q198" t="inlineStr">
+        <is>
+          <t>03/12/2023 01:29</t>
+        </is>
+      </c>
+      <c r="R198" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="S198" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="T198" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="U198" t="inlineStr">
+        <is>
+          <t>03/12/2023 01:27</t>
+        </is>
+      </c>
+      <c r="V198" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-banfield/lpJQvXqO/</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E199" s="2" t="n">
+        <v>45263.9375</v>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>River Plate</t>
+        </is>
+      </c>
+      <c r="G199" t="n">
+        <v>2</v>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>Belgrano</t>
+        </is>
+      </c>
+      <c r="I199" t="n">
+        <v>1</v>
+      </c>
+      <c r="J199" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="L199" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="M199" t="inlineStr">
+        <is>
+          <t>03/12/2023 22:12</t>
+        </is>
+      </c>
+      <c r="N199" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="O199" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="P199" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="Q199" t="inlineStr">
+        <is>
+          <t>03/12/2023 22:29</t>
+        </is>
+      </c>
+      <c r="R199" t="n">
+        <v>6.07</v>
+      </c>
+      <c r="S199" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="T199" t="n">
+        <v>6.73</v>
+      </c>
+      <c r="U199" t="inlineStr">
+        <is>
+          <t>03/12/2023 22:29</t>
+        </is>
+      </c>
+      <c r="V199" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/river-plate-ca-belgrano-de-cordoba/fNJMuDUH/</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E200" s="2" t="n">
+        <v>45264.0625</v>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>Racing Club</t>
+        </is>
+      </c>
+      <c r="G200" t="n">
+        <v>2</v>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>Rosario Central</t>
+        </is>
+      </c>
+      <c r="I200" t="n">
+        <v>2</v>
+      </c>
+      <c r="J200" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="L200" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="M200" t="inlineStr">
+        <is>
+          <t>04/12/2023 01:29</t>
+        </is>
+      </c>
+      <c r="N200" t="n">
         <v>3.5</v>
       </c>
-      <c r="O196" t="inlineStr">
-        <is>
-          <t>12/11/2023 21:12</t>
-        </is>
-      </c>
-      <c r="P196" t="n">
-        <v>3.64</v>
-      </c>
-      <c r="Q196" t="inlineStr">
-        <is>
-          <t>28/11/2023 01:28</t>
-        </is>
-      </c>
-      <c r="R196" t="n">
-        <v>5</v>
-      </c>
-      <c r="S196" t="inlineStr">
-        <is>
-          <t>12/11/2023 21:12</t>
-        </is>
-      </c>
-      <c r="T196" t="n">
-        <v>5.85</v>
-      </c>
-      <c r="U196" t="inlineStr">
-        <is>
-          <t>28/11/2023 01:28</t>
-        </is>
-      </c>
-      <c r="V196" t="inlineStr">
-        <is>
-          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/newells-old-boys-defensa-y-justicia/ETJ7ov6b/</t>
+      <c r="O200" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="P200" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="Q200" t="inlineStr">
+        <is>
+          <t>04/12/2023 01:29</t>
+        </is>
+      </c>
+      <c r="R200" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="S200" t="inlineStr">
+        <is>
+          <t>29/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="T200" t="n">
+        <v>4.62</v>
+      </c>
+      <c r="U200" t="inlineStr">
+        <is>
+          <t>04/12/2023 01:29</t>
+        </is>
+      </c>
+      <c r="V200" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/racing-club-rosario-central/tKFItgFB/</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E201" s="2" t="n">
+        <v>45269.91666666666</v>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>Godoy Cruz</t>
+        </is>
+      </c>
+      <c r="G201" t="n">
+        <v>1</v>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>Platense</t>
+        </is>
+      </c>
+      <c r="I201" t="n">
+        <v>1</v>
+      </c>
+      <c r="J201" t="n">
+        <v>2.47</v>
+      </c>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>06/12/2023 13:11</t>
+        </is>
+      </c>
+      <c r="L201" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="M201" t="inlineStr">
+        <is>
+          <t>09/12/2023 21:27</t>
+        </is>
+      </c>
+      <c r="N201" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="O201" t="inlineStr">
+        <is>
+          <t>06/12/2023 13:11</t>
+        </is>
+      </c>
+      <c r="P201" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="Q201" t="inlineStr">
+        <is>
+          <t>09/12/2023 21:17</t>
+        </is>
+      </c>
+      <c r="R201" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="S201" t="inlineStr">
+        <is>
+          <t>06/12/2023 13:11</t>
+        </is>
+      </c>
+      <c r="T201" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="U201" t="inlineStr">
+        <is>
+          <t>09/12/2023 21:27</t>
+        </is>
+      </c>
+      <c r="V201" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/godoy-cruz-platense/jcFQNmw2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E202" s="2" t="n">
+        <v>45270.08333333334</v>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>River Plate</t>
+        </is>
+      </c>
+      <c r="G202" t="n">
+        <v>0</v>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>Rosario Central</t>
+        </is>
+      </c>
+      <c r="I202" t="n">
+        <v>0</v>
+      </c>
+      <c r="J202" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>06/12/2023 13:12</t>
+        </is>
+      </c>
+      <c r="L202" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="M202" t="inlineStr">
+        <is>
+          <t>10/12/2023 01:59</t>
+        </is>
+      </c>
+      <c r="N202" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="O202" t="inlineStr">
+        <is>
+          <t>06/12/2023 13:12</t>
+        </is>
+      </c>
+      <c r="P202" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="Q202" t="inlineStr">
+        <is>
+          <t>10/12/2023 01:59</t>
+        </is>
+      </c>
+      <c r="R202" t="n">
+        <v>5.81</v>
+      </c>
+      <c r="S202" t="inlineStr">
+        <is>
+          <t>06/12/2023 13:12</t>
+        </is>
+      </c>
+      <c r="T202" t="n">
+        <v>5.59</v>
+      </c>
+      <c r="U202" t="inlineStr">
+        <is>
+          <t>10/12/2023 01:56</t>
+        </is>
+      </c>
+      <c r="V202" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/river-plate-rosario-central/x0z1nXF2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>copa-de-la-liga-profesional</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E203" s="2" t="n">
+        <v>45277.04166666666</v>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>Rosario Central</t>
+        </is>
+      </c>
+      <c r="G203" t="n">
+        <v>1</v>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>Platense</t>
+        </is>
+      </c>
+      <c r="I203" t="n">
+        <v>0</v>
+      </c>
+      <c r="J203" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>11/12/2023 19:11</t>
+        </is>
+      </c>
+      <c r="L203" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="M203" t="inlineStr">
+        <is>
+          <t>17/12/2023 00:59</t>
+        </is>
+      </c>
+      <c r="N203" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="O203" t="inlineStr">
+        <is>
+          <t>11/12/2023 19:11</t>
+        </is>
+      </c>
+      <c r="P203" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="Q203" t="inlineStr">
+        <is>
+          <t>17/12/2023 00:48</t>
+        </is>
+      </c>
+      <c r="R203" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="S203" t="inlineStr">
+        <is>
+          <t>11/12/2023 19:11</t>
+        </is>
+      </c>
+      <c r="T203" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="U203" t="inlineStr">
+        <is>
+          <t>17/12/2023 00:59</t>
+        </is>
+      </c>
+      <c r="V203" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/argentina/copa-de-la-liga-profesional/rosario-central-platense/65Pyeyh3/</t>
         </is>
       </c>
     </row>

</xml_diff>